<commit_message>
WIP: - all counties need to be passed a *DojHistory - need to implement p64 check
[#164636782]
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/los_angeles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F877E9-5598-B242-867D-77774F1D3D3F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68BE6A9-1BB6-8B4D-BE63-0CDA8E0F591F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25620" yWindow="2600" windowWidth="25600" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="480" windowWidth="25600" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -676,9 +676,6 @@
     <t>05/12/2014</t>
   </si>
   <si>
-    <t>Misdemeanor or Infraction</t>
-  </si>
-  <si>
     <t>VONWINKLE,ERNIE</t>
   </si>
   <si>
@@ -725,6 +722,9 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>Two priors</t>
   </si>
 </sst>
 </file>
@@ -2271,8 +2271,8 @@
   </sheetPr>
   <dimension ref="A1:IW34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CV1" workbookViewId="0">
+      <selection activeCell="CZ51" sqref="CZ51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2391,16 +2391,16 @@
       <c r="K1" s="46"/>
       <c r="L1" s="46"/>
       <c r="M1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q1" s="46"/>
       <c r="R1" s="46"/>
@@ -2410,7 +2410,7 @@
       <c r="V1" s="46"/>
       <c r="W1" s="46"/>
       <c r="X1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Y1" s="46"/>
       <c r="Z1" s="46"/>
@@ -2427,12 +2427,12 @@
       <c r="AK1" s="46"/>
       <c r="AL1" s="46"/>
       <c r="AM1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AN1" s="46"/>
       <c r="AO1" s="46"/>
       <c r="AP1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AQ1" s="46"/>
       <c r="AR1" s="46"/>
@@ -2440,23 +2440,23 @@
       <c r="AT1" s="46"/>
       <c r="AU1" s="46"/>
       <c r="AV1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AW1" s="46"/>
       <c r="AX1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AY1" s="46"/>
       <c r="AZ1" s="46"/>
       <c r="BA1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BB1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BC1" s="46"/>
       <c r="BD1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BE1" s="46"/>
       <c r="BF1" s="46"/>
@@ -2484,76 +2484,76 @@
       <c r="CB1" s="46"/>
       <c r="CC1" s="46"/>
       <c r="CD1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CE1" s="46"/>
       <c r="CF1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CG1" s="46"/>
       <c r="CH1" s="46"/>
       <c r="CI1" s="46"/>
       <c r="CJ1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CK1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CL1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CM1" s="46"/>
       <c r="CN1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CO1" s="46"/>
       <c r="CP1" s="46"/>
       <c r="CQ1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CR1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CS1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CT1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CU1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CV1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CW1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CX1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CY1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="CZ1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="DA1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="DB1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="DC1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="DD1" s="46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:108" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -3689,7 +3689,7 @@
     </row>
     <row r="8" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -4045,7 +4045,7 @@
     </row>
     <row r="10" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="12" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
@@ -4757,7 +4757,7 @@
     </row>
     <row r="14" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -5295,7 +5295,7 @@
     </row>
     <row r="17" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -5829,7 +5829,7 @@
     </row>
     <row r="20" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
@@ -6189,7 +6189,7 @@
     </row>
     <row r="22" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
@@ -6385,7 +6385,7 @@
     </row>
     <row r="23" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -6903,7 +6903,7 @@
     </row>
     <row r="26" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
@@ -7091,7 +7091,7 @@
     </row>
     <row r="27" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
@@ -7279,7 +7279,7 @@
     </row>
     <row r="28" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
@@ -7645,7 +7645,7 @@
     </row>
     <row r="30" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="33"/>
@@ -7833,15 +7833,15 @@
         <v>143</v>
       </c>
       <c r="DC30" s="35" t="s">
-        <v>147</v>
+        <v>195</v>
       </c>
       <c r="DD30" s="35" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -7864,7 +7864,7 @@
         <v>183</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="9">
@@ -7999,13 +7999,13 @@
         <v>107</v>
       </c>
       <c r="CS31" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="CT31" s="10" t="s">
         <v>142</v>
       </c>
       <c r="CU31" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="CV31" s="10" t="s">
         <v>143</v>
@@ -8058,7 +8058,7 @@
         <v>183</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="9">
@@ -8124,13 +8124,13 @@
         <v>112</v>
       </c>
       <c r="BD32" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="BE32" s="10" t="s">
         <v>114</v>
       </c>
       <c r="BF32" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="BG32" s="11"/>
       <c r="BH32" s="11"/>
@@ -8207,7 +8207,7 @@
     </row>
     <row r="33" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
@@ -8227,10 +8227,10 @@
       <c r="K33" s="16"/>
       <c r="L33" s="16"/>
       <c r="M33" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="N33" s="15" t="s">
         <v>224</v>
-      </c>
-      <c r="N33" s="15" t="s">
-        <v>225</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="14">
@@ -8370,13 +8370,13 @@
         <v>143</v>
       </c>
       <c r="CX33" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="CY33" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="CY33" s="15" t="s">
-        <v>227</v>
-      </c>
       <c r="CZ33" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="DA33" s="15" t="s">
         <v>146</v>
@@ -8388,12 +8388,12 @@
         <v>147</v>
       </c>
       <c r="DD33" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
@@ -8413,10 +8413,10 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
       <c r="M34" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="N34" s="20" t="s">
         <v>229</v>
-      </c>
-      <c r="N34" s="20" t="s">
-        <v>230</v>
       </c>
       <c r="O34" s="21"/>
       <c r="P34" s="19">
@@ -8558,13 +8558,13 @@
         <v>143</v>
       </c>
       <c r="CX34" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="CY34" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="CY34" s="20" t="s">
-        <v>232</v>
-      </c>
       <c r="CZ34" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="DA34" s="20" t="s">
         <v>146</v>
@@ -8576,7 +8576,7 @@
         <v>190</v>
       </c>
       <c r="DD34" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement LA's Logic - returned to original data processor test format
[#164636782]

Co-authored-by: Symonne Singleton <symonne@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68BE6A9-1BB6-8B4D-BE63-0CDA8E0F591F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733EAF8A-025E-884E-84E7-46219180C8C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="480" windowWidth="25600" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,9 +466,6 @@
     <t>Eligible for Dismissal</t>
   </si>
   <si>
-    <t>No convictions in past 10 years</t>
-  </si>
-  <si>
     <t>BIRD,BIG</t>
   </si>
   <si>
@@ -592,12 +589,6 @@
     <t>2.7</t>
   </si>
   <si>
-    <t>Eligible for Reduction</t>
-  </si>
-  <si>
-    <t>Has convictions in past 10 years</t>
-  </si>
-  <si>
     <t>CONVICTED-PRISON</t>
   </si>
   <si>
@@ -703,9 +694,6 @@
     <t>11.6</t>
   </si>
   <si>
-    <t>Sentence Completed</t>
-  </si>
-  <si>
     <t>A234698573</t>
   </si>
   <si>
@@ -718,13 +706,25 @@
     <t>4.7</t>
   </si>
   <si>
-    <t>Sentence not Completed</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
     <t>Two priors</t>
+  </si>
+  <si>
+    <t>50 years or older</t>
+  </si>
+  <si>
+    <t>Only has 11357-60 charges and completed sentence</t>
+  </si>
+  <si>
+    <t>21 years or younger</t>
+  </si>
+  <si>
+    <t>Hand Review</t>
+  </si>
+  <si>
+    <t>Currently serving sentence</t>
   </si>
 </sst>
 </file>
@@ -2271,8 +2271,8 @@
   </sheetPr>
   <dimension ref="A1:IW34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CV1" workbookViewId="0">
-      <selection activeCell="CZ51" sqref="CZ51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CX1" workbookViewId="0">
+      <selection activeCell="DD34" sqref="DD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2373,7 +2373,7 @@
     <col min="104" max="104" width="10" style="1" customWidth="1"/>
     <col min="105" max="105" width="20.5" style="1" customWidth="1"/>
     <col min="106" max="107" width="25.83203125" style="1" customWidth="1"/>
-    <col min="108" max="108" width="29.83203125" style="1" customWidth="1"/>
+    <col min="108" max="108" width="41.5" style="1" customWidth="1"/>
     <col min="109" max="257" width="8.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2391,16 +2391,16 @@
       <c r="K1" s="46"/>
       <c r="L1" s="46"/>
       <c r="M1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="N1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="O1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="P1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="Q1" s="46"/>
       <c r="R1" s="46"/>
@@ -2410,7 +2410,7 @@
       <c r="V1" s="46"/>
       <c r="W1" s="46"/>
       <c r="X1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="Y1" s="46"/>
       <c r="Z1" s="46"/>
@@ -2427,12 +2427,12 @@
       <c r="AK1" s="46"/>
       <c r="AL1" s="46"/>
       <c r="AM1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="AN1" s="46"/>
       <c r="AO1" s="46"/>
       <c r="AP1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="AQ1" s="46"/>
       <c r="AR1" s="46"/>
@@ -2440,23 +2440,23 @@
       <c r="AT1" s="46"/>
       <c r="AU1" s="46"/>
       <c r="AV1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="AW1" s="46"/>
       <c r="AX1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="AY1" s="46"/>
       <c r="AZ1" s="46"/>
       <c r="BA1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="BB1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="BC1" s="46"/>
       <c r="BD1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="BE1" s="46"/>
       <c r="BF1" s="46"/>
@@ -2484,76 +2484,76 @@
       <c r="CB1" s="46"/>
       <c r="CC1" s="46"/>
       <c r="CD1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CE1" s="46"/>
       <c r="CF1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CG1" s="46"/>
       <c r="CH1" s="46"/>
       <c r="CI1" s="46"/>
       <c r="CJ1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CK1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CL1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CM1" s="46"/>
       <c r="CN1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CO1" s="46"/>
       <c r="CP1" s="46"/>
       <c r="CQ1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CR1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CS1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CT1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CU1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CV1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CW1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CX1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CY1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="CZ1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="DA1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="DB1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="DC1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="DD1" s="46" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:108" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -3689,7 +3689,7 @@
     </row>
     <row r="8" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -3880,7 +3880,7 @@
         <v>147</v>
       </c>
       <c r="DD8" s="10" t="s">
-        <v>148</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -3906,7 +3906,7 @@
         <v>8690594867</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O9" s="16"/>
       <c r="P9" s="14">
@@ -3916,7 +3916,7 @@
         <v>987654321</v>
       </c>
       <c r="R9" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S9" s="16"/>
       <c r="T9" s="16"/>
@@ -4045,7 +4045,7 @@
     </row>
     <row r="10" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
@@ -4068,7 +4068,7 @@
         <v>8690594867</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O10" s="16"/>
       <c r="P10" s="14">
@@ -4078,7 +4078,7 @@
         <v>987654321</v>
       </c>
       <c r="R10" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S10" s="16"/>
       <c r="T10" s="16"/>
@@ -4134,13 +4134,13 @@
         <v>112</v>
       </c>
       <c r="BD10" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BE10" s="15" t="s">
         <v>114</v>
       </c>
       <c r="BF10" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BG10" s="16"/>
       <c r="BH10" s="16"/>
@@ -4203,10 +4203,10 @@
         <v>107</v>
       </c>
       <c r="CS10" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="CT10" s="15" t="s">
         <v>153</v>
-      </c>
-      <c r="CT10" s="15" t="s">
-        <v>154</v>
       </c>
       <c r="CU10" s="15" t="s">
         <v>143</v>
@@ -4215,16 +4215,16 @@
         <v>143</v>
       </c>
       <c r="CW10" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="CX10" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="CX10" s="15" t="s">
+      <c r="CY10" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="CY10" s="15" t="s">
+      <c r="CZ10" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="CZ10" s="15" t="s">
-        <v>158</v>
       </c>
       <c r="DA10" s="15" t="s">
         <v>142</v>
@@ -4233,10 +4233,10 @@
         <v>143</v>
       </c>
       <c r="DC10" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="DD10" s="15" t="s">
         <v>159</v>
-      </c>
-      <c r="DD10" s="15" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -4262,7 +4262,7 @@
         <v>8690594867</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O11" s="16"/>
       <c r="P11" s="14">
@@ -4272,7 +4272,7 @@
         <v>987654321</v>
       </c>
       <c r="R11" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S11" s="16"/>
       <c r="T11" s="16"/>
@@ -4304,7 +4304,7 @@
       </c>
       <c r="AQ11" s="16"/>
       <c r="AR11" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AS11" s="16"/>
       <c r="AT11" s="16"/>
@@ -4328,11 +4328,11 @@
         <v>112</v>
       </c>
       <c r="BD11" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BE11" s="16"/>
       <c r="BF11" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="BG11" s="16"/>
       <c r="BH11" s="16"/>
@@ -4371,7 +4371,7 @@
       <c r="CK11" s="16"/>
       <c r="CL11" s="16"/>
       <c r="CM11" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="CN11" s="14">
         <v>23</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="12" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
@@ -4420,7 +4420,7 @@
         <v>8690594867</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O12" s="16"/>
       <c r="P12" s="14">
@@ -4430,7 +4430,7 @@
         <v>987654321</v>
       </c>
       <c r="R12" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S12" s="16"/>
       <c r="T12" s="16"/>
@@ -4486,13 +4486,13 @@
         <v>112</v>
       </c>
       <c r="BD12" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="BE12" s="15" t="s">
         <v>114</v>
       </c>
       <c r="BF12" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BG12" s="16"/>
       <c r="BH12" s="16"/>
@@ -4555,10 +4555,10 @@
         <v>107</v>
       </c>
       <c r="CS12" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="CT12" s="15" t="s">
         <v>153</v>
-      </c>
-      <c r="CT12" s="15" t="s">
-        <v>154</v>
       </c>
       <c r="CU12" s="15" t="s">
         <v>143</v>
@@ -4567,16 +4567,16 @@
         <v>143</v>
       </c>
       <c r="CW12" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="CX12" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="CY12" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="CY12" s="15" t="s">
-        <v>167</v>
-      </c>
       <c r="CZ12" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="DA12" s="15" t="s">
         <v>142</v>
@@ -4588,7 +4588,7 @@
         <v>147</v>
       </c>
       <c r="DD12" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -4614,7 +4614,7 @@
         <v>8690594867</v>
       </c>
       <c r="N13" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O13" s="16"/>
       <c r="P13" s="14">
@@ -4624,7 +4624,7 @@
         <v>987654321</v>
       </c>
       <c r="R13" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S13" s="16"/>
       <c r="T13" s="16"/>
@@ -4728,10 +4728,10 @@
         <v>10</v>
       </c>
       <c r="CL13" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="CM13" s="15" t="s">
         <v>169</v>
-      </c>
-      <c r="CM13" s="15" t="s">
-        <v>170</v>
       </c>
       <c r="CN13" s="14">
         <v>23</v>
@@ -4757,7 +4757,7 @@
     </row>
     <row r="14" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -4780,7 +4780,7 @@
         <v>1008675309</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O14" s="21"/>
       <c r="P14" s="19">
@@ -4846,7 +4846,7 @@
         <v>112</v>
       </c>
       <c r="BD14" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="BE14" s="20" t="s">
         <v>114</v>
@@ -4917,10 +4917,10 @@
         <v>107</v>
       </c>
       <c r="CS14" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="CT14" s="20" t="s">
         <v>173</v>
-      </c>
-      <c r="CT14" s="20" t="s">
-        <v>174</v>
       </c>
       <c r="CU14" s="20" t="s">
         <v>143</v>
@@ -4941,7 +4941,7 @@
         <v>145</v>
       </c>
       <c r="DA14" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="DB14" s="20" t="s">
         <v>143</v>
@@ -4950,7 +4950,7 @@
         <v>147</v>
       </c>
       <c r="DD14" s="20" t="s">
-        <v>148</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -4976,7 +4976,7 @@
         <v>1008675309</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O15" s="21"/>
       <c r="P15" s="19">
@@ -5026,7 +5026,7 @@
       <c r="AV15" s="21"/>
       <c r="AW15" s="21"/>
       <c r="AX15" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AY15" s="21"/>
       <c r="AZ15" s="40">
@@ -5146,7 +5146,7 @@
         <v>1008675309</v>
       </c>
       <c r="N16" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O16" s="21"/>
       <c r="P16" s="19">
@@ -5196,7 +5196,7 @@
       <c r="AV16" s="21"/>
       <c r="AW16" s="21"/>
       <c r="AX16" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AY16" s="21"/>
       <c r="AZ16" s="40">
@@ -5295,7 +5295,7 @@
     </row>
     <row r="17" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -5318,7 +5318,7 @@
         <v>1008675309</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O17" s="21"/>
       <c r="P17" s="19">
@@ -5384,13 +5384,13 @@
         <v>112</v>
       </c>
       <c r="BD17" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="BE17" s="20" t="s">
         <v>114</v>
       </c>
       <c r="BF17" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="BG17" s="21"/>
       <c r="BH17" s="21"/>
@@ -5453,10 +5453,10 @@
         <v>107</v>
       </c>
       <c r="CS17" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="CT17" s="20" t="s">
         <v>173</v>
-      </c>
-      <c r="CT17" s="20" t="s">
-        <v>174</v>
       </c>
       <c r="CU17" s="20" t="s">
         <v>143</v>
@@ -5468,16 +5468,16 @@
         <v>143</v>
       </c>
       <c r="CX17" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="CY17" s="20" t="s">
         <v>178</v>
-      </c>
-      <c r="CY17" s="20" t="s">
-        <v>179</v>
       </c>
       <c r="CZ17" s="20" t="s">
         <v>145</v>
       </c>
       <c r="DA17" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="DB17" s="20" t="s">
         <v>143</v>
@@ -5486,7 +5486,7 @@
         <v>147</v>
       </c>
       <c r="DD17" s="20" t="s">
-        <v>148</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -5512,7 +5512,7 @@
         <v>1008675309</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O18" s="21"/>
       <c r="P18" s="19">
@@ -5578,7 +5578,7 @@
         <v>112</v>
       </c>
       <c r="BD18" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="BE18" s="20" t="s">
         <v>114</v>
@@ -5624,7 +5624,7 @@
         <v>138</v>
       </c>
       <c r="CJ18" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CK18" s="19">
         <v>6</v>
@@ -5633,7 +5633,7 @@
         <v>128</v>
       </c>
       <c r="CM18" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="CN18" s="19">
         <v>25</v>
@@ -5677,10 +5677,10 @@
       <c r="K19" s="26"/>
       <c r="L19" s="26"/>
       <c r="M19" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="N19" s="25" t="s">
         <v>183</v>
-      </c>
-      <c r="N19" s="25" t="s">
-        <v>184</v>
       </c>
       <c r="O19" s="26"/>
       <c r="P19" s="24">
@@ -5746,7 +5746,7 @@
         <v>112</v>
       </c>
       <c r="BD19" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="BE19" s="25" t="s">
         <v>114</v>
@@ -5829,7 +5829,7 @@
     </row>
     <row r="20" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
@@ -5849,10 +5849,10 @@
       <c r="K20" s="26"/>
       <c r="L20" s="26"/>
       <c r="M20" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O20" s="26"/>
       <c r="P20" s="24">
@@ -5981,16 +5981,16 @@
         <v>107</v>
       </c>
       <c r="CS20" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="CT20" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="CU20" s="25" t="s">
         <v>143</v>
       </c>
       <c r="CV20" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CW20" s="25" t="s">
         <v>143</v>
@@ -6002,7 +6002,7 @@
         <v>145</v>
       </c>
       <c r="CZ20" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="DA20" s="25" t="s">
         <v>142</v>
@@ -6011,10 +6011,10 @@
         <v>143</v>
       </c>
       <c r="DC20" s="25" t="s">
-        <v>190</v>
+        <v>147</v>
       </c>
       <c r="DD20" s="25" t="s">
-        <v>191</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -6037,10 +6037,10 @@
       <c r="K21" s="26"/>
       <c r="L21" s="26"/>
       <c r="M21" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="N21" s="25" t="s">
         <v>183</v>
-      </c>
-      <c r="N21" s="25" t="s">
-        <v>184</v>
       </c>
       <c r="O21" s="26"/>
       <c r="P21" s="24">
@@ -6106,7 +6106,7 @@
         <v>112</v>
       </c>
       <c r="BD21" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="BE21" s="25" t="s">
         <v>114</v>
@@ -6138,10 +6138,10 @@
       <c r="CB21" s="26"/>
       <c r="CC21" s="26"/>
       <c r="CD21" s="25" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="CE21" s="25" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="CF21" s="25" t="s">
         <v>117</v>
@@ -6154,7 +6154,7 @@
         <v>138</v>
       </c>
       <c r="CJ21" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CK21" s="24">
         <v>6</v>
@@ -6163,7 +6163,7 @@
         <v>128</v>
       </c>
       <c r="CM21" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="CN21" s="24">
         <v>25</v>
@@ -6189,7 +6189,7 @@
     </row>
     <row r="22" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
@@ -6209,10 +6209,10 @@
       <c r="K22" s="26"/>
       <c r="L22" s="26"/>
       <c r="M22" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="N22" s="25" t="s">
         <v>183</v>
-      </c>
-      <c r="N22" s="25" t="s">
-        <v>184</v>
       </c>
       <c r="O22" s="26"/>
       <c r="P22" s="24">
@@ -6313,7 +6313,7 @@
         <v>136</v>
       </c>
       <c r="CE22" s="25" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="CF22" s="25" t="s">
         <v>131</v>
@@ -6335,7 +6335,7 @@
         <v>128</v>
       </c>
       <c r="CM22" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="CN22" s="24">
         <v>61</v>
@@ -6347,28 +6347,28 @@
         <v>107</v>
       </c>
       <c r="CS22" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="CT22" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="CU22" s="25" t="s">
         <v>143</v>
       </c>
       <c r="CV22" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CW22" s="25" t="s">
         <v>143</v>
       </c>
       <c r="CX22" s="25" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="CY22" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="CZ22" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="DA22" s="25" t="s">
         <v>142</v>
@@ -6377,15 +6377,15 @@
         <v>143</v>
       </c>
       <c r="DC22" s="25" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="DD22" s="25" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -6396,7 +6396,7 @@
         <v>107</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
@@ -6405,10 +6405,10 @@
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
       <c r="M23" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N23" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="O23" s="31"/>
       <c r="P23" s="29">
@@ -6506,10 +6506,10 @@
       <c r="CB23" s="31"/>
       <c r="CC23" s="31"/>
       <c r="CD23" s="30" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="CE23" s="30" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="CF23" s="30" t="s">
         <v>117</v>
@@ -6522,7 +6522,7 @@
         <v>138</v>
       </c>
       <c r="CJ23" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CK23" s="29">
         <v>6</v>
@@ -6542,10 +6542,10 @@
         <v>757392</v>
       </c>
       <c r="CT23" s="30" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="CU23" s="30" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="CV23" s="30" t="s">
         <v>143</v>
@@ -6554,25 +6554,25 @@
         <v>143</v>
       </c>
       <c r="CX23" s="30" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="CY23" s="30" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="CZ23" s="30" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DA23" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="DB23" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DC23" s="30" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="DD23" s="30" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -6586,7 +6586,7 @@
         <v>107</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -6595,10 +6595,10 @@
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
       <c r="M24" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N24" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="O24" s="31"/>
       <c r="P24" s="29">
@@ -6664,7 +6664,7 @@
         <v>112</v>
       </c>
       <c r="BD24" s="30" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="BE24" s="30" t="s">
         <v>114</v>
@@ -6696,10 +6696,10 @@
       <c r="CB24" s="31"/>
       <c r="CC24" s="31"/>
       <c r="CD24" s="30" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="CE24" s="30" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="CF24" s="30" t="s">
         <v>117</v>
@@ -6712,7 +6712,7 @@
         <v>138</v>
       </c>
       <c r="CJ24" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CK24" s="29">
         <v>6</v>
@@ -6752,7 +6752,7 @@
         <v>107</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
@@ -6761,10 +6761,10 @@
       <c r="K25" s="31"/>
       <c r="L25" s="31"/>
       <c r="M25" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N25" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="O25" s="31"/>
       <c r="P25" s="29">
@@ -6903,7 +6903,7 @@
     </row>
     <row r="26" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
@@ -6914,7 +6914,7 @@
         <v>107</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
@@ -6923,10 +6923,10 @@
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
       <c r="M26" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N26" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="O26" s="31"/>
       <c r="P26" s="29">
@@ -6990,7 +6990,7 @@
         <v>112</v>
       </c>
       <c r="BD26" s="30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BE26" s="30" t="s">
         <v>128</v>
@@ -7056,10 +7056,10 @@
         <v>757392</v>
       </c>
       <c r="CT26" s="30" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="CU26" s="30" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="CV26" s="30" t="s">
         <v>143</v>
@@ -7068,30 +7068,30 @@
         <v>143</v>
       </c>
       <c r="CX26" s="30" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="CY26" s="30" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="CZ26" s="30" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DA26" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="DB26" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DC26" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="DD26" s="30" t="s">
         <v>159</v>
-      </c>
-      <c r="DD26" s="30" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
@@ -7102,7 +7102,7 @@
         <v>107</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
@@ -7111,10 +7111,10 @@
       <c r="K27" s="31"/>
       <c r="L27" s="31"/>
       <c r="M27" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N27" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="O27" s="31"/>
       <c r="P27" s="29">
@@ -7178,7 +7178,7 @@
         <v>112</v>
       </c>
       <c r="BD27" s="30" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="BE27" s="30" t="s">
         <v>114</v>
@@ -7244,10 +7244,10 @@
         <v>757392</v>
       </c>
       <c r="CT27" s="30" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="CU27" s="30" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="CV27" s="30" t="s">
         <v>143</v>
@@ -7256,30 +7256,30 @@
         <v>143</v>
       </c>
       <c r="CX27" s="30" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="CY27" s="30" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="CZ27" s="30" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="DA27" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="DB27" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DC27" s="30" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="DD27" s="30" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
@@ -7302,11 +7302,11 @@
         <v>1008675309</v>
       </c>
       <c r="N28" s="35" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="O28" s="36"/>
       <c r="P28" s="34">
-        <v>19690314</v>
+        <v>19890314</v>
       </c>
       <c r="Q28" s="34">
         <v>743894322</v>
@@ -7368,13 +7368,13 @@
         <v>112</v>
       </c>
       <c r="BD28" s="35" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="BE28" s="35" t="s">
         <v>114</v>
       </c>
       <c r="BF28" s="35" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="BG28" s="36"/>
       <c r="BH28" s="36"/>
@@ -7416,7 +7416,7 @@
         <v>138</v>
       </c>
       <c r="CJ28" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CK28" s="34">
         <v>6</v>
@@ -7425,7 +7425,7 @@
         <v>128</v>
       </c>
       <c r="CM28" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="CN28" s="34">
         <v>25</v>
@@ -7437,10 +7437,10 @@
         <v>107</v>
       </c>
       <c r="CS28" s="35" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="CT28" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CU28" s="35" t="s">
         <v>143</v>
@@ -7452,25 +7452,25 @@
         <v>143</v>
       </c>
       <c r="CX28" s="35" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="CY28" s="35" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="CZ28" s="35" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="DA28" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="DB28" s="35" t="s">
         <v>143</v>
       </c>
       <c r="DC28" s="35" t="s">
-        <v>190</v>
+        <v>147</v>
       </c>
       <c r="DD28" s="35" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -7496,11 +7496,11 @@
         <v>1008675309</v>
       </c>
       <c r="N29" s="35" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="O29" s="36"/>
       <c r="P29" s="34">
-        <v>19690314</v>
+        <v>19890314</v>
       </c>
       <c r="Q29" s="34">
         <v>743894322</v>
@@ -7546,7 +7546,7 @@
       <c r="AV29" s="36"/>
       <c r="AW29" s="36"/>
       <c r="AX29" s="35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AY29" s="36"/>
       <c r="AZ29" s="43">
@@ -7562,13 +7562,13 @@
         <v>112</v>
       </c>
       <c r="BD29" s="35" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="BE29" s="35" t="s">
         <v>114</v>
       </c>
       <c r="BF29" s="35" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="BG29" s="36"/>
       <c r="BH29" s="36"/>
@@ -7610,7 +7610,7 @@
         <v>138</v>
       </c>
       <c r="CJ29" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CK29" s="34">
         <v>6</v>
@@ -7619,7 +7619,7 @@
         <v>128</v>
       </c>
       <c r="CM29" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="CN29" s="34">
         <v>25</v>
@@ -7645,7 +7645,7 @@
     </row>
     <row r="30" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="33"/>
@@ -7668,11 +7668,11 @@
         <v>1008675309</v>
       </c>
       <c r="N30" s="35" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="O30" s="36"/>
       <c r="P30" s="34">
-        <v>19690314</v>
+        <v>19890314</v>
       </c>
       <c r="Q30" s="34">
         <v>743894322</v>
@@ -7734,13 +7734,13 @@
         <v>112</v>
       </c>
       <c r="BD30" s="35" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="BE30" s="35" t="s">
         <v>128</v>
       </c>
       <c r="BF30" s="35" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="BG30" s="36"/>
       <c r="BH30" s="36"/>
@@ -7782,7 +7782,7 @@
         <v>138</v>
       </c>
       <c r="CJ30" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CK30" s="34">
         <v>6</v>
@@ -7791,7 +7791,7 @@
         <v>128</v>
       </c>
       <c r="CM30" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="CN30" s="34">
         <v>25</v>
@@ -7803,10 +7803,10 @@
         <v>107</v>
       </c>
       <c r="CS30" s="35" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="CT30" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CU30" s="35" t="s">
         <v>143</v>
@@ -7818,30 +7818,30 @@
         <v>143</v>
       </c>
       <c r="CX30" s="35" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="CY30" s="35" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="CZ30" s="35" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="DA30" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="DB30" s="35" t="s">
         <v>143</v>
       </c>
       <c r="DC30" s="35" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="DD30" s="35" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -7861,10 +7861,10 @@
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
       <c r="M31" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="9">
@@ -7999,13 +7999,13 @@
         <v>107</v>
       </c>
       <c r="CS31" s="10" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="CT31" s="10" t="s">
         <v>142</v>
       </c>
       <c r="CU31" s="10" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="CV31" s="10" t="s">
         <v>143</v>
@@ -8014,13 +8014,13 @@
         <v>143</v>
       </c>
       <c r="CX31" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="CY31" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="CZ31" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="DA31" s="10" t="s">
         <v>146</v>
@@ -8029,10 +8029,10 @@
         <v>143</v>
       </c>
       <c r="DC31" s="10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="DD31" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -8055,10 +8055,10 @@
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
       <c r="M32" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="9">
@@ -8124,13 +8124,13 @@
         <v>112</v>
       </c>
       <c r="BD32" s="10" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="BE32" s="10" t="s">
         <v>114</v>
       </c>
       <c r="BF32" s="10" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="BG32" s="11"/>
       <c r="BH32" s="11"/>
@@ -8207,7 +8207,7 @@
     </row>
     <row r="33" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
@@ -8227,10 +8227,10 @@
       <c r="K33" s="16"/>
       <c r="L33" s="16"/>
       <c r="M33" s="15" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="14">
@@ -8342,10 +8342,10 @@
         <v>10</v>
       </c>
       <c r="CL33" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="CM33" s="15" t="s">
         <v>169</v>
-      </c>
-      <c r="CM33" s="15" t="s">
-        <v>170</v>
       </c>
       <c r="CN33" s="14">
         <v>2</v>
@@ -8370,13 +8370,13 @@
         <v>143</v>
       </c>
       <c r="CX33" s="15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="CY33" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="CZ33" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="DA33" s="15" t="s">
         <v>146</v>
@@ -8388,12 +8388,12 @@
         <v>147</v>
       </c>
       <c r="DD33" s="15" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="34" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="50" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
@@ -8413,10 +8413,10 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
       <c r="M34" s="20" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="N34" s="20" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="O34" s="21"/>
       <c r="P34" s="19">
@@ -8530,10 +8530,10 @@
         <v>5</v>
       </c>
       <c r="CL34" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="CM34" s="20" t="s">
         <v>169</v>
-      </c>
-      <c r="CM34" s="20" t="s">
-        <v>170</v>
       </c>
       <c r="CN34" s="19">
         <v>35</v>
@@ -8558,13 +8558,13 @@
         <v>143</v>
       </c>
       <c r="CX34" s="20" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="CY34" s="20" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="CZ34" s="20" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="DA34" s="20" t="s">
         <v>146</v>
@@ -8573,10 +8573,10 @@
         <v>143</v>
       </c>
       <c r="DC34" s="20" t="s">
-        <v>190</v>
+        <v>233</v>
       </c>
       <c r="DD34" s="20" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP - failing test in Los Angeles - cannot handle case where there are related charges in the hypothetical, but not in the county
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733EAF8A-025E-884E-84E7-46219180C8C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFC3759-73F7-CD4E-9BB3-BF3EF33812CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="480" windowWidth="25600" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="235">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -676,9 +676,6 @@
     <t>187 PC</t>
   </si>
   <si>
-    <t>187 PC-MURDER</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                     </t>
   </si>
   <si>
@@ -725,6 +722,9 @@
   </si>
   <si>
     <t>Currently serving sentence</t>
+  </si>
+  <si>
+    <t>466 PC-SOMETHING</t>
   </si>
 </sst>
 </file>
@@ -952,7 +952,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1107,6 +1107,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2271,108 +2277,110 @@
   </sheetPr>
   <dimension ref="A1:IW34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CX1" workbookViewId="0">
-      <selection activeCell="DD34" sqref="DD34"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="BD32" sqref="BD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="49"/>
-    <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.33203125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="12" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="9.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="12" style="1" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="18.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.83203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="1" customWidth="1"/>
-    <col min="19" max="20" width="8" style="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="13.33203125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="11.83203125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="12.83203125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="18.33203125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="18" style="1" customWidth="1"/>
-    <col min="28" max="28" width="19" style="1" customWidth="1"/>
-    <col min="29" max="29" width="7.83203125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="8.1640625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="15.5" style="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5" style="1" customWidth="1"/>
-    <col min="33" max="33" width="10.6640625" style="1" customWidth="1"/>
-    <col min="34" max="34" width="10.83203125" style="1" customWidth="1"/>
-    <col min="35" max="35" width="10.1640625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="16.5" style="1" customWidth="1"/>
-    <col min="37" max="37" width="13.5" style="1" customWidth="1"/>
-    <col min="38" max="38" width="11.83203125" style="1" customWidth="1"/>
-    <col min="39" max="39" width="10.1640625" style="1" customWidth="1"/>
-    <col min="40" max="40" width="13" style="1" customWidth="1"/>
-    <col min="41" max="41" width="11.5" style="1" customWidth="1"/>
-    <col min="42" max="42" width="16.1640625" style="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5" style="1" customWidth="1"/>
-    <col min="44" max="44" width="21.6640625" style="1" customWidth="1"/>
-    <col min="45" max="45" width="13.6640625" style="1" customWidth="1"/>
-    <col min="46" max="46" width="20.33203125" style="1" customWidth="1"/>
-    <col min="47" max="47" width="14.1640625" style="1" customWidth="1"/>
-    <col min="48" max="48" width="19.5" style="1" customWidth="1"/>
-    <col min="49" max="50" width="19.6640625" style="1" customWidth="1"/>
-    <col min="51" max="51" width="13.33203125" style="1" customWidth="1"/>
-    <col min="52" max="52" width="19.33203125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="10.5" style="1" customWidth="1"/>
-    <col min="54" max="54" width="7" style="1" customWidth="1"/>
-    <col min="55" max="55" width="14.83203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="8" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="13.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="11.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="12.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="18.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="18" style="1" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="19" style="1" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="7.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="8.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="15.5" style="1" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="14.5" style="1" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="10.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="10.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="10.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="16.5" style="1" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="13.5" style="1" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="11.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="10.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="13" style="1" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="11.5" style="1" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="16.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5" style="1" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="21.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="45" max="45" width="13.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="46" max="46" width="20.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="14.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="19.5" style="1" hidden="1" customWidth="1"/>
+    <col min="49" max="49" width="19.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="19.6640625" style="1" customWidth="1"/>
+    <col min="51" max="51" width="13.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="19.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="10.5" style="1" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="7" style="1" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="14.83203125" style="1" hidden="1" customWidth="1"/>
     <col min="56" max="56" width="37.6640625" style="1" customWidth="1"/>
     <col min="57" max="57" width="13.6640625" style="1" customWidth="1"/>
-    <col min="58" max="58" width="18.6640625" style="1" customWidth="1"/>
-    <col min="59" max="59" width="19.6640625" style="1" customWidth="1"/>
-    <col min="60" max="60" width="20.6640625" style="1" customWidth="1"/>
-    <col min="61" max="61" width="18.33203125" style="1" customWidth="1"/>
-    <col min="62" max="62" width="23.33203125" style="1" customWidth="1"/>
-    <col min="63" max="63" width="21.6640625" style="1" customWidth="1"/>
-    <col min="64" max="64" width="20.5" style="1" customWidth="1"/>
-    <col min="65" max="65" width="21.5" style="1" customWidth="1"/>
-    <col min="66" max="66" width="19.33203125" style="1" customWidth="1"/>
-    <col min="67" max="67" width="24.33203125" style="1" customWidth="1"/>
-    <col min="68" max="68" width="15.1640625" style="1" customWidth="1"/>
-    <col min="69" max="69" width="17.1640625" style="1" customWidth="1"/>
-    <col min="70" max="70" width="20" style="1" customWidth="1"/>
-    <col min="71" max="71" width="13" style="1" customWidth="1"/>
-    <col min="72" max="72" width="16.33203125" style="1" customWidth="1"/>
-    <col min="73" max="74" width="17.1640625" style="1" customWidth="1"/>
-    <col min="75" max="77" width="16.6640625" style="1" customWidth="1"/>
-    <col min="78" max="78" width="18" style="1" customWidth="1"/>
-    <col min="79" max="79" width="17.6640625" style="1" customWidth="1"/>
-    <col min="80" max="80" width="12.1640625" style="1" customWidth="1"/>
-    <col min="81" max="81" width="11" style="1" customWidth="1"/>
-    <col min="82" max="82" width="26.33203125" style="1" customWidth="1"/>
-    <col min="83" max="83" width="16.83203125" style="1" customWidth="1"/>
+    <col min="58" max="58" width="18.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="19.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="60" max="60" width="20.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="18.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="23.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="63" max="63" width="21.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="64" max="64" width="20.5" style="1" hidden="1" customWidth="1"/>
+    <col min="65" max="65" width="21.5" style="1" hidden="1" customWidth="1"/>
+    <col min="66" max="66" width="19.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="24.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="15.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="69" max="69" width="17.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="20" style="1" hidden="1" customWidth="1"/>
+    <col min="71" max="71" width="13" style="1" hidden="1" customWidth="1"/>
+    <col min="72" max="72" width="16.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="73" max="74" width="17.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="75" max="77" width="16.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="78" max="78" width="18" style="1" hidden="1" customWidth="1"/>
+    <col min="79" max="79" width="17.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="80" max="80" width="12.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="81" max="81" width="11" style="1" hidden="1" customWidth="1"/>
+    <col min="82" max="82" width="26.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="83" max="83" width="16.83203125" style="1" hidden="1" customWidth="1"/>
     <col min="84" max="84" width="17.6640625" style="1" customWidth="1"/>
-    <col min="85" max="85" width="14.33203125" style="1" customWidth="1"/>
-    <col min="86" max="86" width="12.6640625" style="1" customWidth="1"/>
-    <col min="87" max="87" width="16" style="1" customWidth="1"/>
-    <col min="88" max="88" width="16.83203125" style="1" customWidth="1"/>
-    <col min="89" max="89" width="13.5" style="1" customWidth="1"/>
-    <col min="90" max="90" width="16.5" style="1" customWidth="1"/>
-    <col min="91" max="91" width="109.5" style="1" customWidth="1"/>
-    <col min="92" max="92" width="9.33203125" style="1" customWidth="1"/>
-    <col min="93" max="93" width="8.83203125" style="1" customWidth="1"/>
-    <col min="94" max="94" width="15.33203125" style="1" customWidth="1"/>
-    <col min="95" max="95" width="26.83203125" style="1" customWidth="1"/>
-    <col min="96" max="96" width="12.5" style="1" customWidth="1"/>
-    <col min="97" max="97" width="29.6640625" style="1" customWidth="1"/>
-    <col min="98" max="98" width="24" style="1" customWidth="1"/>
-    <col min="99" max="101" width="23.6640625" style="1" customWidth="1"/>
-    <col min="102" max="103" width="12.5" style="1" customWidth="1"/>
-    <col min="104" max="104" width="10" style="1" customWidth="1"/>
-    <col min="105" max="105" width="20.5" style="1" customWidth="1"/>
-    <col min="106" max="107" width="25.83203125" style="1" customWidth="1"/>
+    <col min="85" max="85" width="14.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="86" max="86" width="12.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="87" max="87" width="16" style="1" hidden="1" customWidth="1"/>
+    <col min="88" max="88" width="16.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="89" max="89" width="13.5" style="1" hidden="1" customWidth="1"/>
+    <col min="90" max="90" width="16.5" style="1" hidden="1" customWidth="1"/>
+    <col min="91" max="91" width="109.5" style="1" hidden="1" customWidth="1"/>
+    <col min="92" max="92" width="9.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="93" max="93" width="8.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="94" max="94" width="15.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="95" max="95" width="26.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="96" max="96" width="12.5" style="1" hidden="1" customWidth="1"/>
+    <col min="97" max="97" width="29.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="98" max="98" width="24" style="1" hidden="1" customWidth="1"/>
+    <col min="99" max="101" width="23.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="102" max="103" width="12.5" style="1" hidden="1" customWidth="1"/>
+    <col min="104" max="104" width="10" style="1" hidden="1" customWidth="1"/>
+    <col min="105" max="105" width="20.5" style="1" hidden="1" customWidth="1"/>
+    <col min="106" max="106" width="25.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="107" max="107" width="25.83203125" style="1" customWidth="1"/>
     <col min="108" max="108" width="41.5" style="1" customWidth="1"/>
     <col min="109" max="257" width="8.33203125" style="1" customWidth="1"/>
   </cols>
@@ -2391,16 +2399,16 @@
       <c r="K1" s="46"/>
       <c r="L1" s="46"/>
       <c r="M1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q1" s="46"/>
       <c r="R1" s="46"/>
@@ -2410,7 +2418,7 @@
       <c r="V1" s="46"/>
       <c r="W1" s="46"/>
       <c r="X1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Y1" s="46"/>
       <c r="Z1" s="46"/>
@@ -2427,12 +2435,12 @@
       <c r="AK1" s="46"/>
       <c r="AL1" s="46"/>
       <c r="AM1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AN1" s="46"/>
       <c r="AO1" s="46"/>
       <c r="AP1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AQ1" s="46"/>
       <c r="AR1" s="46"/>
@@ -2440,23 +2448,23 @@
       <c r="AT1" s="46"/>
       <c r="AU1" s="46"/>
       <c r="AV1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AW1" s="46"/>
       <c r="AX1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AY1" s="46"/>
       <c r="AZ1" s="46"/>
       <c r="BA1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="BB1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="BC1" s="46"/>
       <c r="BD1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="BE1" s="46"/>
       <c r="BF1" s="46"/>
@@ -2484,76 +2492,76 @@
       <c r="CB1" s="46"/>
       <c r="CC1" s="46"/>
       <c r="CD1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CE1" s="46"/>
       <c r="CF1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CG1" s="46"/>
       <c r="CH1" s="46"/>
       <c r="CI1" s="46"/>
       <c r="CJ1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CK1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CL1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CM1" s="46"/>
       <c r="CN1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CO1" s="46"/>
       <c r="CP1" s="46"/>
       <c r="CQ1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CR1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CS1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CT1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CU1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CV1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CW1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CX1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CY1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="CZ1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="DA1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="DB1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="DC1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="DD1" s="46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:108" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -3689,7 +3697,7 @@
     </row>
     <row r="8" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -3880,7 +3888,7 @@
         <v>147</v>
       </c>
       <c r="DD8" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -4045,7 +4053,7 @@
     </row>
     <row r="10" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
@@ -4397,7 +4405,7 @@
     </row>
     <row r="12" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
@@ -4757,7 +4765,7 @@
     </row>
     <row r="14" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -4950,7 +4958,7 @@
         <v>147</v>
       </c>
       <c r="DD14" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -5295,7 +5303,7 @@
     </row>
     <row r="17" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -5486,7 +5494,7 @@
         <v>147</v>
       </c>
       <c r="DD17" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -5829,7 +5837,7 @@
     </row>
     <row r="20" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
@@ -6014,7 +6022,7 @@
         <v>147</v>
       </c>
       <c r="DD20" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -6189,7 +6197,7 @@
     </row>
     <row r="22" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
@@ -6385,7 +6393,7 @@
     </row>
     <row r="23" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -6903,7 +6911,7 @@
     </row>
     <row r="26" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
@@ -7091,7 +7099,7 @@
     </row>
     <row r="27" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
@@ -7279,7 +7287,7 @@
     </row>
     <row r="28" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
@@ -7470,7 +7478,7 @@
         <v>147</v>
       </c>
       <c r="DD28" s="35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -7645,7 +7653,7 @@
     </row>
     <row r="30" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="33"/>
@@ -7836,12 +7844,12 @@
         <v>192</v>
       </c>
       <c r="DD30" s="35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -8123,14 +8131,14 @@
       <c r="BC32" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="BD32" s="10" t="s">
-        <v>218</v>
+      <c r="BD32" s="52" t="s">
+        <v>234</v>
       </c>
       <c r="BE32" s="10" t="s">
         <v>114</v>
       </c>
       <c r="BF32" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="BG32" s="11"/>
       <c r="BH32" s="11"/>
@@ -8207,7 +8215,7 @@
     </row>
     <row r="33" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
@@ -8227,10 +8235,10 @@
       <c r="K33" s="16"/>
       <c r="L33" s="16"/>
       <c r="M33" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="N33" s="15" t="s">
         <v>220</v>
-      </c>
-      <c r="N33" s="15" t="s">
-        <v>221</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="14">
@@ -8327,7 +8335,9 @@
         <v>136</v>
       </c>
       <c r="CE33" s="16"/>
-      <c r="CF33" s="16"/>
+      <c r="CF33" s="53" t="s">
+        <v>117</v>
+      </c>
       <c r="CG33" s="15" t="s">
         <v>107</v>
       </c>
@@ -8370,13 +8380,13 @@
         <v>143</v>
       </c>
       <c r="CX33" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="CY33" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="CY33" s="15" t="s">
-        <v>223</v>
-      </c>
       <c r="CZ33" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="DA33" s="15" t="s">
         <v>146</v>
@@ -8388,12 +8398,12 @@
         <v>147</v>
       </c>
       <c r="DD33" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="50" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
@@ -8413,10 +8423,10 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
       <c r="M34" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="N34" s="20" t="s">
         <v>224</v>
-      </c>
-      <c r="N34" s="20" t="s">
-        <v>225</v>
       </c>
       <c r="O34" s="21"/>
       <c r="P34" s="19">
@@ -8558,13 +8568,13 @@
         <v>143</v>
       </c>
       <c r="CX34" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="CY34" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="CY34" s="20" t="s">
-        <v>227</v>
-      </c>
       <c r="CZ34" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="DA34" s="20" t="s">
         <v>146</v>
@@ -8573,10 +8583,10 @@
         <v>143</v>
       </c>
       <c r="DC34" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="DD34" s="20" t="s">
         <v>233</v>
-      </c>
-      <c r="DD34" s="20" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip - tests still failing? - when a non related charges county runs eligibility, it does not catch the non p64 charge in the count
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFC3759-73F7-CD4E-9BB3-BF3EF33812CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88719EC1-CEC3-9446-BEE9-5198C715263E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="480" windowWidth="25600" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -2277,8 +2277,8 @@
   </sheetPr>
   <dimension ref="A1:IW34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="BD32" sqref="BD32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="BD8" sqref="AX1:BD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
All related charges flow includes related charge convictions in flow
[#164636782]

Co-authored-by: Symonne Singleton <symonne@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
-  <workbookPr date1904="1" codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88719EC1-CEC3-9446-BEE9-5198C715263E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
+  <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="38740" windowHeight="22040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="234">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -671,9 +670,6 @@
   </si>
   <si>
     <t>140196; 140134</t>
-  </si>
-  <si>
-    <t>187 PC</t>
   </si>
   <si>
     <t xml:space="preserve">                                     </t>
@@ -730,11 +726,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000000000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -753,8 +749,25 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="205"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -801,6 +814,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -947,12 +966,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1115,12 +1140,20 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2271,17 +2304,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IW34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="BD8" sqref="AX1:BD1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CT1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="DD27" sqref="DD27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="49"/>
     <col min="2" max="2" width="11.33203125" style="1" hidden="1" customWidth="1"/>
@@ -2332,7 +2365,7 @@
     <col min="50" max="50" width="19.6640625" style="1" customWidth="1"/>
     <col min="51" max="51" width="13.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="52" max="52" width="19.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="10.5" style="1" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="10.5" style="1" customWidth="1"/>
     <col min="54" max="54" width="7" style="1" hidden="1" customWidth="1"/>
     <col min="55" max="55" width="14.83203125" style="1" hidden="1" customWidth="1"/>
     <col min="56" max="56" width="37.6640625" style="1" customWidth="1"/>
@@ -2361,31 +2394,30 @@
     <col min="82" max="82" width="26.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="83" max="83" width="16.83203125" style="1" hidden="1" customWidth="1"/>
     <col min="84" max="84" width="17.6640625" style="1" customWidth="1"/>
-    <col min="85" max="85" width="14.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="86" max="86" width="12.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="87" max="87" width="16" style="1" hidden="1" customWidth="1"/>
-    <col min="88" max="88" width="16.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="89" max="89" width="13.5" style="1" hidden="1" customWidth="1"/>
-    <col min="90" max="90" width="16.5" style="1" hidden="1" customWidth="1"/>
-    <col min="91" max="91" width="109.5" style="1" hidden="1" customWidth="1"/>
-    <col min="92" max="92" width="9.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="93" max="93" width="8.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="94" max="94" width="15.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="95" max="95" width="26.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="96" max="96" width="12.5" style="1" hidden="1" customWidth="1"/>
-    <col min="97" max="97" width="29.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="98" max="98" width="24" style="1" hidden="1" customWidth="1"/>
-    <col min="99" max="101" width="23.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="102" max="103" width="12.5" style="1" hidden="1" customWidth="1"/>
-    <col min="104" max="104" width="10" style="1" hidden="1" customWidth="1"/>
-    <col min="105" max="105" width="20.5" style="1" hidden="1" customWidth="1"/>
-    <col min="106" max="106" width="25.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="107" max="107" width="25.83203125" style="1" customWidth="1"/>
+    <col min="85" max="85" width="14.33203125" style="1" customWidth="1"/>
+    <col min="86" max="86" width="12.6640625" style="1" customWidth="1"/>
+    <col min="87" max="87" width="16" style="1" customWidth="1"/>
+    <col min="88" max="88" width="16.83203125" style="1" customWidth="1"/>
+    <col min="89" max="89" width="13.5" style="1" customWidth="1"/>
+    <col min="90" max="90" width="16.5" style="1" customWidth="1"/>
+    <col min="91" max="91" width="109.5" style="1" customWidth="1"/>
+    <col min="92" max="92" width="9.33203125" style="1" customWidth="1"/>
+    <col min="93" max="93" width="8.83203125" style="1" customWidth="1"/>
+    <col min="94" max="94" width="15.33203125" style="1" customWidth="1"/>
+    <col min="95" max="95" width="26.83203125" style="1" customWidth="1"/>
+    <col min="96" max="96" width="12.5" style="1" customWidth="1"/>
+    <col min="97" max="97" width="29.6640625" style="1" customWidth="1"/>
+    <col min="98" max="98" width="24" style="1" customWidth="1"/>
+    <col min="99" max="101" width="23.6640625" style="1" customWidth="1"/>
+    <col min="102" max="103" width="12.5" style="1" customWidth="1"/>
+    <col min="104" max="104" width="10" style="1" customWidth="1"/>
+    <col min="105" max="105" width="20.5" style="1" customWidth="1"/>
+    <col min="106" max="107" width="25.83203125" style="1" customWidth="1"/>
     <col min="108" max="108" width="41.5" style="1" customWidth="1"/>
     <col min="109" max="257" width="8.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:108" s="47" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:108" s="47" customFormat="1" ht="27.75" customHeight="1">
       <c r="A1" s="48"/>
       <c r="B1" s="44"/>
       <c r="C1" s="45"/>
@@ -2399,16 +2431,16 @@
       <c r="K1" s="46"/>
       <c r="L1" s="46"/>
       <c r="M1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q1" s="46"/>
       <c r="R1" s="46"/>
@@ -2418,7 +2450,7 @@
       <c r="V1" s="46"/>
       <c r="W1" s="46"/>
       <c r="X1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Y1" s="46"/>
       <c r="Z1" s="46"/>
@@ -2435,12 +2467,12 @@
       <c r="AK1" s="46"/>
       <c r="AL1" s="46"/>
       <c r="AM1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AN1" s="46"/>
       <c r="AO1" s="46"/>
       <c r="AP1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AQ1" s="46"/>
       <c r="AR1" s="46"/>
@@ -2448,23 +2480,23 @@
       <c r="AT1" s="46"/>
       <c r="AU1" s="46"/>
       <c r="AV1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AW1" s="46"/>
       <c r="AX1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AY1" s="46"/>
       <c r="AZ1" s="46"/>
       <c r="BA1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="BB1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="BC1" s="46"/>
       <c r="BD1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="BE1" s="46"/>
       <c r="BF1" s="46"/>
@@ -2492,76 +2524,76 @@
       <c r="CB1" s="46"/>
       <c r="CC1" s="46"/>
       <c r="CD1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CE1" s="46"/>
       <c r="CF1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CG1" s="46"/>
       <c r="CH1" s="46"/>
       <c r="CI1" s="46"/>
       <c r="CJ1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CK1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CL1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CM1" s="46"/>
       <c r="CN1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CO1" s="46"/>
       <c r="CP1" s="46"/>
       <c r="CQ1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CR1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CS1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CT1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CU1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CV1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CW1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CX1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CY1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="CZ1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="DA1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="DB1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="DC1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="DD1" s="46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:108" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:108" ht="20.25" customHeight="1">
       <c r="A2" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2885,7 +2917,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:108" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:108" ht="20.25" customHeight="1">
       <c r="A3" s="50"/>
       <c r="B3" s="3"/>
       <c r="C3" s="51"/>
@@ -3045,7 +3077,7 @@
       <c r="DC3" s="6"/>
       <c r="DD3" s="6"/>
     </row>
-    <row r="4" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:108" ht="20" customHeight="1">
       <c r="A4" s="50"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -3215,7 +3247,7 @@
       <c r="DC4" s="11"/>
       <c r="DD4" s="11"/>
     </row>
-    <row r="5" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:108" ht="20" customHeight="1">
       <c r="A5" s="50"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -3375,7 +3407,7 @@
       <c r="DC5" s="11"/>
       <c r="DD5" s="11"/>
     </row>
-    <row r="6" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:108" ht="20" customHeight="1">
       <c r="A6" s="50"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -3535,7 +3567,7 @@
       <c r="DC6" s="11"/>
       <c r="DD6" s="11"/>
     </row>
-    <row r="7" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:108" ht="20" customHeight="1">
       <c r="A7" s="50"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -3695,9 +3727,9 @@
       <c r="DC7" s="11"/>
       <c r="DD7" s="11"/>
     </row>
-    <row r="8" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:108" ht="20" customHeight="1">
       <c r="A8" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -3888,10 +3920,10 @@
         <v>147</v>
       </c>
       <c r="DD8" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:108" ht="20" customHeight="1">
       <c r="A9" s="50"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
@@ -4051,9 +4083,9 @@
       <c r="DC9" s="16"/>
       <c r="DD9" s="16"/>
     </row>
-    <row r="10" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:108" ht="20" customHeight="1">
       <c r="A10" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
@@ -4247,7 +4279,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:108" ht="20" customHeight="1">
       <c r="A11" s="50"/>
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
@@ -4403,9 +4435,9 @@
       <c r="DC11" s="16"/>
       <c r="DD11" s="16"/>
     </row>
-    <row r="12" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:108" ht="20" customHeight="1">
       <c r="A12" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
@@ -4599,7 +4631,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:108" ht="20" customHeight="1">
       <c r="A13" s="50"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
@@ -4763,9 +4795,9 @@
       <c r="DC13" s="16"/>
       <c r="DD13" s="16"/>
     </row>
-    <row r="14" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:108" ht="20" customHeight="1">
       <c r="A14" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -4958,10 +4990,10 @@
         <v>147</v>
       </c>
       <c r="DD14" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:108" ht="20" customHeight="1">
       <c r="A15" s="50"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -5131,7 +5163,7 @@
       <c r="DC15" s="21"/>
       <c r="DD15" s="21"/>
     </row>
-    <row r="16" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:108" ht="20" customHeight="1">
       <c r="A16" s="50"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -5301,9 +5333,9 @@
       <c r="DC16" s="21"/>
       <c r="DD16" s="21"/>
     </row>
-    <row r="17" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:108" ht="20" customHeight="1">
       <c r="A17" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -5494,10 +5526,10 @@
         <v>147</v>
       </c>
       <c r="DD17" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
-    <row r="18" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:108" ht="20" customHeight="1">
       <c r="A18" s="50"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
@@ -5665,7 +5697,7 @@
       <c r="DC18" s="21"/>
       <c r="DD18" s="21"/>
     </row>
-    <row r="19" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:108" ht="20" customHeight="1">
       <c r="A19" s="50"/>
       <c r="B19" s="22"/>
       <c r="C19" s="23"/>
@@ -5835,9 +5867,9 @@
       <c r="DC19" s="26"/>
       <c r="DD19" s="26"/>
     </row>
-    <row r="20" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:108" ht="20" customHeight="1">
       <c r="A20" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
@@ -6022,10 +6054,10 @@
         <v>147</v>
       </c>
       <c r="DD20" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
-    <row r="21" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:108" ht="20" customHeight="1">
       <c r="A21" s="50"/>
       <c r="B21" s="22"/>
       <c r="C21" s="23"/>
@@ -6195,9 +6227,9 @@
       <c r="DC21" s="26"/>
       <c r="DD21" s="26"/>
     </row>
-    <row r="22" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:108" ht="20" customHeight="1">
       <c r="A22" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
@@ -6391,9 +6423,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="23" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:108" ht="20" customHeight="1">
       <c r="A23" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -6583,7 +6615,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:108" ht="20" customHeight="1">
       <c r="A24" s="50"/>
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
@@ -6749,7 +6781,7 @@
       <c r="DC24" s="31"/>
       <c r="DD24" s="31"/>
     </row>
-    <row r="25" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:108" ht="20" customHeight="1">
       <c r="A25" s="50"/>
       <c r="B25" s="27"/>
       <c r="C25" s="28"/>
@@ -6909,9 +6941,9 @@
       <c r="DC25" s="31"/>
       <c r="DD25" s="31"/>
     </row>
-    <row r="26" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:108" ht="20" customHeight="1">
       <c r="A26" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
@@ -7097,9 +7129,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:108" ht="20" customHeight="1">
       <c r="A27" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
@@ -7285,9 +7317,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:108" ht="20" customHeight="1">
       <c r="A28" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
@@ -7478,10 +7510,10 @@
         <v>147</v>
       </c>
       <c r="DD28" s="35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
-    <row r="29" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:108" ht="20" customHeight="1">
       <c r="A29" s="50"/>
       <c r="B29" s="32"/>
       <c r="C29" s="33"/>
@@ -7651,9 +7683,9 @@
       <c r="DC29" s="36"/>
       <c r="DD29" s="36"/>
     </row>
-    <row r="30" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:108" ht="20" customHeight="1">
       <c r="A30" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="33"/>
@@ -7844,12 +7876,12 @@
         <v>192</v>
       </c>
       <c r="DD30" s="35" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
-    <row r="31" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:108" ht="20" customHeight="1">
       <c r="A31" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -8012,8 +8044,8 @@
       <c r="CT31" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="CU31" s="10" t="s">
-        <v>217</v>
+      <c r="CU31" s="54" t="s">
+        <v>143</v>
       </c>
       <c r="CV31" s="10" t="s">
         <v>143</v>
@@ -8036,14 +8068,14 @@
       <c r="DB31" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="DC31" s="10" t="s">
-        <v>192</v>
+      <c r="DC31" s="55" t="s">
+        <v>147</v>
       </c>
       <c r="DD31" s="10" t="s">
-        <v>201</v>
+        <v>228</v>
       </c>
     </row>
-    <row r="32" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:108" ht="20" customHeight="1">
       <c r="A32" s="50"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
@@ -8132,13 +8164,13 @@
         <v>112</v>
       </c>
       <c r="BD32" s="52" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BE32" s="10" t="s">
         <v>114</v>
       </c>
       <c r="BF32" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="BG32" s="11"/>
       <c r="BH32" s="11"/>
@@ -8213,9 +8245,9 @@
       <c r="DC32" s="11"/>
       <c r="DD32" s="11"/>
     </row>
-    <row r="33" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:108" ht="20" customHeight="1">
       <c r="A33" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
@@ -8235,10 +8267,10 @@
       <c r="K33" s="16"/>
       <c r="L33" s="16"/>
       <c r="M33" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="N33" s="15" t="s">
         <v>219</v>
-      </c>
-      <c r="N33" s="15" t="s">
-        <v>220</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="14">
@@ -8380,13 +8412,13 @@
         <v>143</v>
       </c>
       <c r="CX33" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="CY33" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="CY33" s="15" t="s">
-        <v>222</v>
-      </c>
       <c r="CZ33" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="DA33" s="15" t="s">
         <v>146</v>
@@ -8398,12 +8430,12 @@
         <v>147</v>
       </c>
       <c r="DD33" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
-    <row r="34" spans="1:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:108" ht="20" customHeight="1">
       <c r="A34" s="50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
@@ -8423,10 +8455,10 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
       <c r="M34" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="N34" s="20" t="s">
         <v>223</v>
-      </c>
-      <c r="N34" s="20" t="s">
-        <v>224</v>
       </c>
       <c r="O34" s="21"/>
       <c r="P34" s="19">
@@ -8568,13 +8600,13 @@
         <v>143</v>
       </c>
       <c r="CX34" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="CY34" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="CY34" s="20" t="s">
-        <v>226</v>
-      </c>
       <c r="CZ34" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="DA34" s="20" t="s">
         <v>146</v>
@@ -8583,10 +8615,10 @@
         <v>143</v>
       </c>
       <c r="DC34" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="DD34" s="20" t="s">
         <v>232</v>
-      </c>
-      <c r="DD34" s="20" t="s">
-        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -8595,5 +8627,10 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ineligible if person has a PC290
- add tests explicitly for both convictions and registrations

[#164636782]
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="31960" windowHeight="15820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="240">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -736,6 +736,9 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>PC 290</t>
   </si>
 </sst>
 </file>
@@ -2341,8 +2344,8 @@
   </sheetPr>
   <dimension ref="A1:JA34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CY24" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="DC29" sqref="DC29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CZ14" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="DH21" sqref="DH21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -6226,10 +6229,10 @@
         <v>143</v>
       </c>
       <c r="DG20" s="25" t="s">
-        <v>147</v>
+        <v>192</v>
       </c>
       <c r="DH20" s="25" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:112" ht="20" customHeight="1">

</xml_diff>

<commit_message>
Change from "Maybe eligible" to "Hand review" for other 11357
[#168061144]
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen_pilots/test_fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022551CA-E7E8-0540-89B2-A435A506DA36}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="31960" windowHeight="15820"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="31960" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="239">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -493,9 +499,6 @@
   </si>
   <si>
     <t>38.0</t>
-  </si>
-  <si>
-    <t>Maybe Eligible - Flag for Review</t>
   </si>
   <si>
     <t>Other 11357</t>
@@ -744,7 +747,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000000000000"/>
   </numFmts>
@@ -2338,17 +2341,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:JA34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CZ14" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="DH21" sqref="DH21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CF14" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="DH10" sqref="DH10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="49"/>
     <col min="2" max="2" width="11.33203125" style="1" hidden="1" customWidth="1"/>
@@ -2451,7 +2454,7 @@
     <col min="113" max="261" width="8.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" s="47" customFormat="1" ht="27.75" customHeight="1">
+    <row r="1" spans="1:112" s="47" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="48"/>
       <c r="B1" s="44"/>
       <c r="C1" s="45"/>
@@ -2465,16 +2468,16 @@
       <c r="K1" s="46"/>
       <c r="L1" s="46"/>
       <c r="M1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q1" s="46"/>
       <c r="R1" s="46"/>
@@ -2484,7 +2487,7 @@
       <c r="V1" s="46"/>
       <c r="W1" s="46"/>
       <c r="X1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Y1" s="46"/>
       <c r="Z1" s="46"/>
@@ -2501,12 +2504,12 @@
       <c r="AK1" s="46"/>
       <c r="AL1" s="46"/>
       <c r="AM1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AN1" s="46"/>
       <c r="AO1" s="46"/>
       <c r="AP1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AQ1" s="46"/>
       <c r="AR1" s="46"/>
@@ -2514,23 +2517,23 @@
       <c r="AT1" s="46"/>
       <c r="AU1" s="46"/>
       <c r="AV1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AW1" s="46"/>
       <c r="AX1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AY1" s="46"/>
       <c r="AZ1" s="46"/>
       <c r="BA1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="BB1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="BC1" s="46"/>
       <c r="BD1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="BE1" s="46"/>
       <c r="BF1" s="46"/>
@@ -2558,88 +2561,88 @@
       <c r="CB1" s="46"/>
       <c r="CC1" s="46"/>
       <c r="CD1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CE1" s="46"/>
       <c r="CF1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CG1" s="46"/>
       <c r="CH1" s="46"/>
       <c r="CI1" s="46"/>
       <c r="CJ1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CK1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CL1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CM1" s="46"/>
       <c r="CN1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CO1" s="46"/>
       <c r="CP1" s="46"/>
       <c r="CQ1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CR1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CS1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CT1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CU1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CV1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CW1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CX1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CY1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="CZ1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="DA1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="DB1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="DC1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="DD1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="DE1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="DF1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="DG1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="DH1" s="46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:112" ht="20.25" customHeight="1">
+    <row r="2" spans="1:112" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2954,16 +2957,16 @@
         <v>103</v>
       </c>
       <c r="DB2" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="DC2" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="DC2" s="2" t="s">
+      <c r="DD2" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="DD2" s="2" t="s">
+      <c r="DE2" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="DE2" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="DF2" s="2" t="s">
         <v>104</v>
@@ -2975,7 +2978,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:112" ht="20.25" customHeight="1">
+    <row r="3" spans="1:112" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="50"/>
       <c r="B3" s="3"/>
       <c r="C3" s="51"/>
@@ -3139,7 +3142,7 @@
       <c r="DG3" s="6"/>
       <c r="DH3" s="6"/>
     </row>
-    <row r="4" spans="1:112" ht="20" customHeight="1">
+    <row r="4" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="50"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -3313,7 +3316,7 @@
       <c r="DG4" s="11"/>
       <c r="DH4" s="11"/>
     </row>
-    <row r="5" spans="1:112" ht="20" customHeight="1">
+    <row r="5" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="50"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -3477,7 +3480,7 @@
       <c r="DG5" s="11"/>
       <c r="DH5" s="11"/>
     </row>
-    <row r="6" spans="1:112" ht="20" customHeight="1">
+    <row r="6" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="50"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -3641,7 +3644,7 @@
       <c r="DG6" s="11"/>
       <c r="DH6" s="11"/>
     </row>
-    <row r="7" spans="1:112" ht="20" customHeight="1">
+    <row r="7" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="50"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -3805,9 +3808,9 @@
       <c r="DG7" s="11"/>
       <c r="DH7" s="11"/>
     </row>
-    <row r="8" spans="1:112" ht="20" customHeight="1">
+    <row r="8" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -3992,16 +3995,16 @@
         <v>146</v>
       </c>
       <c r="DB8" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DC8" s="10" t="s">
         <v>146</v>
       </c>
       <c r="DD8" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DE8" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF8" s="10" t="s">
         <v>104</v>
@@ -4010,10 +4013,10 @@
         <v>147</v>
       </c>
       <c r="DH8" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:112" ht="20" customHeight="1">
+    <row r="9" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="50"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
@@ -4177,9 +4180,9 @@
       <c r="DG9" s="16"/>
       <c r="DH9" s="16"/>
     </row>
-    <row r="10" spans="1:112" ht="20" customHeight="1">
+    <row r="10" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
@@ -4367,25 +4370,25 @@
         <v>142</v>
       </c>
       <c r="DC10" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DD10" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DE10" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF10" s="15" t="s">
         <v>143</v>
       </c>
       <c r="DG10" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="DH10" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="DH10" s="15" t="s">
-        <v>159</v>
-      </c>
     </row>
-    <row r="11" spans="1:112" ht="20" customHeight="1">
+    <row r="11" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="50"/>
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
@@ -4450,7 +4453,7 @@
       </c>
       <c r="AQ11" s="16"/>
       <c r="AR11" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AS11" s="16"/>
       <c r="AT11" s="16"/>
@@ -4474,11 +4477,11 @@
         <v>112</v>
       </c>
       <c r="BD11" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BE11" s="16"/>
       <c r="BF11" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BG11" s="16"/>
       <c r="BH11" s="16"/>
@@ -4517,7 +4520,7 @@
       <c r="CK11" s="16"/>
       <c r="CL11" s="16"/>
       <c r="CM11" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="CN11" s="14">
         <v>23</v>
@@ -4545,9 +4548,9 @@
       <c r="DG11" s="16"/>
       <c r="DH11" s="16"/>
     </row>
-    <row r="12" spans="1:112" ht="20" customHeight="1">
+    <row r="12" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
@@ -4636,7 +4639,7 @@
         <v>112</v>
       </c>
       <c r="BD12" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BE12" s="15" t="s">
         <v>114</v>
@@ -4720,10 +4723,10 @@
         <v>154</v>
       </c>
       <c r="CX12" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="CY12" s="15" t="s">
         <v>165</v>
-      </c>
-      <c r="CY12" s="15" t="s">
-        <v>166</v>
       </c>
       <c r="CZ12" s="15" t="s">
         <v>157</v>
@@ -4735,13 +4738,13 @@
         <v>142</v>
       </c>
       <c r="DC12" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DD12" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DE12" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF12" s="15" t="s">
         <v>143</v>
@@ -4750,10 +4753,10 @@
         <v>147</v>
       </c>
       <c r="DH12" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:112" ht="20" customHeight="1">
+    <row r="13" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="50"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
@@ -4890,10 +4893,10 @@
         <v>10</v>
       </c>
       <c r="CL13" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="CM13" s="15" t="s">
         <v>168</v>
-      </c>
-      <c r="CM13" s="15" t="s">
-        <v>169</v>
       </c>
       <c r="CN13" s="14">
         <v>23</v>
@@ -4921,9 +4924,9 @@
       <c r="DG13" s="16"/>
       <c r="DH13" s="16"/>
     </row>
-    <row r="14" spans="1:112" ht="20" customHeight="1">
+    <row r="14" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -4946,7 +4949,7 @@
         <v>1008675309</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O14" s="21"/>
       <c r="P14" s="19">
@@ -5012,7 +5015,7 @@
         <v>112</v>
       </c>
       <c r="BD14" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="BE14" s="20" t="s">
         <v>114</v>
@@ -5083,10 +5086,10 @@
         <v>107</v>
       </c>
       <c r="CS14" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="CT14" s="20" t="s">
         <v>172</v>
-      </c>
-      <c r="CT14" s="20" t="s">
-        <v>173</v>
       </c>
       <c r="CU14" s="20" t="s">
         <v>143</v>
@@ -5107,10 +5110,10 @@
         <v>145</v>
       </c>
       <c r="DA14" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="DB14" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DC14" s="20" t="s">
         <v>153</v>
@@ -5119,7 +5122,7 @@
         <v>146</v>
       </c>
       <c r="DE14" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF14" s="20" t="s">
         <v>143</v>
@@ -5128,10 +5131,10 @@
         <v>147</v>
       </c>
       <c r="DH14" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
-    <row r="15" spans="1:112" ht="20" customHeight="1">
+    <row r="15" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="50"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -5154,7 +5157,7 @@
         <v>1008675309</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O15" s="21"/>
       <c r="P15" s="19">
@@ -5204,7 +5207,7 @@
       <c r="AV15" s="21"/>
       <c r="AW15" s="21"/>
       <c r="AX15" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AY15" s="21"/>
       <c r="AZ15" s="40">
@@ -5305,7 +5308,7 @@
       <c r="DG15" s="21"/>
       <c r="DH15" s="21"/>
     </row>
-    <row r="16" spans="1:112" ht="20" customHeight="1">
+    <row r="16" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="50"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -5328,7 +5331,7 @@
         <v>1008675309</v>
       </c>
       <c r="N16" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O16" s="21"/>
       <c r="P16" s="19">
@@ -5378,7 +5381,7 @@
       <c r="AV16" s="21"/>
       <c r="AW16" s="21"/>
       <c r="AX16" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AY16" s="21"/>
       <c r="AZ16" s="40">
@@ -5479,9 +5482,9 @@
       <c r="DG16" s="21"/>
       <c r="DH16" s="21"/>
     </row>
-    <row r="17" spans="1:112" ht="20" customHeight="1">
+    <row r="17" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -5504,7 +5507,7 @@
         <v>1008675309</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O17" s="21"/>
       <c r="P17" s="19">
@@ -5570,13 +5573,13 @@
         <v>112</v>
       </c>
       <c r="BD17" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BE17" s="20" t="s">
         <v>114</v>
       </c>
       <c r="BF17" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="BG17" s="21"/>
       <c r="BH17" s="21"/>
@@ -5639,10 +5642,10 @@
         <v>107</v>
       </c>
       <c r="CS17" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="CT17" s="20" t="s">
         <v>172</v>
-      </c>
-      <c r="CT17" s="20" t="s">
-        <v>173</v>
       </c>
       <c r="CU17" s="20" t="s">
         <v>143</v>
@@ -5654,19 +5657,19 @@
         <v>143</v>
       </c>
       <c r="CX17" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="CY17" s="20" t="s">
         <v>177</v>
-      </c>
-      <c r="CY17" s="20" t="s">
-        <v>178</v>
       </c>
       <c r="CZ17" s="20" t="s">
         <v>145</v>
       </c>
       <c r="DA17" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="DB17" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DC17" s="20" t="s">
         <v>153</v>
@@ -5675,7 +5678,7 @@
         <v>146</v>
       </c>
       <c r="DE17" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF17" s="20" t="s">
         <v>143</v>
@@ -5684,10 +5687,10 @@
         <v>147</v>
       </c>
       <c r="DH17" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
-    <row r="18" spans="1:112" ht="20" customHeight="1">
+    <row r="18" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="50"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
@@ -5710,7 +5713,7 @@
         <v>1008675309</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O18" s="21"/>
       <c r="P18" s="19">
@@ -5776,7 +5779,7 @@
         <v>112</v>
       </c>
       <c r="BD18" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BE18" s="20" t="s">
         <v>114</v>
@@ -5822,7 +5825,7 @@
         <v>138</v>
       </c>
       <c r="CJ18" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="CK18" s="19">
         <v>6</v>
@@ -5831,7 +5834,7 @@
         <v>128</v>
       </c>
       <c r="CM18" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CN18" s="19">
         <v>25</v>
@@ -5859,7 +5862,7 @@
       <c r="DG18" s="21"/>
       <c r="DH18" s="21"/>
     </row>
-    <row r="19" spans="1:112" ht="20" customHeight="1">
+    <row r="19" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="50"/>
       <c r="B19" s="22"/>
       <c r="C19" s="23"/>
@@ -5879,10 +5882,10 @@
       <c r="K19" s="26"/>
       <c r="L19" s="26"/>
       <c r="M19" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="N19" s="25" t="s">
         <v>182</v>
-      </c>
-      <c r="N19" s="25" t="s">
-        <v>183</v>
       </c>
       <c r="O19" s="26"/>
       <c r="P19" s="24">
@@ -5948,7 +5951,7 @@
         <v>112</v>
       </c>
       <c r="BD19" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="BE19" s="25" t="s">
         <v>114</v>
@@ -6033,9 +6036,9 @@
       <c r="DG19" s="26"/>
       <c r="DH19" s="26"/>
     </row>
-    <row r="20" spans="1:112" ht="20" customHeight="1">
+    <row r="20" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
@@ -6055,10 +6058,10 @@
       <c r="K20" s="26"/>
       <c r="L20" s="26"/>
       <c r="M20" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O20" s="26"/>
       <c r="P20" s="24">
@@ -6187,16 +6190,16 @@
         <v>107</v>
       </c>
       <c r="CS20" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="CT20" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="CU20" s="25" t="s">
         <v>143</v>
       </c>
       <c r="CV20" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="CW20" s="25" t="s">
         <v>143</v>
@@ -6208,34 +6211,34 @@
         <v>145</v>
       </c>
       <c r="CZ20" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="DA20" s="25" t="s">
         <v>142</v>
       </c>
       <c r="DB20" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DC20" s="25" t="s">
         <v>142</v>
       </c>
       <c r="DD20" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DE20" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF20" s="25" t="s">
         <v>143</v>
       </c>
       <c r="DG20" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="DH20" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
-    <row r="21" spans="1:112" ht="20" customHeight="1">
+    <row r="21" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="50"/>
       <c r="B21" s="22"/>
       <c r="C21" s="23"/>
@@ -6255,10 +6258,10 @@
       <c r="K21" s="26"/>
       <c r="L21" s="26"/>
       <c r="M21" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="N21" s="25" t="s">
         <v>182</v>
-      </c>
-      <c r="N21" s="25" t="s">
-        <v>183</v>
       </c>
       <c r="O21" s="26"/>
       <c r="P21" s="24">
@@ -6324,7 +6327,7 @@
         <v>112</v>
       </c>
       <c r="BD21" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BE21" s="25" t="s">
         <v>114</v>
@@ -6356,10 +6359,10 @@
       <c r="CB21" s="26"/>
       <c r="CC21" s="26"/>
       <c r="CD21" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="CE21" s="25" t="s">
         <v>189</v>
-      </c>
-      <c r="CE21" s="25" t="s">
-        <v>190</v>
       </c>
       <c r="CF21" s="25" t="s">
         <v>117</v>
@@ -6372,7 +6375,7 @@
         <v>138</v>
       </c>
       <c r="CJ21" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="CK21" s="24">
         <v>6</v>
@@ -6381,7 +6384,7 @@
         <v>128</v>
       </c>
       <c r="CM21" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CN21" s="24">
         <v>25</v>
@@ -6409,9 +6412,9 @@
       <c r="DG21" s="26"/>
       <c r="DH21" s="26"/>
     </row>
-    <row r="22" spans="1:112" ht="20" customHeight="1">
+    <row r="22" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
@@ -6431,10 +6434,10 @@
       <c r="K22" s="26"/>
       <c r="L22" s="26"/>
       <c r="M22" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="N22" s="25" t="s">
         <v>182</v>
-      </c>
-      <c r="N22" s="25" t="s">
-        <v>183</v>
       </c>
       <c r="O22" s="26"/>
       <c r="P22" s="24">
@@ -6535,7 +6538,7 @@
         <v>136</v>
       </c>
       <c r="CE22" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="CF22" s="25" t="s">
         <v>131</v>
@@ -6557,7 +6560,7 @@
         <v>128</v>
       </c>
       <c r="CM22" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CN22" s="24">
         <v>61</v>
@@ -6569,57 +6572,57 @@
         <v>107</v>
       </c>
       <c r="CS22" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="CT22" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="CU22" s="25" t="s">
         <v>143</v>
       </c>
       <c r="CV22" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="CW22" s="25" t="s">
         <v>143</v>
       </c>
       <c r="CX22" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="CY22" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="CZ22" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="DA22" s="25" t="s">
         <v>142</v>
       </c>
       <c r="DB22" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DC22" s="25" t="s">
         <v>142</v>
       </c>
       <c r="DD22" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DE22" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF22" s="25" t="s">
         <v>143</v>
       </c>
       <c r="DG22" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="DH22" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="DH22" s="25" t="s">
-        <v>193</v>
-      </c>
     </row>
-    <row r="23" spans="1:112" ht="20" customHeight="1">
+    <row r="23" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -6630,7 +6633,7 @@
         <v>107</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
@@ -6639,10 +6642,10 @@
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
       <c r="M23" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="N23" s="30" t="s">
         <v>194</v>
-      </c>
-      <c r="N23" s="30" t="s">
-        <v>195</v>
       </c>
       <c r="O23" s="31"/>
       <c r="P23" s="29">
@@ -6740,10 +6743,10 @@
       <c r="CB23" s="31"/>
       <c r="CC23" s="31"/>
       <c r="CD23" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="CE23" s="30" t="s">
         <v>189</v>
-      </c>
-      <c r="CE23" s="30" t="s">
-        <v>190</v>
       </c>
       <c r="CF23" s="30" t="s">
         <v>117</v>
@@ -6756,7 +6759,7 @@
         <v>138</v>
       </c>
       <c r="CJ23" s="30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="CK23" s="29">
         <v>6</v>
@@ -6776,10 +6779,10 @@
         <v>757392</v>
       </c>
       <c r="CT23" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="CU23" s="30" t="s">
         <v>196</v>
-      </c>
-      <c r="CU23" s="30" t="s">
-        <v>197</v>
       </c>
       <c r="CV23" s="30" t="s">
         <v>143</v>
@@ -6788,13 +6791,13 @@
         <v>143</v>
       </c>
       <c r="CX23" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="CY23" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="CY23" s="30" t="s">
+      <c r="CZ23" s="30" t="s">
         <v>199</v>
-      </c>
-      <c r="CZ23" s="30" t="s">
-        <v>200</v>
       </c>
       <c r="DA23" s="30" t="s">
         <v>153</v>
@@ -6809,19 +6812,19 @@
         <v>146</v>
       </c>
       <c r="DE23" s="30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF23" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DG23" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="DH23" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:112" ht="20" customHeight="1">
+    <row r="24" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="50"/>
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
@@ -6832,7 +6835,7 @@
         <v>107</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -6841,10 +6844,10 @@
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
       <c r="M24" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="N24" s="30" t="s">
         <v>194</v>
-      </c>
-      <c r="N24" s="30" t="s">
-        <v>195</v>
       </c>
       <c r="O24" s="31"/>
       <c r="P24" s="29">
@@ -6910,7 +6913,7 @@
         <v>112</v>
       </c>
       <c r="BD24" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BE24" s="30" t="s">
         <v>114</v>
@@ -6942,10 +6945,10 @@
       <c r="CB24" s="31"/>
       <c r="CC24" s="31"/>
       <c r="CD24" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="CE24" s="30" t="s">
         <v>189</v>
-      </c>
-      <c r="CE24" s="30" t="s">
-        <v>190</v>
       </c>
       <c r="CF24" s="30" t="s">
         <v>117</v>
@@ -6958,7 +6961,7 @@
         <v>138</v>
       </c>
       <c r="CJ24" s="30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="CK24" s="29">
         <v>6</v>
@@ -6991,7 +6994,7 @@
       <c r="DG24" s="31"/>
       <c r="DH24" s="31"/>
     </row>
-    <row r="25" spans="1:112" ht="20" customHeight="1">
+    <row r="25" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="50"/>
       <c r="B25" s="27"/>
       <c r="C25" s="28"/>
@@ -7002,7 +7005,7 @@
         <v>107</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
@@ -7011,10 +7014,10 @@
       <c r="K25" s="31"/>
       <c r="L25" s="31"/>
       <c r="M25" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="N25" s="30" t="s">
         <v>194</v>
-      </c>
-      <c r="N25" s="30" t="s">
-        <v>195</v>
       </c>
       <c r="O25" s="31"/>
       <c r="P25" s="29">
@@ -7155,9 +7158,9 @@
       <c r="DG25" s="31"/>
       <c r="DH25" s="31"/>
     </row>
-    <row r="26" spans="1:112" ht="20" customHeight="1">
+    <row r="26" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
@@ -7168,7 +7171,7 @@
         <v>107</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
@@ -7177,10 +7180,10 @@
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
       <c r="M26" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="N26" s="30" t="s">
         <v>194</v>
-      </c>
-      <c r="N26" s="30" t="s">
-        <v>195</v>
       </c>
       <c r="O26" s="31"/>
       <c r="P26" s="29">
@@ -7310,10 +7313,10 @@
         <v>757392</v>
       </c>
       <c r="CT26" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="CU26" s="30" t="s">
         <v>196</v>
-      </c>
-      <c r="CU26" s="30" t="s">
-        <v>197</v>
       </c>
       <c r="CV26" s="30" t="s">
         <v>143</v>
@@ -7322,13 +7325,13 @@
         <v>143</v>
       </c>
       <c r="CX26" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="CY26" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="CY26" s="30" t="s">
-        <v>204</v>
-      </c>
       <c r="CZ26" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="DA26" s="30" t="s">
         <v>153</v>
@@ -7343,21 +7346,21 @@
         <v>146</v>
       </c>
       <c r="DE26" s="30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF26" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DG26" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="DH26" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="DH26" s="30" t="s">
-        <v>159</v>
-      </c>
     </row>
-    <row r="27" spans="1:112" ht="20" customHeight="1">
+    <row r="27" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
@@ -7368,7 +7371,7 @@
         <v>107</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
@@ -7377,10 +7380,10 @@
       <c r="K27" s="31"/>
       <c r="L27" s="31"/>
       <c r="M27" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="N27" s="30" t="s">
         <v>194</v>
-      </c>
-      <c r="N27" s="30" t="s">
-        <v>195</v>
       </c>
       <c r="O27" s="31"/>
       <c r="P27" s="29">
@@ -7444,7 +7447,7 @@
         <v>112</v>
       </c>
       <c r="BD27" s="30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="BE27" s="30" t="s">
         <v>114</v>
@@ -7510,10 +7513,10 @@
         <v>757392</v>
       </c>
       <c r="CT27" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="CU27" s="30" t="s">
         <v>196</v>
-      </c>
-      <c r="CU27" s="30" t="s">
-        <v>197</v>
       </c>
       <c r="CV27" s="30" t="s">
         <v>143</v>
@@ -7522,13 +7525,13 @@
         <v>143</v>
       </c>
       <c r="CX27" s="30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="CY27" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="CZ27" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="DA27" s="30" t="s">
         <v>153</v>
@@ -7543,21 +7546,21 @@
         <v>146</v>
       </c>
       <c r="DE27" s="30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF27" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DG27" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="DH27" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:112" ht="20" customHeight="1">
+    <row r="28" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
@@ -7580,7 +7583,7 @@
         <v>1008675309</v>
       </c>
       <c r="N28" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O28" s="36"/>
       <c r="P28" s="34">
@@ -7646,13 +7649,13 @@
         <v>112</v>
       </c>
       <c r="BD28" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="BE28" s="35" t="s">
         <v>114</v>
       </c>
       <c r="BF28" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="BG28" s="36"/>
       <c r="BH28" s="36"/>
@@ -7694,7 +7697,7 @@
         <v>138</v>
       </c>
       <c r="CJ28" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="CK28" s="34">
         <v>6</v>
@@ -7703,7 +7706,7 @@
         <v>128</v>
       </c>
       <c r="CM28" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CN28" s="34">
         <v>25</v>
@@ -7715,7 +7718,7 @@
         <v>107</v>
       </c>
       <c r="CS28" s="35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="CT28" s="35" t="s">
         <v>153</v>
@@ -7730,28 +7733,28 @@
         <v>143</v>
       </c>
       <c r="CX28" s="35" t="s">
+        <v>210</v>
+      </c>
+      <c r="CY28" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="CY28" s="35" t="s">
+      <c r="CZ28" s="35" t="s">
         <v>212</v>
-      </c>
-      <c r="CZ28" s="35" t="s">
-        <v>213</v>
       </c>
       <c r="DA28" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DB28" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DC28" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DD28" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DE28" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF28" s="35" t="s">
         <v>143</v>
@@ -7760,10 +7763,10 @@
         <v>147</v>
       </c>
       <c r="DH28" s="35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
-    <row r="29" spans="1:112" ht="20" customHeight="1">
+    <row r="29" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="50"/>
       <c r="B29" s="32"/>
       <c r="C29" s="33"/>
@@ -7786,7 +7789,7 @@
         <v>1008675309</v>
       </c>
       <c r="N29" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O29" s="36"/>
       <c r="P29" s="34">
@@ -7836,7 +7839,7 @@
       <c r="AV29" s="36"/>
       <c r="AW29" s="36"/>
       <c r="AX29" s="35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AY29" s="36"/>
       <c r="AZ29" s="43">
@@ -7852,13 +7855,13 @@
         <v>112</v>
       </c>
       <c r="BD29" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="BE29" s="35" t="s">
         <v>114</v>
       </c>
       <c r="BF29" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="BG29" s="36"/>
       <c r="BH29" s="36"/>
@@ -7900,7 +7903,7 @@
         <v>138</v>
       </c>
       <c r="CJ29" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="CK29" s="34">
         <v>6</v>
@@ -7909,7 +7912,7 @@
         <v>128</v>
       </c>
       <c r="CM29" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CN29" s="34">
         <v>25</v>
@@ -7937,9 +7940,9 @@
       <c r="DG29" s="36"/>
       <c r="DH29" s="36"/>
     </row>
-    <row r="30" spans="1:112" ht="20" customHeight="1">
+    <row r="30" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="33"/>
@@ -7962,7 +7965,7 @@
         <v>1008675309</v>
       </c>
       <c r="N30" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O30" s="36"/>
       <c r="P30" s="34">
@@ -8028,13 +8031,13 @@
         <v>112</v>
       </c>
       <c r="BD30" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="BE30" s="35" t="s">
         <v>128</v>
       </c>
       <c r="BF30" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="BG30" s="36"/>
       <c r="BH30" s="36"/>
@@ -8076,7 +8079,7 @@
         <v>138</v>
       </c>
       <c r="CJ30" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="CK30" s="34">
         <v>6</v>
@@ -8085,7 +8088,7 @@
         <v>128</v>
       </c>
       <c r="CM30" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CN30" s="34">
         <v>25</v>
@@ -8097,7 +8100,7 @@
         <v>107</v>
       </c>
       <c r="CS30" s="35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="CT30" s="35" t="s">
         <v>153</v>
@@ -8112,42 +8115,42 @@
         <v>143</v>
       </c>
       <c r="CX30" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="CY30" s="35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="CZ30" s="35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="DA30" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DB30" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DC30" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DD30" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DE30" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF30" s="35" t="s">
         <v>143</v>
       </c>
       <c r="DG30" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="DH30" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:112" ht="20" customHeight="1">
+    <row r="31" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -8167,10 +8170,10 @@
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
       <c r="M31" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="9">
@@ -8305,7 +8308,7 @@
         <v>107</v>
       </c>
       <c r="CS31" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="CT31" s="10" t="s">
         <v>142</v>
@@ -8320,28 +8323,28 @@
         <v>143</v>
       </c>
       <c r="CX31" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="CY31" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="CY31" s="10" t="s">
-        <v>212</v>
-      </c>
       <c r="CZ31" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="DA31" s="10" t="s">
         <v>146</v>
       </c>
       <c r="DB31" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DC31" s="10" t="s">
         <v>146</v>
       </c>
       <c r="DD31" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DE31" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF31" s="10" t="s">
         <v>143</v>
@@ -8350,10 +8353,10 @@
         <v>147</v>
       </c>
       <c r="DH31" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:112" ht="20" customHeight="1">
+    <row r="32" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="50"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
@@ -8373,10 +8376,10 @@
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
       <c r="M32" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="9">
@@ -8442,13 +8445,13 @@
         <v>112</v>
       </c>
       <c r="BD32" s="52" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BE32" s="10" t="s">
         <v>114</v>
       </c>
       <c r="BF32" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="BG32" s="11"/>
       <c r="BH32" s="11"/>
@@ -8527,9 +8530,9 @@
       <c r="DG32" s="11"/>
       <c r="DH32" s="11"/>
     </row>
-    <row r="33" spans="1:112" ht="20" customHeight="1">
+    <row r="33" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
@@ -8549,10 +8552,10 @@
       <c r="K33" s="16"/>
       <c r="L33" s="16"/>
       <c r="M33" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="N33" s="15" t="s">
         <v>218</v>
-      </c>
-      <c r="N33" s="15" t="s">
-        <v>219</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="14">
@@ -8666,10 +8669,10 @@
         <v>10</v>
       </c>
       <c r="CL33" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="CM33" s="15" t="s">
         <v>168</v>
-      </c>
-      <c r="CM33" s="15" t="s">
-        <v>169</v>
       </c>
       <c r="CN33" s="14">
         <v>2</v>
@@ -8694,28 +8697,28 @@
         <v>143</v>
       </c>
       <c r="CX33" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="CY33" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="CY33" s="15" t="s">
-        <v>221</v>
-      </c>
       <c r="CZ33" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="DA33" s="15" t="s">
         <v>146</v>
       </c>
       <c r="DB33" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DC33" s="15" t="s">
         <v>146</v>
       </c>
       <c r="DD33" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DE33" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF33" s="15" t="s">
         <v>143</v>
@@ -8724,12 +8727,12 @@
         <v>147</v>
       </c>
       <c r="DH33" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
-    <row r="34" spans="1:112" ht="20" customHeight="1">
+    <row r="34" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
@@ -8749,10 +8752,10 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
       <c r="M34" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="N34" s="20" t="s">
         <v>222</v>
-      </c>
-      <c r="N34" s="20" t="s">
-        <v>223</v>
       </c>
       <c r="O34" s="21"/>
       <c r="P34" s="19">
@@ -8866,10 +8869,10 @@
         <v>5</v>
       </c>
       <c r="CL34" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="CM34" s="20" t="s">
         <v>168</v>
-      </c>
-      <c r="CM34" s="20" t="s">
-        <v>169</v>
       </c>
       <c r="CN34" s="19">
         <v>35</v>
@@ -8894,37 +8897,37 @@
         <v>143</v>
       </c>
       <c r="CX34" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="CY34" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="CY34" s="20" t="s">
-        <v>225</v>
-      </c>
       <c r="CZ34" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="DA34" s="20" t="s">
         <v>146</v>
       </c>
       <c r="DB34" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DC34" s="20" t="s">
         <v>146</v>
       </c>
       <c r="DD34" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DE34" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="DF34" s="20" t="s">
         <v>143</v>
       </c>
       <c r="DG34" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="DH34" s="20" t="s">
         <v>231</v>
-      </c>
-      <c r="DH34" s="20" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filter midemeanors and infractions - change eligibility determination and reason
[#167267647]
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen_pilots/test_fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022551CA-E7E8-0540-89B2-A435A506DA36}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD81DFB-77C4-544E-9494-07CB38EC3C70}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="31960" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-360" yWindow="2320" windowWidth="51200" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -603,9 +603,6 @@
     <t>Not eligible</t>
   </si>
   <si>
-    <t>Occurred after 11/09/2016</t>
-  </si>
-  <si>
     <t>A971951352</t>
   </si>
   <si>
@@ -705,9 +702,6 @@
     <t>true</t>
   </si>
   <si>
-    <t>Two priors</t>
-  </si>
-  <si>
     <t>50 years or older</t>
   </si>
   <si>
@@ -742,6 +736,12 @@
   </si>
   <si>
     <t>PC 290</t>
+  </si>
+  <si>
+    <t>To be reviewed by City Attorneys</t>
+  </si>
+  <si>
+    <t>Misdemeanor or Infraction</t>
   </si>
 </sst>
 </file>
@@ -2347,89 +2347,88 @@
   </sheetPr>
   <dimension ref="A1:JA34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CF14" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="DH10" sqref="DH10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CT1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="DG22" sqref="DG22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="49"/>
-    <col min="2" max="2" width="11.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="9.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="13" width="12" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.33203125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="12" style="1" customWidth="1"/>
     <col min="14" max="14" width="18.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="9.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="20" width="8" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="13.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="11.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="12.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="18.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="18" style="1" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="19" style="1" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="7.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="8.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="15.5" style="1" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5" style="1" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="10.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="10.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="10.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="16.5" style="1" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="13.5" style="1" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="11.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="10.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="13" style="1" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="11.5" style="1" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="16.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5" style="1" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="21.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="13.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="20.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="14.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="19.5" style="1" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="19.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="19.6640625" style="1" customWidth="1"/>
-    <col min="51" max="51" width="13.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="19.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.83203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" customWidth="1"/>
+    <col min="19" max="20" width="8" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.33203125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.83203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.83203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="18.33203125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="18" style="1" customWidth="1"/>
+    <col min="28" max="28" width="19" style="1" customWidth="1"/>
+    <col min="29" max="29" width="7.83203125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="8.1640625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15.5" style="1" customWidth="1"/>
+    <col min="32" max="32" width="14.5" style="1" customWidth="1"/>
+    <col min="33" max="33" width="10.6640625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="10.83203125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="10.1640625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="16.5" style="1" customWidth="1"/>
+    <col min="37" max="37" width="13.5" style="1" customWidth="1"/>
+    <col min="38" max="38" width="11.83203125" style="1" customWidth="1"/>
+    <col min="39" max="39" width="10.1640625" style="1" customWidth="1"/>
+    <col min="40" max="40" width="13" style="1" customWidth="1"/>
+    <col min="41" max="41" width="11.5" style="1" customWidth="1"/>
+    <col min="42" max="42" width="16.1640625" style="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5" style="1" customWidth="1"/>
+    <col min="44" max="44" width="21.6640625" style="1" customWidth="1"/>
+    <col min="45" max="45" width="13.6640625" style="1" customWidth="1"/>
+    <col min="46" max="46" width="20.33203125" style="1" customWidth="1"/>
+    <col min="47" max="47" width="14.1640625" style="1" customWidth="1"/>
+    <col min="48" max="48" width="19.5" style="1" customWidth="1"/>
+    <col min="49" max="50" width="19.6640625" style="1" customWidth="1"/>
+    <col min="51" max="51" width="13.33203125" style="1" customWidth="1"/>
+    <col min="52" max="52" width="19.33203125" style="1" customWidth="1"/>
     <col min="53" max="53" width="10.5" style="1" customWidth="1"/>
-    <col min="54" max="54" width="7" style="1" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="14.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="7" style="1" customWidth="1"/>
+    <col min="55" max="55" width="14.83203125" style="1" customWidth="1"/>
     <col min="56" max="56" width="37.6640625" style="1" customWidth="1"/>
     <col min="57" max="57" width="13.6640625" style="1" customWidth="1"/>
-    <col min="58" max="58" width="18.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="19.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="60" max="60" width="20.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="18.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="23.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="63" max="63" width="21.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="64" max="64" width="20.5" style="1" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="21.5" style="1" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="19.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="24.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="15.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="69" max="69" width="17.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="70" max="70" width="20" style="1" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="13" style="1" hidden="1" customWidth="1"/>
-    <col min="72" max="72" width="16.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="73" max="74" width="17.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="75" max="77" width="16.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="78" max="78" width="18" style="1" hidden="1" customWidth="1"/>
-    <col min="79" max="79" width="17.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="80" max="80" width="12.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="81" max="81" width="11" style="1" hidden="1" customWidth="1"/>
-    <col min="82" max="82" width="26.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="83" max="83" width="16.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="58" max="58" width="18.6640625" style="1" customWidth="1"/>
+    <col min="59" max="59" width="19.6640625" style="1" customWidth="1"/>
+    <col min="60" max="60" width="20.6640625" style="1" customWidth="1"/>
+    <col min="61" max="61" width="18.33203125" style="1" customWidth="1"/>
+    <col min="62" max="62" width="23.33203125" style="1" customWidth="1"/>
+    <col min="63" max="63" width="21.6640625" style="1" customWidth="1"/>
+    <col min="64" max="64" width="20.5" style="1" customWidth="1"/>
+    <col min="65" max="65" width="21.5" style="1" customWidth="1"/>
+    <col min="66" max="66" width="19.33203125" style="1" customWidth="1"/>
+    <col min="67" max="67" width="24.33203125" style="1" customWidth="1"/>
+    <col min="68" max="68" width="15.1640625" style="1" customWidth="1"/>
+    <col min="69" max="69" width="17.1640625" style="1" customWidth="1"/>
+    <col min="70" max="70" width="20" style="1" customWidth="1"/>
+    <col min="71" max="71" width="13" style="1" customWidth="1"/>
+    <col min="72" max="72" width="16.33203125" style="1" customWidth="1"/>
+    <col min="73" max="74" width="17.1640625" style="1" customWidth="1"/>
+    <col min="75" max="77" width="16.6640625" style="1" customWidth="1"/>
+    <col min="78" max="78" width="18" style="1" customWidth="1"/>
+    <col min="79" max="79" width="17.6640625" style="1" customWidth="1"/>
+    <col min="80" max="80" width="12.1640625" style="1" customWidth="1"/>
+    <col min="81" max="81" width="11" style="1" customWidth="1"/>
+    <col min="82" max="82" width="26.33203125" style="1" customWidth="1"/>
+    <col min="83" max="83" width="16.83203125" style="1" customWidth="1"/>
     <col min="84" max="84" width="17.6640625" style="1" customWidth="1"/>
     <col min="85" max="85" width="14.33203125" style="1" customWidth="1"/>
     <col min="86" max="86" width="12.6640625" style="1" customWidth="1"/>
@@ -2449,7 +2448,8 @@
     <col min="102" max="103" width="12.5" style="1" customWidth="1"/>
     <col min="104" max="104" width="10" style="1" customWidth="1"/>
     <col min="105" max="109" width="20.5" style="1" customWidth="1"/>
-    <col min="110" max="111" width="25.83203125" style="1" customWidth="1"/>
+    <col min="110" max="110" width="25.83203125" style="1" customWidth="1"/>
+    <col min="111" max="111" width="37" style="1" customWidth="1"/>
     <col min="112" max="112" width="41.5" style="1" customWidth="1"/>
     <col min="113" max="261" width="8.33203125" style="1" customWidth="1"/>
   </cols>
@@ -2468,16 +2468,16 @@
       <c r="K1" s="46"/>
       <c r="L1" s="46"/>
       <c r="M1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Q1" s="46"/>
       <c r="R1" s="46"/>
@@ -2487,7 +2487,7 @@
       <c r="V1" s="46"/>
       <c r="W1" s="46"/>
       <c r="X1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Y1" s="46"/>
       <c r="Z1" s="46"/>
@@ -2504,12 +2504,12 @@
       <c r="AK1" s="46"/>
       <c r="AL1" s="46"/>
       <c r="AM1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AN1" s="46"/>
       <c r="AO1" s="46"/>
       <c r="AP1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AQ1" s="46"/>
       <c r="AR1" s="46"/>
@@ -2517,23 +2517,23 @@
       <c r="AT1" s="46"/>
       <c r="AU1" s="46"/>
       <c r="AV1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AW1" s="46"/>
       <c r="AX1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AY1" s="46"/>
       <c r="AZ1" s="46"/>
       <c r="BA1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="BB1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="BC1" s="46"/>
       <c r="BD1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="BE1" s="46"/>
       <c r="BF1" s="46"/>
@@ -2561,88 +2561,88 @@
       <c r="CB1" s="46"/>
       <c r="CC1" s="46"/>
       <c r="CD1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CE1" s="46"/>
       <c r="CF1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CG1" s="46"/>
       <c r="CH1" s="46"/>
       <c r="CI1" s="46"/>
       <c r="CJ1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CK1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CL1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CM1" s="46"/>
       <c r="CN1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CO1" s="46"/>
       <c r="CP1" s="46"/>
       <c r="CQ1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CR1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CS1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CT1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CU1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CV1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CW1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CX1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CY1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="CZ1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="DA1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="DB1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="DC1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="DD1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="DE1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="DF1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="DG1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="DH1" s="46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:112" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2957,16 +2957,16 @@
         <v>103</v>
       </c>
       <c r="DB2" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="DC2" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="DD2" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="DC2" s="2" t="s">
+      <c r="DE2" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="DD2" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="DE2" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="DF2" s="2" t="s">
         <v>104</v>
@@ -3810,7 +3810,7 @@
     </row>
     <row r="8" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -3995,16 +3995,16 @@
         <v>146</v>
       </c>
       <c r="DB8" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DC8" s="10" t="s">
         <v>146</v>
       </c>
       <c r="DD8" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DE8" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF8" s="10" t="s">
         <v>104</v>
@@ -4013,7 +4013,7 @@
         <v>147</v>
       </c>
       <c r="DH8" s="10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -4182,7 +4182,7 @@
     </row>
     <row r="10" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
@@ -4370,19 +4370,19 @@
         <v>142</v>
       </c>
       <c r="DC10" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DD10" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DE10" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF10" s="15" t="s">
         <v>143</v>
       </c>
       <c r="DG10" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="DH10" s="15" t="s">
         <v>158</v>
@@ -4550,7 +4550,7 @@
     </row>
     <row r="12" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
@@ -4738,13 +4738,13 @@
         <v>142</v>
       </c>
       <c r="DC12" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DD12" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DE12" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF12" s="15" t="s">
         <v>143</v>
@@ -4926,7 +4926,7 @@
     </row>
     <row r="14" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -5113,7 +5113,7 @@
         <v>172</v>
       </c>
       <c r="DB14" s="20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DC14" s="20" t="s">
         <v>153</v>
@@ -5122,7 +5122,7 @@
         <v>146</v>
       </c>
       <c r="DE14" s="20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF14" s="20" t="s">
         <v>143</v>
@@ -5131,7 +5131,7 @@
         <v>147</v>
       </c>
       <c r="DH14" s="20" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -5484,7 +5484,7 @@
     </row>
     <row r="17" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -5669,7 +5669,7 @@
         <v>172</v>
       </c>
       <c r="DB17" s="20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DC17" s="20" t="s">
         <v>153</v>
@@ -5678,7 +5678,7 @@
         <v>146</v>
       </c>
       <c r="DE17" s="20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF17" s="20" t="s">
         <v>143</v>
@@ -5687,7 +5687,7 @@
         <v>147</v>
       </c>
       <c r="DH17" s="20" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -6038,7 +6038,7 @@
     </row>
     <row r="20" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
@@ -6217,16 +6217,16 @@
         <v>142</v>
       </c>
       <c r="DB20" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DC20" s="25" t="s">
         <v>142</v>
       </c>
       <c r="DD20" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DE20" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF20" s="25" t="s">
         <v>143</v>
@@ -6235,7 +6235,7 @@
         <v>191</v>
       </c>
       <c r="DH20" s="25" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -6414,7 +6414,7 @@
     </row>
     <row r="22" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
@@ -6599,30 +6599,30 @@
         <v>142</v>
       </c>
       <c r="DB22" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DC22" s="25" t="s">
         <v>142</v>
       </c>
       <c r="DD22" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DE22" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF22" s="25" t="s">
         <v>143</v>
       </c>
       <c r="DG22" s="25" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="DH22" s="25" t="s">
-        <v>192</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -6633,7 +6633,7 @@
         <v>107</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
@@ -6642,10 +6642,10 @@
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
       <c r="M23" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="N23" s="30" t="s">
         <v>193</v>
-      </c>
-      <c r="N23" s="30" t="s">
-        <v>194</v>
       </c>
       <c r="O23" s="31"/>
       <c r="P23" s="29">
@@ -6779,10 +6779,10 @@
         <v>757392</v>
       </c>
       <c r="CT23" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="CU23" s="30" t="s">
         <v>195</v>
-      </c>
-      <c r="CU23" s="30" t="s">
-        <v>196</v>
       </c>
       <c r="CV23" s="30" t="s">
         <v>143</v>
@@ -6791,13 +6791,13 @@
         <v>143</v>
       </c>
       <c r="CX23" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="CY23" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="CY23" s="30" t="s">
+      <c r="CZ23" s="30" t="s">
         <v>198</v>
-      </c>
-      <c r="CZ23" s="30" t="s">
-        <v>199</v>
       </c>
       <c r="DA23" s="30" t="s">
         <v>153</v>
@@ -6812,7 +6812,7 @@
         <v>146</v>
       </c>
       <c r="DE23" s="30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF23" s="30" t="s">
         <v>143</v>
@@ -6821,7 +6821,7 @@
         <v>191</v>
       </c>
       <c r="DH23" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -6835,7 +6835,7 @@
         <v>107</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -6844,10 +6844,10 @@
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
       <c r="M24" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="N24" s="30" t="s">
         <v>193</v>
-      </c>
-      <c r="N24" s="30" t="s">
-        <v>194</v>
       </c>
       <c r="O24" s="31"/>
       <c r="P24" s="29">
@@ -6913,7 +6913,7 @@
         <v>112</v>
       </c>
       <c r="BD24" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="BE24" s="30" t="s">
         <v>114</v>
@@ -7005,7 +7005,7 @@
         <v>107</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
@@ -7014,10 +7014,10 @@
       <c r="K25" s="31"/>
       <c r="L25" s="31"/>
       <c r="M25" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="N25" s="30" t="s">
         <v>193</v>
-      </c>
-      <c r="N25" s="30" t="s">
-        <v>194</v>
       </c>
       <c r="O25" s="31"/>
       <c r="P25" s="29">
@@ -7160,7 +7160,7 @@
     </row>
     <row r="26" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
@@ -7171,7 +7171,7 @@
         <v>107</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
@@ -7180,10 +7180,10 @@
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
       <c r="M26" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="N26" s="30" t="s">
         <v>193</v>
-      </c>
-      <c r="N26" s="30" t="s">
-        <v>194</v>
       </c>
       <c r="O26" s="31"/>
       <c r="P26" s="29">
@@ -7313,10 +7313,10 @@
         <v>757392</v>
       </c>
       <c r="CT26" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="CU26" s="30" t="s">
         <v>195</v>
-      </c>
-      <c r="CU26" s="30" t="s">
-        <v>196</v>
       </c>
       <c r="CV26" s="30" t="s">
         <v>143</v>
@@ -7325,13 +7325,13 @@
         <v>143</v>
       </c>
       <c r="CX26" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="CY26" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="CY26" s="30" t="s">
-        <v>203</v>
-      </c>
       <c r="CZ26" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="DA26" s="30" t="s">
         <v>153</v>
@@ -7346,21 +7346,21 @@
         <v>146</v>
       </c>
       <c r="DE26" s="30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF26" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DG26" s="30" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="DH26" s="30" t="s">
-        <v>158</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
@@ -7371,7 +7371,7 @@
         <v>107</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
@@ -7380,10 +7380,10 @@
       <c r="K27" s="31"/>
       <c r="L27" s="31"/>
       <c r="M27" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="N27" s="30" t="s">
         <v>193</v>
-      </c>
-      <c r="N27" s="30" t="s">
-        <v>194</v>
       </c>
       <c r="O27" s="31"/>
       <c r="P27" s="29">
@@ -7447,7 +7447,7 @@
         <v>112</v>
       </c>
       <c r="BD27" s="30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BE27" s="30" t="s">
         <v>114</v>
@@ -7513,10 +7513,10 @@
         <v>757392</v>
       </c>
       <c r="CT27" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="CU27" s="30" t="s">
         <v>195</v>
-      </c>
-      <c r="CU27" s="30" t="s">
-        <v>196</v>
       </c>
       <c r="CV27" s="30" t="s">
         <v>143</v>
@@ -7525,13 +7525,13 @@
         <v>143</v>
       </c>
       <c r="CX27" s="30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="CY27" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="CZ27" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="DA27" s="30" t="s">
         <v>153</v>
@@ -7546,7 +7546,7 @@
         <v>146</v>
       </c>
       <c r="DE27" s="30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF27" s="30" t="s">
         <v>143</v>
@@ -7555,12 +7555,12 @@
         <v>191</v>
       </c>
       <c r="DH27" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
@@ -7583,7 +7583,7 @@
         <v>1008675309</v>
       </c>
       <c r="N28" s="35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O28" s="36"/>
       <c r="P28" s="34">
@@ -7649,13 +7649,13 @@
         <v>112</v>
       </c>
       <c r="BD28" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="BE28" s="35" t="s">
         <v>114</v>
       </c>
       <c r="BF28" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="BG28" s="36"/>
       <c r="BH28" s="36"/>
@@ -7718,7 +7718,7 @@
         <v>107</v>
       </c>
       <c r="CS28" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="CT28" s="35" t="s">
         <v>153</v>
@@ -7733,28 +7733,28 @@
         <v>143</v>
       </c>
       <c r="CX28" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="CY28" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="CY28" s="35" t="s">
+      <c r="CZ28" s="35" t="s">
         <v>211</v>
-      </c>
-      <c r="CZ28" s="35" t="s">
-        <v>212</v>
       </c>
       <c r="DA28" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DB28" s="35" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DC28" s="35" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DD28" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DE28" s="35" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF28" s="35" t="s">
         <v>143</v>
@@ -7763,7 +7763,7 @@
         <v>147</v>
       </c>
       <c r="DH28" s="35" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -7789,7 +7789,7 @@
         <v>1008675309</v>
       </c>
       <c r="N29" s="35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O29" s="36"/>
       <c r="P29" s="34">
@@ -7855,13 +7855,13 @@
         <v>112</v>
       </c>
       <c r="BD29" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="BE29" s="35" t="s">
         <v>114</v>
       </c>
       <c r="BF29" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="BG29" s="36"/>
       <c r="BH29" s="36"/>
@@ -7942,7 +7942,7 @@
     </row>
     <row r="30" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="33"/>
@@ -7965,7 +7965,7 @@
         <v>1008675309</v>
       </c>
       <c r="N30" s="35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O30" s="36"/>
       <c r="P30" s="34">
@@ -8031,13 +8031,13 @@
         <v>112</v>
       </c>
       <c r="BD30" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="BE30" s="35" t="s">
         <v>128</v>
       </c>
       <c r="BF30" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="BG30" s="36"/>
       <c r="BH30" s="36"/>
@@ -8100,7 +8100,7 @@
         <v>107</v>
       </c>
       <c r="CS30" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="CT30" s="35" t="s">
         <v>153</v>
@@ -8115,42 +8115,42 @@
         <v>143</v>
       </c>
       <c r="CX30" s="35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="CY30" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="CZ30" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="DA30" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DB30" s="35" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DC30" s="35" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DD30" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DE30" s="35" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF30" s="35" t="s">
         <v>143</v>
       </c>
       <c r="DG30" s="35" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="DH30" s="35" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -8173,7 +8173,7 @@
         <v>181</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="9">
@@ -8308,7 +8308,7 @@
         <v>107</v>
       </c>
       <c r="CS31" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="CT31" s="10" t="s">
         <v>142</v>
@@ -8323,28 +8323,28 @@
         <v>143</v>
       </c>
       <c r="CX31" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="CY31" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="CY31" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="CZ31" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="DA31" s="10" t="s">
         <v>146</v>
       </c>
       <c r="DB31" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DC31" s="10" t="s">
         <v>146</v>
       </c>
       <c r="DD31" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DE31" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF31" s="10" t="s">
         <v>143</v>
@@ -8353,7 +8353,7 @@
         <v>147</v>
       </c>
       <c r="DH31" s="10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -8379,7 +8379,7 @@
         <v>181</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="9">
@@ -8445,13 +8445,13 @@
         <v>112</v>
       </c>
       <c r="BD32" s="52" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="BE32" s="10" t="s">
         <v>114</v>
       </c>
       <c r="BF32" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="BG32" s="11"/>
       <c r="BH32" s="11"/>
@@ -8532,7 +8532,7 @@
     </row>
     <row r="33" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
@@ -8552,10 +8552,10 @@
       <c r="K33" s="16"/>
       <c r="L33" s="16"/>
       <c r="M33" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="N33" s="15" t="s">
         <v>217</v>
-      </c>
-      <c r="N33" s="15" t="s">
-        <v>218</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="14">
@@ -8697,28 +8697,28 @@
         <v>143</v>
       </c>
       <c r="CX33" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="CY33" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="CY33" s="15" t="s">
-        <v>220</v>
-      </c>
       <c r="CZ33" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="DA33" s="15" t="s">
         <v>146</v>
       </c>
       <c r="DB33" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DC33" s="15" t="s">
         <v>146</v>
       </c>
       <c r="DD33" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DE33" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF33" s="15" t="s">
         <v>143</v>
@@ -8727,12 +8727,12 @@
         <v>147</v>
       </c>
       <c r="DH33" s="15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
@@ -8752,10 +8752,10 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
       <c r="M34" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="N34" s="20" t="s">
         <v>221</v>
-      </c>
-      <c r="N34" s="20" t="s">
-        <v>222</v>
       </c>
       <c r="O34" s="21"/>
       <c r="P34" s="19">
@@ -8897,37 +8897,37 @@
         <v>143</v>
       </c>
       <c r="CX34" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="CY34" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="CY34" s="20" t="s">
-        <v>224</v>
-      </c>
       <c r="CZ34" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="DA34" s="20" t="s">
         <v>146</v>
       </c>
       <c r="DB34" s="20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DC34" s="20" t="s">
         <v>146</v>
       </c>
       <c r="DD34" s="20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DE34" s="20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DF34" s="20" t="s">
         <v>143</v>
       </c>
       <c r="DG34" s="20" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="DH34" s="20" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Classify specific pairs of code sections within case as superstrike
[#166297321]
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen_pilots/test_fixtures/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD81DFB-77C4-544E-9494-07CB38EC3C70}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-360" yWindow="2320" windowWidth="51200" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="244">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -742,12 +736,27 @@
   </si>
   <si>
     <t>Misdemeanor or Infraction</t>
+  </si>
+  <si>
+    <t>LECTER, HANNIBAL</t>
+  </si>
+  <si>
+    <t>136.1 PC-SPYING ON CATS</t>
+  </si>
+  <si>
+    <t>1009123456</t>
+  </si>
+  <si>
+    <t>136.1 PC + 186.22(B)(4) PC</t>
+  </si>
+  <si>
+    <t>186.22(B)(4) PC- GANG STUFF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000000000000"/>
   </numFmts>
@@ -987,8 +996,86 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1180,13 +1267,39 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2341,17 +2454,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:JA34"/>
+  <dimension ref="A1:JA37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CT1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="DG22" sqref="DG22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AQ1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="BE48" sqref="BE48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="49"/>
     <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
@@ -2366,8 +2479,8 @@
     <col min="12" max="13" width="12" style="1" customWidth="1"/>
     <col min="14" max="14" width="18.6640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="8.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9" style="1" customWidth="1"/>
     <col min="19" max="20" width="8" style="1" customWidth="1"/>
     <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
@@ -2454,7 +2567,7 @@
     <col min="113" max="261" width="8.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" s="47" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:112" s="47" customFormat="1" ht="27.75" customHeight="1">
       <c r="A1" s="48"/>
       <c r="B1" s="44"/>
       <c r="C1" s="45"/>
@@ -2640,7 +2753,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="2" spans="1:112" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:112" ht="20.25" customHeight="1">
       <c r="A2" s="50" t="s">
         <v>224</v>
       </c>
@@ -2978,7 +3091,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:112" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:112" ht="20.25" customHeight="1">
       <c r="A3" s="50"/>
       <c r="B3" s="3"/>
       <c r="C3" s="51"/>
@@ -3142,7 +3255,7 @@
       <c r="DG3" s="6"/>
       <c r="DH3" s="6"/>
     </row>
-    <row r="4" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:112" ht="20" customHeight="1">
       <c r="A4" s="50"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -3316,7 +3429,7 @@
       <c r="DG4" s="11"/>
       <c r="DH4" s="11"/>
     </row>
-    <row r="5" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:112" ht="20" customHeight="1">
       <c r="A5" s="50"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -3480,7 +3593,7 @@
       <c r="DG5" s="11"/>
       <c r="DH5" s="11"/>
     </row>
-    <row r="6" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:112" ht="20" customHeight="1">
       <c r="A6" s="50"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -3644,7 +3757,7 @@
       <c r="DG6" s="11"/>
       <c r="DH6" s="11"/>
     </row>
-    <row r="7" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:112" ht="20" customHeight="1">
       <c r="A7" s="50"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -3808,7 +3921,7 @@
       <c r="DG7" s="11"/>
       <c r="DH7" s="11"/>
     </row>
-    <row r="8" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:112" ht="20" customHeight="1">
       <c r="A8" s="50" t="s">
         <v>224</v>
       </c>
@@ -4016,7 +4129,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:112" ht="20" customHeight="1">
       <c r="A9" s="50"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
@@ -4180,7 +4293,7 @@
       <c r="DG9" s="16"/>
       <c r="DH9" s="16"/>
     </row>
-    <row r="10" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:112" ht="20" customHeight="1">
       <c r="A10" s="50" t="s">
         <v>224</v>
       </c>
@@ -4388,7 +4501,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:112" ht="20" customHeight="1">
       <c r="A11" s="50"/>
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
@@ -4548,7 +4661,7 @@
       <c r="DG11" s="16"/>
       <c r="DH11" s="16"/>
     </row>
-    <row r="12" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:112" ht="20" customHeight="1">
       <c r="A12" s="50" t="s">
         <v>224</v>
       </c>
@@ -4756,7 +4869,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:112" ht="20" customHeight="1">
       <c r="A13" s="50"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
@@ -4924,7 +5037,7 @@
       <c r="DG13" s="16"/>
       <c r="DH13" s="16"/>
     </row>
-    <row r="14" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:112" ht="20" customHeight="1">
       <c r="A14" s="50" t="s">
         <v>224</v>
       </c>
@@ -5134,7 +5247,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:112" ht="20" customHeight="1">
       <c r="A15" s="50"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -5308,7 +5421,7 @@
       <c r="DG15" s="21"/>
       <c r="DH15" s="21"/>
     </row>
-    <row r="16" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:112" ht="20" customHeight="1">
       <c r="A16" s="50"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -5482,7 +5595,7 @@
       <c r="DG16" s="21"/>
       <c r="DH16" s="21"/>
     </row>
-    <row r="17" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:112" ht="20" customHeight="1">
       <c r="A17" s="50" t="s">
         <v>224</v>
       </c>
@@ -5690,7 +5803,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="18" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:112" ht="20" customHeight="1">
       <c r="A18" s="50"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
@@ -5862,7 +5975,7 @@
       <c r="DG18" s="21"/>
       <c r="DH18" s="21"/>
     </row>
-    <row r="19" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:112" ht="20" customHeight="1">
       <c r="A19" s="50"/>
       <c r="B19" s="22"/>
       <c r="C19" s="23"/>
@@ -6036,7 +6149,7 @@
       <c r="DG19" s="26"/>
       <c r="DH19" s="26"/>
     </row>
-    <row r="20" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:112" ht="20" customHeight="1">
       <c r="A20" s="50" t="s">
         <v>224</v>
       </c>
@@ -6238,7 +6351,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="21" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:112" ht="20" customHeight="1">
       <c r="A21" s="50"/>
       <c r="B21" s="22"/>
       <c r="C21" s="23"/>
@@ -6412,7 +6525,7 @@
       <c r="DG21" s="26"/>
       <c r="DH21" s="26"/>
     </row>
-    <row r="22" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:112" ht="20" customHeight="1">
       <c r="A22" s="50" t="s">
         <v>224</v>
       </c>
@@ -6620,7 +6733,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="23" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:112" ht="20" customHeight="1">
       <c r="A23" s="50" t="s">
         <v>224</v>
       </c>
@@ -6824,7 +6937,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:112" ht="20" customHeight="1">
       <c r="A24" s="50"/>
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
@@ -6994,7 +7107,7 @@
       <c r="DG24" s="31"/>
       <c r="DH24" s="31"/>
     </row>
-    <row r="25" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:112" ht="20" customHeight="1">
       <c r="A25" s="50"/>
       <c r="B25" s="27"/>
       <c r="C25" s="28"/>
@@ -7158,7 +7271,7 @@
       <c r="DG25" s="31"/>
       <c r="DH25" s="31"/>
     </row>
-    <row r="26" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:112" ht="20" customHeight="1">
       <c r="A26" s="50" t="s">
         <v>224</v>
       </c>
@@ -7358,7 +7471,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="27" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:112" ht="20" customHeight="1">
       <c r="A27" s="50" t="s">
         <v>224</v>
       </c>
@@ -7558,7 +7671,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:112" ht="20" customHeight="1">
       <c r="A28" s="50" t="s">
         <v>224</v>
       </c>
@@ -7766,7 +7879,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="29" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:112" ht="20" customHeight="1">
       <c r="A29" s="50"/>
       <c r="B29" s="32"/>
       <c r="C29" s="33"/>
@@ -7940,7 +8053,7 @@
       <c r="DG29" s="36"/>
       <c r="DH29" s="36"/>
     </row>
-    <row r="30" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:112" ht="20" customHeight="1">
       <c r="A30" s="50" t="s">
         <v>224</v>
       </c>
@@ -8148,7 +8261,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:112" ht="20" customHeight="1">
       <c r="A31" s="50" t="s">
         <v>224</v>
       </c>
@@ -8356,7 +8469,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:112" ht="20" customHeight="1">
       <c r="A32" s="50"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
@@ -8530,7 +8643,7 @@
       <c r="DG32" s="11"/>
       <c r="DH32" s="11"/>
     </row>
-    <row r="33" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:112" ht="20" customHeight="1">
       <c r="A33" s="50" t="s">
         <v>224</v>
       </c>
@@ -8730,7 +8843,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:112" ht="20" customHeight="1">
       <c r="A34" s="50" t="s">
         <v>224</v>
       </c>
@@ -8930,6 +9043,534 @@
         <v>229</v>
       </c>
     </row>
+    <row r="35" spans="1:112" ht="20" customHeight="1">
+      <c r="A35" s="50"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="29">
+        <v>84734893</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="N35" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="O35" s="31"/>
+      <c r="P35" s="29">
+        <v>19721127</v>
+      </c>
+      <c r="Q35" s="29">
+        <v>859349027</v>
+      </c>
+      <c r="R35" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="S35" s="31"/>
+      <c r="T35" s="31"/>
+      <c r="U35" s="31"/>
+      <c r="V35" s="31"/>
+      <c r="W35" s="31"/>
+      <c r="X35" s="31"/>
+      <c r="Y35" s="31"/>
+      <c r="Z35" s="31"/>
+      <c r="AA35" s="31"/>
+      <c r="AB35" s="31"/>
+      <c r="AC35" s="31"/>
+      <c r="AD35" s="31"/>
+      <c r="AE35" s="31"/>
+      <c r="AF35" s="31"/>
+      <c r="AG35" s="31"/>
+      <c r="AH35" s="31"/>
+      <c r="AI35" s="31"/>
+      <c r="AJ35" s="31"/>
+      <c r="AK35" s="31"/>
+      <c r="AL35" s="31"/>
+      <c r="AM35" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN35" s="31"/>
+      <c r="AO35" s="31"/>
+      <c r="AP35" s="29">
+        <v>20150214</v>
+      </c>
+      <c r="AQ35" s="31"/>
+      <c r="AR35" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS35" s="31"/>
+      <c r="AT35" s="31"/>
+      <c r="AU35" s="31"/>
+      <c r="AV35" s="31"/>
+      <c r="AW35" s="31"/>
+      <c r="AX35" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="AY35" s="31"/>
+      <c r="AZ35" s="42">
+        <v>101001022000</v>
+      </c>
+      <c r="BA35" s="29">
+        <v>20150315</v>
+      </c>
+      <c r="BB35" s="31"/>
+      <c r="BC35" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="BD35" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="BE35" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="BF35" s="31"/>
+      <c r="BG35" s="31"/>
+      <c r="BH35" s="31"/>
+      <c r="BI35" s="31"/>
+      <c r="BJ35" s="31"/>
+      <c r="BK35" s="31"/>
+      <c r="BL35" s="31"/>
+      <c r="BM35" s="31"/>
+      <c r="BN35" s="31"/>
+      <c r="BO35" s="31"/>
+      <c r="BP35" s="31"/>
+      <c r="BQ35" s="31"/>
+      <c r="BR35" s="31"/>
+      <c r="BS35" s="31"/>
+      <c r="BT35" s="31"/>
+      <c r="BU35" s="31"/>
+      <c r="BV35" s="31"/>
+      <c r="BW35" s="31"/>
+      <c r="BX35" s="31"/>
+      <c r="BY35" s="31"/>
+      <c r="BZ35" s="31"/>
+      <c r="CA35" s="31"/>
+      <c r="CB35" s="31"/>
+      <c r="CC35" s="31"/>
+      <c r="CD35" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="CE35" s="31"/>
+      <c r="CF35" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="CG35" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="CH35" s="31"/>
+      <c r="CI35" s="31"/>
+      <c r="CJ35" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="CK35" s="29">
+        <v>2</v>
+      </c>
+      <c r="CL35" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="CM35" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="CN35" s="29">
+        <v>42</v>
+      </c>
+      <c r="CO35" s="31"/>
+      <c r="CP35" s="31"/>
+      <c r="CQ35" s="31"/>
+      <c r="CR35" s="31"/>
+      <c r="CS35" s="31"/>
+      <c r="CT35" s="30"/>
+      <c r="CU35" s="30"/>
+      <c r="CV35" s="30"/>
+      <c r="CW35" s="30"/>
+      <c r="CX35" s="30"/>
+      <c r="CY35" s="30"/>
+      <c r="CZ35" s="30"/>
+      <c r="DA35" s="30"/>
+      <c r="DB35" s="30"/>
+      <c r="DC35" s="30"/>
+      <c r="DD35" s="30"/>
+      <c r="DE35" s="30"/>
+      <c r="DF35" s="31"/>
+      <c r="DG35" s="31"/>
+      <c r="DH35" s="31"/>
+    </row>
+    <row r="36" spans="1:112" ht="20" customHeight="1">
+      <c r="A36" s="50" t="s">
+        <v>224</v>
+      </c>
+      <c r="B36" s="27"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="29">
+        <v>84734893</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="N36" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="O36" s="31"/>
+      <c r="P36" s="29">
+        <v>19721127</v>
+      </c>
+      <c r="Q36" s="29">
+        <v>859349027</v>
+      </c>
+      <c r="R36" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="S36" s="31"/>
+      <c r="T36" s="31"/>
+      <c r="U36" s="31"/>
+      <c r="V36" s="31"/>
+      <c r="W36" s="31"/>
+      <c r="X36" s="31"/>
+      <c r="Y36" s="31"/>
+      <c r="Z36" s="31"/>
+      <c r="AA36" s="31"/>
+      <c r="AB36" s="31"/>
+      <c r="AC36" s="31"/>
+      <c r="AD36" s="31"/>
+      <c r="AE36" s="31"/>
+      <c r="AF36" s="31"/>
+      <c r="AG36" s="31"/>
+      <c r="AH36" s="31"/>
+      <c r="AI36" s="31"/>
+      <c r="AJ36" s="31"/>
+      <c r="AK36" s="31"/>
+      <c r="AL36" s="31"/>
+      <c r="AM36" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN36" s="31"/>
+      <c r="AO36" s="31"/>
+      <c r="AP36" s="29">
+        <v>20150519</v>
+      </c>
+      <c r="AQ36" s="31"/>
+      <c r="AR36" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS36" s="31"/>
+      <c r="AT36" s="31"/>
+      <c r="AU36" s="31"/>
+      <c r="AV36" s="31"/>
+      <c r="AW36" s="31"/>
+      <c r="AX36" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="AY36" s="31"/>
+      <c r="AZ36" s="42">
+        <v>101001023000</v>
+      </c>
+      <c r="BA36" s="29">
+        <v>20150522</v>
+      </c>
+      <c r="BB36" s="31"/>
+      <c r="BC36" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="BD36" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="BE36" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="BF36" s="31"/>
+      <c r="BG36" s="31"/>
+      <c r="BH36" s="31"/>
+      <c r="BI36" s="31"/>
+      <c r="BJ36" s="31"/>
+      <c r="BK36" s="31"/>
+      <c r="BL36" s="31"/>
+      <c r="BM36" s="31"/>
+      <c r="BN36" s="31"/>
+      <c r="BO36" s="31"/>
+      <c r="BP36" s="31"/>
+      <c r="BQ36" s="31"/>
+      <c r="BR36" s="31"/>
+      <c r="BS36" s="31"/>
+      <c r="BT36" s="31"/>
+      <c r="BU36" s="31"/>
+      <c r="BV36" s="31"/>
+      <c r="BW36" s="31"/>
+      <c r="BX36" s="31"/>
+      <c r="BY36" s="31"/>
+      <c r="BZ36" s="31"/>
+      <c r="CA36" s="31"/>
+      <c r="CB36" s="31"/>
+      <c r="CC36" s="31"/>
+      <c r="CD36" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="CE36" s="31"/>
+      <c r="CF36" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="CG36" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="CH36" s="31"/>
+      <c r="CI36" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="CJ36" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="CK36" s="29">
+        <v>2</v>
+      </c>
+      <c r="CL36" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="CM36" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="CN36" s="29">
+        <v>42</v>
+      </c>
+      <c r="CO36" s="31"/>
+      <c r="CP36" s="31"/>
+      <c r="CQ36" s="31"/>
+      <c r="CR36" s="31"/>
+      <c r="CS36" s="29"/>
+      <c r="CT36" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="CU36" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="CV36" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="CW36" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="CX36" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="CY36" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="CZ36" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="DA36" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="DB36" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="DC36" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="DD36" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="DE36" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="DF36" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="DG36" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="DH36" s="30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:112" ht="20" customHeight="1">
+      <c r="A37" s="50"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="29">
+        <v>84734893</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="N37" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="O37" s="31"/>
+      <c r="P37" s="29">
+        <v>19721127</v>
+      </c>
+      <c r="Q37" s="29">
+        <v>859349027</v>
+      </c>
+      <c r="R37" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="S37" s="31"/>
+      <c r="T37" s="31"/>
+      <c r="U37" s="31"/>
+      <c r="V37" s="31"/>
+      <c r="W37" s="31"/>
+      <c r="X37" s="31"/>
+      <c r="Y37" s="31"/>
+      <c r="Z37" s="31"/>
+      <c r="AA37" s="31"/>
+      <c r="AB37" s="31"/>
+      <c r="AC37" s="31"/>
+      <c r="AD37" s="31"/>
+      <c r="AE37" s="31"/>
+      <c r="AF37" s="31"/>
+      <c r="AG37" s="31"/>
+      <c r="AH37" s="31"/>
+      <c r="AI37" s="31"/>
+      <c r="AJ37" s="31"/>
+      <c r="AK37" s="31"/>
+      <c r="AL37" s="31"/>
+      <c r="AM37" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN37" s="31"/>
+      <c r="AO37" s="31"/>
+      <c r="AP37" s="29">
+        <v>20151031</v>
+      </c>
+      <c r="AQ37" s="31"/>
+      <c r="AR37" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="AS37" s="31"/>
+      <c r="AT37" s="31"/>
+      <c r="AU37" s="31"/>
+      <c r="AV37" s="31"/>
+      <c r="AW37" s="31"/>
+      <c r="AX37" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="AY37" s="31"/>
+      <c r="AZ37" s="42">
+        <v>101001024000</v>
+      </c>
+      <c r="BA37" s="29">
+        <v>20151031</v>
+      </c>
+      <c r="BB37" s="31"/>
+      <c r="BC37" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="BD37" s="30" t="s">
+        <v>243</v>
+      </c>
+      <c r="BE37" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="BF37" s="31"/>
+      <c r="BG37" s="31"/>
+      <c r="BH37" s="31"/>
+      <c r="BI37" s="31"/>
+      <c r="BJ37" s="31"/>
+      <c r="BK37" s="31"/>
+      <c r="BL37" s="31"/>
+      <c r="BM37" s="31"/>
+      <c r="BN37" s="31"/>
+      <c r="BO37" s="31"/>
+      <c r="BP37" s="31"/>
+      <c r="BQ37" s="31"/>
+      <c r="BR37" s="31"/>
+      <c r="BS37" s="31"/>
+      <c r="BT37" s="31"/>
+      <c r="BU37" s="31"/>
+      <c r="BV37" s="31"/>
+      <c r="BW37" s="31"/>
+      <c r="BX37" s="31"/>
+      <c r="BY37" s="31"/>
+      <c r="BZ37" s="31"/>
+      <c r="CA37" s="31"/>
+      <c r="CB37" s="31"/>
+      <c r="CC37" s="31"/>
+      <c r="CD37" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="CE37" s="31"/>
+      <c r="CF37" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="CG37" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="CH37" s="31"/>
+      <c r="CI37" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="CJ37" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="CK37" s="29">
+        <v>2</v>
+      </c>
+      <c r="CL37" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="CM37" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="CN37" s="29">
+        <v>42</v>
+      </c>
+      <c r="CO37" s="31"/>
+      <c r="CP37" s="31"/>
+      <c r="CQ37" s="31"/>
+      <c r="CR37" s="31"/>
+      <c r="CS37" s="29"/>
+      <c r="CT37" s="30"/>
+      <c r="CU37" s="30"/>
+      <c r="CV37" s="30"/>
+      <c r="CW37" s="30"/>
+      <c r="CX37" s="30"/>
+      <c r="CY37" s="30"/>
+      <c r="CZ37" s="30"/>
+      <c r="DA37" s="30"/>
+      <c r="DB37" s="30"/>
+      <c r="DC37" s="30"/>
+      <c r="DD37" s="30"/>
+      <c r="DE37" s="30"/>
+      <c r="DF37" s="30"/>
+      <c r="DG37" s="30"/>
+      <c r="DH37" s="30"/>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Flag possible Prp64 charges even when OFFENSE_DESCR has charges
Include special logic for handling 11357 sub-sections.

[#167404950]
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="250">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -753,10 +753,22 @@
     <t>186.22(B)(4) PC- GANG STUFF</t>
   </si>
   <si>
-    <t>Suspect 11358</t>
-  </si>
-  <si>
     <t>Possible Other P64 Charges</t>
+  </si>
+  <si>
+    <t>11359 - Should be flagged as 11359 != 11358</t>
+  </si>
+  <si>
+    <t>11358 - should not be flagged as charge same as OFFENSE_DESCR</t>
+  </si>
+  <si>
+    <t>11357(D) - Should not be flagged as we don't distinguish (C) from (D)</t>
+  </si>
+  <si>
+    <t>11358 - should be flagged as it's different from OFFENSE_DESCR</t>
+  </si>
+  <si>
+    <t>11357(D) - Should be flagged as we distinguish (B) from (D)</t>
   </si>
 </sst>
 </file>
@@ -1002,8 +1014,86 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1279,7 +1369,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1297,6 +1387,19 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1314,6 +1417,19 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2474,8 +2590,8 @@
   </sheetPr>
   <dimension ref="A1:JB37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CQ1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="CU26" sqref="CU26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BA1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="CU19" sqref="CU19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2533,44 +2649,45 @@
     <col min="55" max="55" width="14.83203125" style="1" customWidth="1"/>
     <col min="56" max="56" width="37.6640625" style="1" customWidth="1"/>
     <col min="57" max="57" width="13.6640625" style="1" customWidth="1"/>
-    <col min="58" max="58" width="18.6640625" style="1" customWidth="1"/>
-    <col min="59" max="59" width="19.6640625" style="1" customWidth="1"/>
-    <col min="60" max="60" width="20.6640625" style="1" customWidth="1"/>
-    <col min="61" max="61" width="18.33203125" style="1" customWidth="1"/>
-    <col min="62" max="62" width="23.33203125" style="1" customWidth="1"/>
-    <col min="63" max="63" width="21.6640625" style="1" customWidth="1"/>
-    <col min="64" max="64" width="20.5" style="1" customWidth="1"/>
-    <col min="65" max="65" width="21.5" style="1" customWidth="1"/>
-    <col min="66" max="66" width="19.33203125" style="1" customWidth="1"/>
-    <col min="67" max="67" width="24.33203125" style="1" customWidth="1"/>
-    <col min="68" max="68" width="15.1640625" style="1" customWidth="1"/>
-    <col min="69" max="69" width="17.1640625" style="1" customWidth="1"/>
-    <col min="70" max="70" width="20" style="1" customWidth="1"/>
-    <col min="71" max="71" width="13" style="1" customWidth="1"/>
-    <col min="72" max="72" width="16.33203125" style="1" customWidth="1"/>
-    <col min="73" max="74" width="17.1640625" style="1" customWidth="1"/>
-    <col min="75" max="77" width="16.6640625" style="1" customWidth="1"/>
-    <col min="78" max="78" width="18" style="1" customWidth="1"/>
-    <col min="79" max="79" width="17.6640625" style="1" customWidth="1"/>
-    <col min="80" max="80" width="12.1640625" style="1" customWidth="1"/>
-    <col min="81" max="81" width="11" style="1" customWidth="1"/>
-    <col min="82" max="82" width="26.33203125" style="1" customWidth="1"/>
-    <col min="83" max="83" width="16.83203125" style="1" customWidth="1"/>
-    <col min="84" max="84" width="17.6640625" style="1" customWidth="1"/>
-    <col min="85" max="85" width="14.33203125" style="1" customWidth="1"/>
-    <col min="86" max="86" width="12.6640625" style="1" customWidth="1"/>
-    <col min="87" max="87" width="16" style="1" customWidth="1"/>
-    <col min="88" max="88" width="16.83203125" style="1" customWidth="1"/>
-    <col min="89" max="89" width="13.5" style="1" customWidth="1"/>
-    <col min="90" max="90" width="16.5" style="1" customWidth="1"/>
-    <col min="91" max="91" width="109.5" style="1" customWidth="1"/>
-    <col min="92" max="92" width="9.33203125" style="1" customWidth="1"/>
+    <col min="58" max="58" width="18.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="19.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="60" max="60" width="20.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="18.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="23.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="63" max="63" width="21.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="64" max="64" width="20.5" style="1" hidden="1" customWidth="1"/>
+    <col min="65" max="65" width="21.5" style="1" hidden="1" customWidth="1"/>
+    <col min="66" max="66" width="19.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="24.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="15.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="69" max="69" width="17.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="20" style="1" hidden="1" customWidth="1"/>
+    <col min="71" max="71" width="13" style="1" hidden="1" customWidth="1"/>
+    <col min="72" max="72" width="16.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="73" max="74" width="17.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="75" max="77" width="16.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="78" max="78" width="18" style="1" hidden="1" customWidth="1"/>
+    <col min="79" max="79" width="17.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="80" max="80" width="12.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="81" max="81" width="11" style="1" hidden="1" customWidth="1"/>
+    <col min="82" max="82" width="26.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="83" max="83" width="16.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="84" max="84" width="17.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="85" max="85" width="14.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="86" max="86" width="12.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="87" max="87" width="16" style="1" hidden="1" customWidth="1"/>
+    <col min="88" max="88" width="16.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="89" max="89" width="13.5" style="1" hidden="1" customWidth="1"/>
+    <col min="90" max="90" width="16.5" style="1" hidden="1" customWidth="1"/>
+    <col min="91" max="91" width="17.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="92" max="92" width="9.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="93" max="93" width="8.83203125" style="1" customWidth="1"/>
     <col min="94" max="94" width="15.33203125" style="1" customWidth="1"/>
-    <col min="95" max="95" width="26.83203125" style="1" customWidth="1"/>
+    <col min="95" max="95" width="59.5" style="1" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="12.5" style="1" customWidth="1"/>
     <col min="97" max="97" width="29.6640625" style="1" customWidth="1"/>
-    <col min="98" max="99" width="24" style="1" customWidth="1"/>
+    <col min="98" max="98" width="24" style="1" customWidth="1"/>
+    <col min="99" max="99" width="56.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="100" max="102" width="23.6640625" style="1" customWidth="1"/>
     <col min="103" max="104" width="12.5" style="1" customWidth="1"/>
     <col min="105" max="105" width="10" style="1" customWidth="1"/>
@@ -3066,7 +3183,7 @@
         <v>96</v>
       </c>
       <c r="CU2" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="CV2" s="2" t="s">
         <v>97</v>
@@ -4101,7 +4218,9 @@
       </c>
       <c r="CO8" s="11"/>
       <c r="CP8" s="11"/>
-      <c r="CQ8" s="11"/>
+      <c r="CQ8" s="11" t="s">
+        <v>245</v>
+      </c>
       <c r="CR8" s="10" t="s">
         <v>107</v>
       </c>
@@ -4111,7 +4230,9 @@
       <c r="CT8" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="CU8" s="10"/>
+      <c r="CU8" s="11" t="s">
+        <v>245</v>
+      </c>
       <c r="CV8" s="10" t="s">
         <v>143</v>
       </c>
@@ -4845,7 +4966,9 @@
       </c>
       <c r="CO12" s="16"/>
       <c r="CP12" s="16"/>
-      <c r="CQ12" s="16"/>
+      <c r="CQ12" s="16" t="s">
+        <v>249</v>
+      </c>
       <c r="CR12" s="15" t="s">
         <v>107</v>
       </c>
@@ -4855,7 +4978,9 @@
       <c r="CT12" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="CU12" s="15"/>
+      <c r="CU12" s="16" t="s">
+        <v>249</v>
+      </c>
       <c r="CV12" s="15" t="s">
         <v>143</v>
       </c>
@@ -6719,7 +6844,9 @@
       </c>
       <c r="CO22" s="26"/>
       <c r="CP22" s="26"/>
-      <c r="CQ22" s="26"/>
+      <c r="CQ22" s="26" t="s">
+        <v>246</v>
+      </c>
       <c r="CR22" s="25" t="s">
         <v>107</v>
       </c>
@@ -7463,7 +7590,9 @@
       </c>
       <c r="CO26" s="31"/>
       <c r="CP26" s="31"/>
-      <c r="CQ26" s="31"/>
+      <c r="CQ26" s="30" t="s">
+        <v>247</v>
+      </c>
       <c r="CR26" s="31"/>
       <c r="CS26" s="29">
         <v>757392</v>
@@ -8672,7 +8801,7 @@
       <c r="CO32" s="11"/>
       <c r="CP32" s="11"/>
       <c r="CQ32" s="11" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="CR32" s="10" t="s">
         <v>107</v>
@@ -8680,7 +8809,7 @@
       <c r="CS32" s="11"/>
       <c r="CT32" s="10"/>
       <c r="CU32" s="11" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="CV32" s="10"/>
       <c r="CW32" s="10"/>

</xml_diff>

<commit_message>
Superstrikes and PC290s only disqualify convictions that happen afterward
- if a disqualifying conviction and a Prop64 conviction happen on the same date, the Prop64 conviction is still eligible

[#169372524]

Co-authored-by: Symonne Singleton <symonne@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33840" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -729,9 +729,6 @@
     <t>0</t>
   </si>
   <si>
-    <t>PC 290</t>
-  </si>
-  <si>
     <t>To be reviewed by City Attorneys</t>
   </si>
   <si>
@@ -769,6 +766,9 @@
   </si>
   <si>
     <t>11357(D) - Should be flagged as we distinguish (B) from (D)</t>
+  </si>
+  <si>
+    <t>No applicable eligibility criteria</t>
   </si>
 </sst>
 </file>
@@ -2590,8 +2590,8 @@
   </sheetPr>
   <dimension ref="A1:JB37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BA1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="CU19" sqref="CU19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="DA11" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="DH24" sqref="DH24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -3183,7 +3183,7 @@
         <v>96</v>
       </c>
       <c r="CU2" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="CV2" s="2" t="s">
         <v>97</v>
@@ -4219,7 +4219,7 @@
       <c r="CO8" s="11"/>
       <c r="CP8" s="11"/>
       <c r="CQ8" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="CR8" s="10" t="s">
         <v>107</v>
@@ -4231,7 +4231,7 @@
         <v>142</v>
       </c>
       <c r="CU8" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="CV8" s="10" t="s">
         <v>143</v>
@@ -4967,7 +4967,7 @@
       <c r="CO12" s="16"/>
       <c r="CP12" s="16"/>
       <c r="CQ12" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="CR12" s="15" t="s">
         <v>107</v>
@@ -4979,7 +4979,7 @@
         <v>153</v>
       </c>
       <c r="CU12" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="CV12" s="15" t="s">
         <v>143</v>
@@ -6508,10 +6508,10 @@
         <v>143</v>
       </c>
       <c r="DH20" s="25" t="s">
-        <v>191</v>
+        <v>147</v>
       </c>
       <c r="DI20" s="25" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:113" ht="20" customHeight="1">
@@ -6845,7 +6845,7 @@
       <c r="CO22" s="26"/>
       <c r="CP22" s="26"/>
       <c r="CQ22" s="26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="CR22" s="25" t="s">
         <v>107</v>
@@ -6894,10 +6894,10 @@
         <v>143</v>
       </c>
       <c r="DH22" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="DI22" s="25" t="s">
         <v>237</v>
-      </c>
-      <c r="DI22" s="25" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:113" ht="20" customHeight="1">
@@ -7099,10 +7099,10 @@
         <v>143</v>
       </c>
       <c r="DH23" s="30" t="s">
-        <v>191</v>
+        <v>228</v>
       </c>
       <c r="DI23" s="30" t="s">
-        <v>199</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:113" ht="20" customHeight="1">
@@ -7591,7 +7591,7 @@
       <c r="CO26" s="31"/>
       <c r="CP26" s="31"/>
       <c r="CQ26" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="CR26" s="31"/>
       <c r="CS26" s="29">
@@ -7638,10 +7638,10 @@
         <v>143</v>
       </c>
       <c r="DH26" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="DI26" s="30" t="s">
         <v>237</v>
-      </c>
-      <c r="DI26" s="30" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:113" ht="20" customHeight="1">
@@ -8432,10 +8432,10 @@
         <v>143</v>
       </c>
       <c r="DH30" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="DI30" s="35" t="s">
         <v>237</v>
-      </c>
-      <c r="DI30" s="35" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:113" ht="20" customHeight="1">
@@ -8801,7 +8801,7 @@
       <c r="CO32" s="11"/>
       <c r="CP32" s="11"/>
       <c r="CQ32" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="CR32" s="10" t="s">
         <v>107</v>
@@ -8809,7 +8809,7 @@
       <c r="CS32" s="11"/>
       <c r="CT32" s="10"/>
       <c r="CU32" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="CV32" s="10"/>
       <c r="CW32" s="10"/>
@@ -9239,7 +9239,7 @@
         <v>107</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>
@@ -9248,10 +9248,10 @@
       <c r="K35" s="31"/>
       <c r="L35" s="31"/>
       <c r="M35" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N35" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O35" s="31"/>
       <c r="P35" s="29">
@@ -9315,7 +9315,7 @@
         <v>112</v>
       </c>
       <c r="BD35" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="BE35" s="30" t="s">
         <v>114</v>
@@ -9406,7 +9406,7 @@
         <v>107</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G36" s="31"/>
       <c r="H36" s="31"/>
@@ -9415,10 +9415,10 @@
       <c r="K36" s="31"/>
       <c r="L36" s="31"/>
       <c r="M36" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N36" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O36" s="31"/>
       <c r="P36" s="29">
@@ -9550,7 +9550,7 @@
       </c>
       <c r="CU36" s="30"/>
       <c r="CV36" s="30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="CW36" s="30" t="s">
         <v>143</v>
@@ -9603,7 +9603,7 @@
         <v>107</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G37" s="31"/>
       <c r="H37" s="31"/>
@@ -9612,10 +9612,10 @@
       <c r="K37" s="31"/>
       <c r="L37" s="31"/>
       <c r="M37" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N37" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O37" s="31"/>
       <c r="P37" s="29">
@@ -9679,7 +9679,7 @@
         <v>112</v>
       </c>
       <c r="BD37" s="30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="BE37" s="30" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
Superstrikes don't disqualify convictions
[#169406636]

Co-authored-by: Christa Hartsock <christa@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="248">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -594,9 +594,6 @@
     <t>03/12/2017</t>
   </si>
   <si>
-    <t>Not eligible</t>
-  </si>
-  <si>
     <t>A971951352</t>
   </si>
   <si>
@@ -616,9 +613,6 @@
   </si>
   <si>
     <t>4.0</t>
-  </si>
-  <si>
-    <t>PC 667(e)(2)(c)(iv)</t>
   </si>
   <si>
     <t>220 PC- COMMIT MAYHEM</t>
@@ -1014,8 +1008,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1369,7 +1369,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1400,6 +1400,7 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1430,6 +1431,7 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2590,8 +2592,8 @@
   </sheetPr>
   <dimension ref="A1:JB37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="DA11" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="DH24" sqref="DH24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="DC18" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="DI36" sqref="DI36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2712,16 +2714,16 @@
       <c r="K1" s="46"/>
       <c r="L1" s="46"/>
       <c r="M1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="N1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="P1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Q1" s="46"/>
       <c r="R1" s="46"/>
@@ -2731,7 +2733,7 @@
       <c r="V1" s="46"/>
       <c r="W1" s="46"/>
       <c r="X1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Y1" s="46"/>
       <c r="Z1" s="46"/>
@@ -2748,12 +2750,12 @@
       <c r="AK1" s="46"/>
       <c r="AL1" s="46"/>
       <c r="AM1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AN1" s="46"/>
       <c r="AO1" s="46"/>
       <c r="AP1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AQ1" s="46"/>
       <c r="AR1" s="46"/>
@@ -2761,23 +2763,23 @@
       <c r="AT1" s="46"/>
       <c r="AU1" s="46"/>
       <c r="AV1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AW1" s="46"/>
       <c r="AX1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AY1" s="46"/>
       <c r="AZ1" s="46"/>
       <c r="BA1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="BB1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="BC1" s="46"/>
       <c r="BD1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="BE1" s="46"/>
       <c r="BF1" s="46"/>
@@ -2805,91 +2807,91 @@
       <c r="CB1" s="46"/>
       <c r="CC1" s="46"/>
       <c r="CD1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CE1" s="46"/>
       <c r="CF1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CG1" s="46"/>
       <c r="CH1" s="46"/>
       <c r="CI1" s="46"/>
       <c r="CJ1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CK1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CL1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CM1" s="46"/>
       <c r="CN1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CO1" s="46"/>
       <c r="CP1" s="46"/>
       <c r="CQ1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CR1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CS1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CT1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CU1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CV1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CW1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CX1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CY1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CZ1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DA1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DB1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DC1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DD1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DE1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DF1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DG1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DH1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DI1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:113" ht="20.25" customHeight="1">
       <c r="A2" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -3183,7 +3185,7 @@
         <v>96</v>
       </c>
       <c r="CU2" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="CV2" s="2" t="s">
         <v>97</v>
@@ -3207,16 +3209,16 @@
         <v>103</v>
       </c>
       <c r="DC2" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="DD2" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="DE2" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="DD2" s="2" t="s">
+      <c r="DF2" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="DE2" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="DF2" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="DG2" s="2" t="s">
         <v>104</v>
@@ -4065,7 +4067,7 @@
     </row>
     <row r="8" spans="1:113" ht="20" customHeight="1">
       <c r="A8" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -4219,7 +4221,7 @@
       <c r="CO8" s="11"/>
       <c r="CP8" s="11"/>
       <c r="CQ8" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="CR8" s="10" t="s">
         <v>107</v>
@@ -4231,7 +4233,7 @@
         <v>142</v>
       </c>
       <c r="CU8" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="CV8" s="10" t="s">
         <v>143</v>
@@ -4255,16 +4257,16 @@
         <v>146</v>
       </c>
       <c r="DC8" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD8" s="10" t="s">
         <v>146</v>
       </c>
       <c r="DE8" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF8" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG8" s="10" t="s">
         <v>104</v>
@@ -4273,7 +4275,7 @@
         <v>147</v>
       </c>
       <c r="DI8" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:113" ht="20" customHeight="1">
@@ -4443,7 +4445,7 @@
     </row>
     <row r="10" spans="1:113" ht="20" customHeight="1">
       <c r="A10" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
@@ -4632,19 +4634,19 @@
         <v>142</v>
       </c>
       <c r="DD10" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DE10" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF10" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG10" s="15" t="s">
         <v>143</v>
       </c>
       <c r="DH10" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="DI10" s="15" t="s">
         <v>158</v>
@@ -4813,7 +4815,7 @@
     </row>
     <row r="12" spans="1:113" ht="20" customHeight="1">
       <c r="A12" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
@@ -4967,7 +4969,7 @@
       <c r="CO12" s="16"/>
       <c r="CP12" s="16"/>
       <c r="CQ12" s="16" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="CR12" s="15" t="s">
         <v>107</v>
@@ -4979,7 +4981,7 @@
         <v>153</v>
       </c>
       <c r="CU12" s="16" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="CV12" s="15" t="s">
         <v>143</v>
@@ -5006,13 +5008,13 @@
         <v>142</v>
       </c>
       <c r="DD12" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DE12" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF12" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG12" s="15" t="s">
         <v>143</v>
@@ -5195,7 +5197,7 @@
     </row>
     <row r="14" spans="1:113" ht="20" customHeight="1">
       <c r="A14" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -5383,7 +5385,7 @@
         <v>172</v>
       </c>
       <c r="DC14" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD14" s="20" t="s">
         <v>153</v>
@@ -5392,7 +5394,7 @@
         <v>146</v>
       </c>
       <c r="DF14" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG14" s="20" t="s">
         <v>143</v>
@@ -5401,7 +5403,7 @@
         <v>147</v>
       </c>
       <c r="DI14" s="20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:113" ht="20" customHeight="1">
@@ -5756,7 +5758,7 @@
     </row>
     <row r="17" spans="1:113" ht="20" customHeight="1">
       <c r="A17" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -5942,7 +5944,7 @@
         <v>172</v>
       </c>
       <c r="DC17" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD17" s="20" t="s">
         <v>153</v>
@@ -5951,7 +5953,7 @@
         <v>146</v>
       </c>
       <c r="DF17" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG17" s="20" t="s">
         <v>143</v>
@@ -5960,7 +5962,7 @@
         <v>147</v>
       </c>
       <c r="DI17" s="20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:113" ht="20" customHeight="1">
@@ -6313,7 +6315,7 @@
     </row>
     <row r="20" spans="1:113" ht="20" customHeight="1">
       <c r="A20" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
@@ -6493,16 +6495,16 @@
         <v>142</v>
       </c>
       <c r="DC20" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD20" s="25" t="s">
         <v>142</v>
       </c>
       <c r="DE20" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF20" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG20" s="25" t="s">
         <v>143</v>
@@ -6511,7 +6513,7 @@
         <v>147</v>
       </c>
       <c r="DI20" s="25" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:113" ht="20" customHeight="1">
@@ -6691,7 +6693,7 @@
     </row>
     <row r="22" spans="1:113" ht="20" customHeight="1">
       <c r="A22" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
@@ -6845,7 +6847,7 @@
       <c r="CO22" s="26"/>
       <c r="CP22" s="26"/>
       <c r="CQ22" s="26" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="CR22" s="25" t="s">
         <v>107</v>
@@ -6879,30 +6881,30 @@
         <v>142</v>
       </c>
       <c r="DC22" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD22" s="25" t="s">
         <v>142</v>
       </c>
       <c r="DE22" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF22" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG22" s="25" t="s">
         <v>143</v>
       </c>
       <c r="DH22" s="25" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="DI22" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:113" ht="20" customHeight="1">
       <c r="A23" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -6913,7 +6915,7 @@
         <v>107</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
@@ -6922,10 +6924,10 @@
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
       <c r="M23" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="N23" s="30" t="s">
         <v>192</v>
-      </c>
-      <c r="N23" s="30" t="s">
-        <v>193</v>
       </c>
       <c r="O23" s="31"/>
       <c r="P23" s="29">
@@ -7059,11 +7061,11 @@
         <v>757392</v>
       </c>
       <c r="CT23" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="CU23" s="30"/>
       <c r="CV23" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="CW23" s="30" t="s">
         <v>143</v>
@@ -7072,13 +7074,13 @@
         <v>143</v>
       </c>
       <c r="CY23" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="CZ23" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="CZ23" s="30" t="s">
+      <c r="DA23" s="30" t="s">
         <v>197</v>
-      </c>
-      <c r="DA23" s="30" t="s">
-        <v>198</v>
       </c>
       <c r="DB23" s="30" t="s">
         <v>153</v>
@@ -7093,16 +7095,16 @@
         <v>146</v>
       </c>
       <c r="DF23" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG23" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DH23" s="30" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="DI23" s="30" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:113" ht="20" customHeight="1">
@@ -7116,7 +7118,7 @@
         <v>107</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -7125,10 +7127,10 @@
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
       <c r="M24" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="N24" s="30" t="s">
         <v>192</v>
-      </c>
-      <c r="N24" s="30" t="s">
-        <v>193</v>
       </c>
       <c r="O24" s="31"/>
       <c r="P24" s="29">
@@ -7194,7 +7196,7 @@
         <v>112</v>
       </c>
       <c r="BD24" s="30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="BE24" s="30" t="s">
         <v>114</v>
@@ -7287,7 +7289,7 @@
         <v>107</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
@@ -7296,10 +7298,10 @@
       <c r="K25" s="31"/>
       <c r="L25" s="31"/>
       <c r="M25" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="N25" s="30" t="s">
         <v>192</v>
-      </c>
-      <c r="N25" s="30" t="s">
-        <v>193</v>
       </c>
       <c r="O25" s="31"/>
       <c r="P25" s="29">
@@ -7443,7 +7445,7 @@
     </row>
     <row r="26" spans="1:113" ht="20" customHeight="1">
       <c r="A26" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
@@ -7454,7 +7456,7 @@
         <v>107</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
@@ -7463,10 +7465,10 @@
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
       <c r="M26" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="N26" s="30" t="s">
         <v>192</v>
-      </c>
-      <c r="N26" s="30" t="s">
-        <v>193</v>
       </c>
       <c r="O26" s="31"/>
       <c r="P26" s="29">
@@ -7591,18 +7593,18 @@
       <c r="CO26" s="31"/>
       <c r="CP26" s="31"/>
       <c r="CQ26" s="30" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="CR26" s="31"/>
       <c r="CS26" s="29">
         <v>757392</v>
       </c>
       <c r="CT26" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="CU26" s="30"/>
       <c r="CV26" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="CW26" s="30" t="s">
         <v>143</v>
@@ -7611,13 +7613,13 @@
         <v>143</v>
       </c>
       <c r="CY26" s="30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="CZ26" s="30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="DA26" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="DB26" s="30" t="s">
         <v>153</v>
@@ -7632,21 +7634,21 @@
         <v>146</v>
       </c>
       <c r="DF26" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG26" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DH26" s="30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="DI26" s="30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:113" ht="20" customHeight="1">
       <c r="A27" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
@@ -7657,7 +7659,7 @@
         <v>107</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
@@ -7666,10 +7668,10 @@
       <c r="K27" s="31"/>
       <c r="L27" s="31"/>
       <c r="M27" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="N27" s="30" t="s">
         <v>192</v>
-      </c>
-      <c r="N27" s="30" t="s">
-        <v>193</v>
       </c>
       <c r="O27" s="31"/>
       <c r="P27" s="29">
@@ -7733,7 +7735,7 @@
         <v>112</v>
       </c>
       <c r="BD27" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="BE27" s="30" t="s">
         <v>114</v>
@@ -7799,11 +7801,11 @@
         <v>757392</v>
       </c>
       <c r="CT27" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="CU27" s="30"/>
       <c r="CV27" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="CW27" s="30" t="s">
         <v>143</v>
@@ -7812,13 +7814,13 @@
         <v>143</v>
       </c>
       <c r="CY27" s="30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="CZ27" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="DA27" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="DB27" s="30" t="s">
         <v>153</v>
@@ -7833,21 +7835,21 @@
         <v>146</v>
       </c>
       <c r="DF27" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG27" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DH27" s="30" t="s">
-        <v>191</v>
+        <v>226</v>
       </c>
       <c r="DI27" s="30" t="s">
-        <v>199</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:113" ht="20" customHeight="1">
       <c r="A28" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
@@ -7870,7 +7872,7 @@
         <v>1008675309</v>
       </c>
       <c r="N28" s="35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="O28" s="36"/>
       <c r="P28" s="34">
@@ -7936,13 +7938,13 @@
         <v>112</v>
       </c>
       <c r="BD28" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="BE28" s="35" t="s">
         <v>114</v>
       </c>
       <c r="BF28" s="35" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="BG28" s="36"/>
       <c r="BH28" s="36"/>
@@ -8005,7 +8007,7 @@
         <v>107</v>
       </c>
       <c r="CS28" s="35" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="CT28" s="35" t="s">
         <v>153</v>
@@ -8021,28 +8023,28 @@
         <v>143</v>
       </c>
       <c r="CY28" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="CZ28" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="DA28" s="35" t="s">
         <v>209</v>
-      </c>
-      <c r="CZ28" s="35" t="s">
-        <v>210</v>
-      </c>
-      <c r="DA28" s="35" t="s">
-        <v>211</v>
       </c>
       <c r="DB28" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DC28" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD28" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DE28" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DF28" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG28" s="35" t="s">
         <v>143</v>
@@ -8051,7 +8053,7 @@
         <v>147</v>
       </c>
       <c r="DI28" s="35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="29" spans="1:113" ht="20" customHeight="1">
@@ -8077,7 +8079,7 @@
         <v>1008675309</v>
       </c>
       <c r="N29" s="35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="O29" s="36"/>
       <c r="P29" s="34">
@@ -8143,13 +8145,13 @@
         <v>112</v>
       </c>
       <c r="BD29" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="BE29" s="35" t="s">
         <v>114</v>
       </c>
       <c r="BF29" s="35" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="BG29" s="36"/>
       <c r="BH29" s="36"/>
@@ -8231,7 +8233,7 @@
     </row>
     <row r="30" spans="1:113" ht="20" customHeight="1">
       <c r="A30" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="33"/>
@@ -8254,7 +8256,7 @@
         <v>1008675309</v>
       </c>
       <c r="N30" s="35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="O30" s="36"/>
       <c r="P30" s="34">
@@ -8320,13 +8322,13 @@
         <v>112</v>
       </c>
       <c r="BD30" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="BE30" s="35" t="s">
         <v>128</v>
       </c>
       <c r="BF30" s="35" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="BG30" s="36"/>
       <c r="BH30" s="36"/>
@@ -8389,7 +8391,7 @@
         <v>107</v>
       </c>
       <c r="CS30" s="35" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="CT30" s="35" t="s">
         <v>153</v>
@@ -8405,42 +8407,42 @@
         <v>143</v>
       </c>
       <c r="CY30" s="35" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="CZ30" s="35" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="DA30" s="35" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="DB30" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DC30" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD30" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DE30" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DF30" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG30" s="35" t="s">
         <v>143</v>
       </c>
       <c r="DH30" s="35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="DI30" s="35" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:113" ht="20" customHeight="1">
       <c r="A31" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -8463,7 +8465,7 @@
         <v>181</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="9">
@@ -8598,7 +8600,7 @@
         <v>107</v>
       </c>
       <c r="CS31" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="CT31" s="10" t="s">
         <v>142</v>
@@ -8614,28 +8616,28 @@
         <v>143</v>
       </c>
       <c r="CY31" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="CZ31" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="DA31" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="DB31" s="10" t="s">
         <v>146</v>
       </c>
       <c r="DC31" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD31" s="10" t="s">
         <v>146</v>
       </c>
       <c r="DE31" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF31" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG31" s="10" t="s">
         <v>143</v>
@@ -8644,7 +8646,7 @@
         <v>147</v>
       </c>
       <c r="DI31" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:113" ht="20" customHeight="1">
@@ -8670,7 +8672,7 @@
         <v>181</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="9">
@@ -8736,13 +8738,13 @@
         <v>112</v>
       </c>
       <c r="BD32" s="52" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="BE32" s="10" t="s">
         <v>114</v>
       </c>
       <c r="BF32" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="BG32" s="11"/>
       <c r="BH32" s="11"/>
@@ -8801,7 +8803,7 @@
       <c r="CO32" s="11"/>
       <c r="CP32" s="11"/>
       <c r="CQ32" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="CR32" s="10" t="s">
         <v>107</v>
@@ -8809,7 +8811,7 @@
       <c r="CS32" s="11"/>
       <c r="CT32" s="10"/>
       <c r="CU32" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="CV32" s="10"/>
       <c r="CW32" s="10"/>
@@ -8828,7 +8830,7 @@
     </row>
     <row r="33" spans="1:113" ht="20" customHeight="1">
       <c r="A33" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
@@ -8848,10 +8850,10 @@
       <c r="K33" s="16"/>
       <c r="L33" s="16"/>
       <c r="M33" s="15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="14">
@@ -8994,28 +8996,28 @@
         <v>143</v>
       </c>
       <c r="CY33" s="15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="CZ33" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="DA33" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="DB33" s="15" t="s">
         <v>146</v>
       </c>
       <c r="DC33" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD33" s="15" t="s">
         <v>146</v>
       </c>
       <c r="DE33" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF33" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG33" s="15" t="s">
         <v>143</v>
@@ -9024,12 +9026,12 @@
         <v>147</v>
       </c>
       <c r="DI33" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:113" ht="20" customHeight="1">
       <c r="A34" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
@@ -9049,10 +9051,10 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
       <c r="M34" s="20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="N34" s="20" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O34" s="21"/>
       <c r="P34" s="19">
@@ -9195,37 +9197,37 @@
         <v>143</v>
       </c>
       <c r="CY34" s="20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="CZ34" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="DA34" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="DB34" s="20" t="s">
         <v>146</v>
       </c>
       <c r="DC34" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD34" s="20" t="s">
         <v>146</v>
       </c>
       <c r="DE34" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF34" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG34" s="20" t="s">
         <v>143</v>
       </c>
       <c r="DH34" s="20" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="DI34" s="20" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:113" ht="20" customHeight="1">
@@ -9239,7 +9241,7 @@
         <v>107</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>
@@ -9248,10 +9250,10 @@
       <c r="K35" s="31"/>
       <c r="L35" s="31"/>
       <c r="M35" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="N35" s="30" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O35" s="31"/>
       <c r="P35" s="29">
@@ -9315,7 +9317,7 @@
         <v>112</v>
       </c>
       <c r="BD35" s="30" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BE35" s="30" t="s">
         <v>114</v>
@@ -9395,7 +9397,7 @@
     </row>
     <row r="36" spans="1:113" ht="20" customHeight="1">
       <c r="A36" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B36" s="27"/>
       <c r="C36" s="28"/>
@@ -9406,7 +9408,7 @@
         <v>107</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G36" s="31"/>
       <c r="H36" s="31"/>
@@ -9415,10 +9417,10 @@
       <c r="K36" s="31"/>
       <c r="L36" s="31"/>
       <c r="M36" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="N36" s="30" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O36" s="31"/>
       <c r="P36" s="29">
@@ -9550,7 +9552,7 @@
       </c>
       <c r="CU36" s="30"/>
       <c r="CV36" s="30" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="CW36" s="30" t="s">
         <v>143</v>
@@ -9559,37 +9561,37 @@
         <v>143</v>
       </c>
       <c r="CY36" s="30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="CZ36" s="30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="DA36" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="DB36" s="30" t="s">
         <v>146</v>
       </c>
       <c r="DC36" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD36" s="30" t="s">
         <v>146</v>
       </c>
       <c r="DE36" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF36" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG36" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DH36" s="30" t="s">
-        <v>191</v>
+        <v>226</v>
       </c>
       <c r="DI36" s="30" t="s">
-        <v>199</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:113" ht="20" customHeight="1">
@@ -9603,7 +9605,7 @@
         <v>107</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G37" s="31"/>
       <c r="H37" s="31"/>
@@ -9612,10 +9614,10 @@
       <c r="K37" s="31"/>
       <c r="L37" s="31"/>
       <c r="M37" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="N37" s="30" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O37" s="31"/>
       <c r="P37" s="29">
@@ -9679,7 +9681,7 @@
         <v>112</v>
       </c>
       <c r="BD37" s="30" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="BE37" s="30" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
Don't disqualify for superstrikes or 290s
[#169406636]

Co-authored-by: Christa Hartsock <christa@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="248">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -594,9 +594,6 @@
     <t>03/12/2017</t>
   </si>
   <si>
-    <t>Not eligible</t>
-  </si>
-  <si>
     <t>A971951352</t>
   </si>
   <si>
@@ -616,9 +613,6 @@
   </si>
   <si>
     <t>4.0</t>
-  </si>
-  <si>
-    <t>PC 667(e)(2)(c)(iv)</t>
   </si>
   <si>
     <t>220 PC- COMMIT MAYHEM</t>
@@ -1014,8 +1008,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1369,7 +1381,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1400,6 +1412,9 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1430,6 +1445,9 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2590,8 +2608,8 @@
   </sheetPr>
   <dimension ref="A1:JB37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="DA11" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="DH24" sqref="DH24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="DA25" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="DI36" sqref="DI36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2712,16 +2730,16 @@
       <c r="K1" s="46"/>
       <c r="L1" s="46"/>
       <c r="M1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="N1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="O1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="P1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Q1" s="46"/>
       <c r="R1" s="46"/>
@@ -2731,7 +2749,7 @@
       <c r="V1" s="46"/>
       <c r="W1" s="46"/>
       <c r="X1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Y1" s="46"/>
       <c r="Z1" s="46"/>
@@ -2748,12 +2766,12 @@
       <c r="AK1" s="46"/>
       <c r="AL1" s="46"/>
       <c r="AM1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AN1" s="46"/>
       <c r="AO1" s="46"/>
       <c r="AP1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AQ1" s="46"/>
       <c r="AR1" s="46"/>
@@ -2761,23 +2779,23 @@
       <c r="AT1" s="46"/>
       <c r="AU1" s="46"/>
       <c r="AV1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AW1" s="46"/>
       <c r="AX1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AY1" s="46"/>
       <c r="AZ1" s="46"/>
       <c r="BA1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="BB1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="BC1" s="46"/>
       <c r="BD1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="BE1" s="46"/>
       <c r="BF1" s="46"/>
@@ -2805,91 +2823,91 @@
       <c r="CB1" s="46"/>
       <c r="CC1" s="46"/>
       <c r="CD1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CE1" s="46"/>
       <c r="CF1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CG1" s="46"/>
       <c r="CH1" s="46"/>
       <c r="CI1" s="46"/>
       <c r="CJ1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CK1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CL1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CM1" s="46"/>
       <c r="CN1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CO1" s="46"/>
       <c r="CP1" s="46"/>
       <c r="CQ1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CR1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CS1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CT1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CU1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CV1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CW1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CX1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CY1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="CZ1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DA1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DB1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DC1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DD1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DE1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DF1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DG1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DH1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="DI1" s="46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:113" ht="20.25" customHeight="1">
       <c r="A2" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -3183,7 +3201,7 @@
         <v>96</v>
       </c>
       <c r="CU2" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="CV2" s="2" t="s">
         <v>97</v>
@@ -3207,16 +3225,16 @@
         <v>103</v>
       </c>
       <c r="DC2" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="DD2" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="DE2" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="DD2" s="2" t="s">
+      <c r="DF2" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="DE2" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="DF2" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="DG2" s="2" t="s">
         <v>104</v>
@@ -4065,7 +4083,7 @@
     </row>
     <row r="8" spans="1:113" ht="20" customHeight="1">
       <c r="A8" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -4219,7 +4237,7 @@
       <c r="CO8" s="11"/>
       <c r="CP8" s="11"/>
       <c r="CQ8" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="CR8" s="10" t="s">
         <v>107</v>
@@ -4231,7 +4249,7 @@
         <v>142</v>
       </c>
       <c r="CU8" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="CV8" s="10" t="s">
         <v>143</v>
@@ -4255,16 +4273,16 @@
         <v>146</v>
       </c>
       <c r="DC8" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD8" s="10" t="s">
         <v>146</v>
       </c>
       <c r="DE8" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF8" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG8" s="10" t="s">
         <v>104</v>
@@ -4273,7 +4291,7 @@
         <v>147</v>
       </c>
       <c r="DI8" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:113" ht="20" customHeight="1">
@@ -4443,7 +4461,7 @@
     </row>
     <row r="10" spans="1:113" ht="20" customHeight="1">
       <c r="A10" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
@@ -4632,19 +4650,19 @@
         <v>142</v>
       </c>
       <c r="DD10" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DE10" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF10" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG10" s="15" t="s">
         <v>143</v>
       </c>
       <c r="DH10" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="DI10" s="15" t="s">
         <v>158</v>
@@ -4813,7 +4831,7 @@
     </row>
     <row r="12" spans="1:113" ht="20" customHeight="1">
       <c r="A12" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
@@ -4967,7 +4985,7 @@
       <c r="CO12" s="16"/>
       <c r="CP12" s="16"/>
       <c r="CQ12" s="16" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="CR12" s="15" t="s">
         <v>107</v>
@@ -4979,7 +4997,7 @@
         <v>153</v>
       </c>
       <c r="CU12" s="16" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="CV12" s="15" t="s">
         <v>143</v>
@@ -5006,13 +5024,13 @@
         <v>142</v>
       </c>
       <c r="DD12" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DE12" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF12" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG12" s="15" t="s">
         <v>143</v>
@@ -5195,7 +5213,7 @@
     </row>
     <row r="14" spans="1:113" ht="20" customHeight="1">
       <c r="A14" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B14" s="17"/>
       <c r="C14" s="18"/>
@@ -5383,7 +5401,7 @@
         <v>172</v>
       </c>
       <c r="DC14" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD14" s="20" t="s">
         <v>153</v>
@@ -5392,7 +5410,7 @@
         <v>146</v>
       </c>
       <c r="DF14" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG14" s="20" t="s">
         <v>143</v>
@@ -5401,7 +5419,7 @@
         <v>147</v>
       </c>
       <c r="DI14" s="20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:113" ht="20" customHeight="1">
@@ -5756,7 +5774,7 @@
     </row>
     <row r="17" spans="1:113" ht="20" customHeight="1">
       <c r="A17" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
@@ -5942,7 +5960,7 @@
         <v>172</v>
       </c>
       <c r="DC17" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD17" s="20" t="s">
         <v>153</v>
@@ -5951,7 +5969,7 @@
         <v>146</v>
       </c>
       <c r="DF17" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG17" s="20" t="s">
         <v>143</v>
@@ -5960,7 +5978,7 @@
         <v>147</v>
       </c>
       <c r="DI17" s="20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:113" ht="20" customHeight="1">
@@ -6313,7 +6331,7 @@
     </row>
     <row r="20" spans="1:113" ht="20" customHeight="1">
       <c r="A20" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
@@ -6493,16 +6511,16 @@
         <v>142</v>
       </c>
       <c r="DC20" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD20" s="25" t="s">
         <v>142</v>
       </c>
       <c r="DE20" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF20" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG20" s="25" t="s">
         <v>143</v>
@@ -6511,7 +6529,7 @@
         <v>147</v>
       </c>
       <c r="DI20" s="25" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:113" ht="20" customHeight="1">
@@ -6691,7 +6709,7 @@
     </row>
     <row r="22" spans="1:113" ht="20" customHeight="1">
       <c r="A22" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
@@ -6845,7 +6863,7 @@
       <c r="CO22" s="26"/>
       <c r="CP22" s="26"/>
       <c r="CQ22" s="26" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="CR22" s="25" t="s">
         <v>107</v>
@@ -6879,30 +6897,30 @@
         <v>142</v>
       </c>
       <c r="DC22" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD22" s="25" t="s">
         <v>142</v>
       </c>
       <c r="DE22" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF22" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG22" s="25" t="s">
         <v>143</v>
       </c>
       <c r="DH22" s="25" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="DI22" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:113" ht="20" customHeight="1">
       <c r="A23" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="28"/>
@@ -6913,7 +6931,7 @@
         <v>107</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
@@ -6922,10 +6940,10 @@
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
       <c r="M23" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="N23" s="30" t="s">
         <v>192</v>
-      </c>
-      <c r="N23" s="30" t="s">
-        <v>193</v>
       </c>
       <c r="O23" s="31"/>
       <c r="P23" s="29">
@@ -7059,11 +7077,11 @@
         <v>757392</v>
       </c>
       <c r="CT23" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="CU23" s="30"/>
       <c r="CV23" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="CW23" s="30" t="s">
         <v>143</v>
@@ -7072,13 +7090,13 @@
         <v>143</v>
       </c>
       <c r="CY23" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="CZ23" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="CZ23" s="30" t="s">
+      <c r="DA23" s="30" t="s">
         <v>197</v>
-      </c>
-      <c r="DA23" s="30" t="s">
-        <v>198</v>
       </c>
       <c r="DB23" s="30" t="s">
         <v>153</v>
@@ -7093,16 +7111,16 @@
         <v>146</v>
       </c>
       <c r="DF23" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG23" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DH23" s="30" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="DI23" s="30" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:113" ht="20" customHeight="1">
@@ -7116,7 +7134,7 @@
         <v>107</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -7125,10 +7143,10 @@
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
       <c r="M24" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="N24" s="30" t="s">
         <v>192</v>
-      </c>
-      <c r="N24" s="30" t="s">
-        <v>193</v>
       </c>
       <c r="O24" s="31"/>
       <c r="P24" s="29">
@@ -7194,7 +7212,7 @@
         <v>112</v>
       </c>
       <c r="BD24" s="30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="BE24" s="30" t="s">
         <v>114</v>
@@ -7287,7 +7305,7 @@
         <v>107</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
@@ -7296,10 +7314,10 @@
       <c r="K25" s="31"/>
       <c r="L25" s="31"/>
       <c r="M25" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="N25" s="30" t="s">
         <v>192</v>
-      </c>
-      <c r="N25" s="30" t="s">
-        <v>193</v>
       </c>
       <c r="O25" s="31"/>
       <c r="P25" s="29">
@@ -7443,7 +7461,7 @@
     </row>
     <row r="26" spans="1:113" ht="20" customHeight="1">
       <c r="A26" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="28"/>
@@ -7454,7 +7472,7 @@
         <v>107</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
@@ -7463,10 +7481,10 @@
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
       <c r="M26" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="N26" s="30" t="s">
         <v>192</v>
-      </c>
-      <c r="N26" s="30" t="s">
-        <v>193</v>
       </c>
       <c r="O26" s="31"/>
       <c r="P26" s="29">
@@ -7591,18 +7609,18 @@
       <c r="CO26" s="31"/>
       <c r="CP26" s="31"/>
       <c r="CQ26" s="30" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="CR26" s="31"/>
       <c r="CS26" s="29">
         <v>757392</v>
       </c>
       <c r="CT26" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="CU26" s="30"/>
       <c r="CV26" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="CW26" s="30" t="s">
         <v>143</v>
@@ -7611,13 +7629,13 @@
         <v>143</v>
       </c>
       <c r="CY26" s="30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="CZ26" s="30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="DA26" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="DB26" s="30" t="s">
         <v>153</v>
@@ -7632,21 +7650,21 @@
         <v>146</v>
       </c>
       <c r="DF26" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG26" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DH26" s="30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="DI26" s="30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:113" ht="20" customHeight="1">
       <c r="A27" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="28"/>
@@ -7657,7 +7675,7 @@
         <v>107</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
@@ -7666,10 +7684,10 @@
       <c r="K27" s="31"/>
       <c r="L27" s="31"/>
       <c r="M27" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="N27" s="30" t="s">
         <v>192</v>
-      </c>
-      <c r="N27" s="30" t="s">
-        <v>193</v>
       </c>
       <c r="O27" s="31"/>
       <c r="P27" s="29">
@@ -7733,7 +7751,7 @@
         <v>112</v>
       </c>
       <c r="BD27" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="BE27" s="30" t="s">
         <v>114</v>
@@ -7799,11 +7817,11 @@
         <v>757392</v>
       </c>
       <c r="CT27" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="CU27" s="30"/>
       <c r="CV27" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="CW27" s="30" t="s">
         <v>143</v>
@@ -7812,13 +7830,13 @@
         <v>143</v>
       </c>
       <c r="CY27" s="30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="CZ27" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="DA27" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="DB27" s="30" t="s">
         <v>153</v>
@@ -7833,21 +7851,21 @@
         <v>146</v>
       </c>
       <c r="DF27" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG27" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DH27" s="30" t="s">
-        <v>191</v>
+        <v>226</v>
       </c>
       <c r="DI27" s="30" t="s">
-        <v>199</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:113" ht="20" customHeight="1">
       <c r="A28" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
@@ -7870,7 +7888,7 @@
         <v>1008675309</v>
       </c>
       <c r="N28" s="35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="O28" s="36"/>
       <c r="P28" s="34">
@@ -7936,13 +7954,13 @@
         <v>112</v>
       </c>
       <c r="BD28" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="BE28" s="35" t="s">
         <v>114</v>
       </c>
       <c r="BF28" s="35" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="BG28" s="36"/>
       <c r="BH28" s="36"/>
@@ -8005,7 +8023,7 @@
         <v>107</v>
       </c>
       <c r="CS28" s="35" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="CT28" s="35" t="s">
         <v>153</v>
@@ -8021,28 +8039,28 @@
         <v>143</v>
       </c>
       <c r="CY28" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="CZ28" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="DA28" s="35" t="s">
         <v>209</v>
-      </c>
-      <c r="CZ28" s="35" t="s">
-        <v>210</v>
-      </c>
-      <c r="DA28" s="35" t="s">
-        <v>211</v>
       </c>
       <c r="DB28" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DC28" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD28" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DE28" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DF28" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG28" s="35" t="s">
         <v>143</v>
@@ -8051,7 +8069,7 @@
         <v>147</v>
       </c>
       <c r="DI28" s="35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="29" spans="1:113" ht="20" customHeight="1">
@@ -8077,7 +8095,7 @@
         <v>1008675309</v>
       </c>
       <c r="N29" s="35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="O29" s="36"/>
       <c r="P29" s="34">
@@ -8143,13 +8161,13 @@
         <v>112</v>
       </c>
       <c r="BD29" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="BE29" s="35" t="s">
         <v>114</v>
       </c>
       <c r="BF29" s="35" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="BG29" s="36"/>
       <c r="BH29" s="36"/>
@@ -8231,7 +8249,7 @@
     </row>
     <row r="30" spans="1:113" ht="20" customHeight="1">
       <c r="A30" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="33"/>
@@ -8254,7 +8272,7 @@
         <v>1008675309</v>
       </c>
       <c r="N30" s="35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="O30" s="36"/>
       <c r="P30" s="34">
@@ -8320,13 +8338,13 @@
         <v>112</v>
       </c>
       <c r="BD30" s="35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="BE30" s="35" t="s">
         <v>128</v>
       </c>
       <c r="BF30" s="35" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="BG30" s="36"/>
       <c r="BH30" s="36"/>
@@ -8389,7 +8407,7 @@
         <v>107</v>
       </c>
       <c r="CS30" s="35" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="CT30" s="35" t="s">
         <v>153</v>
@@ -8405,42 +8423,42 @@
         <v>143</v>
       </c>
       <c r="CY30" s="35" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="CZ30" s="35" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="DA30" s="35" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="DB30" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DC30" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD30" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DE30" s="35" t="s">
         <v>153</v>
       </c>
       <c r="DF30" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG30" s="35" t="s">
         <v>143</v>
       </c>
       <c r="DH30" s="35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="DI30" s="35" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:113" ht="20" customHeight="1">
       <c r="A31" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -8463,7 +8481,7 @@
         <v>181</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="9">
@@ -8598,7 +8616,7 @@
         <v>107</v>
       </c>
       <c r="CS31" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="CT31" s="10" t="s">
         <v>142</v>
@@ -8614,28 +8632,28 @@
         <v>143</v>
       </c>
       <c r="CY31" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="CZ31" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="DA31" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="DB31" s="10" t="s">
         <v>146</v>
       </c>
       <c r="DC31" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD31" s="10" t="s">
         <v>146</v>
       </c>
       <c r="DE31" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF31" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG31" s="10" t="s">
         <v>143</v>
@@ -8644,7 +8662,7 @@
         <v>147</v>
       </c>
       <c r="DI31" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:113" ht="20" customHeight="1">
@@ -8670,7 +8688,7 @@
         <v>181</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="9">
@@ -8736,13 +8754,13 @@
         <v>112</v>
       </c>
       <c r="BD32" s="52" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="BE32" s="10" t="s">
         <v>114</v>
       </c>
       <c r="BF32" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="BG32" s="11"/>
       <c r="BH32" s="11"/>
@@ -8801,7 +8819,7 @@
       <c r="CO32" s="11"/>
       <c r="CP32" s="11"/>
       <c r="CQ32" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="CR32" s="10" t="s">
         <v>107</v>
@@ -8809,7 +8827,7 @@
       <c r="CS32" s="11"/>
       <c r="CT32" s="10"/>
       <c r="CU32" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="CV32" s="10"/>
       <c r="CW32" s="10"/>
@@ -8828,7 +8846,7 @@
     </row>
     <row r="33" spans="1:113" ht="20" customHeight="1">
       <c r="A33" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
@@ -8848,10 +8866,10 @@
       <c r="K33" s="16"/>
       <c r="L33" s="16"/>
       <c r="M33" s="15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="14">
@@ -8994,28 +9012,28 @@
         <v>143</v>
       </c>
       <c r="CY33" s="15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="CZ33" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="DA33" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="DB33" s="15" t="s">
         <v>146</v>
       </c>
       <c r="DC33" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD33" s="15" t="s">
         <v>146</v>
       </c>
       <c r="DE33" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF33" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG33" s="15" t="s">
         <v>143</v>
@@ -9024,12 +9042,12 @@
         <v>147</v>
       </c>
       <c r="DI33" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:113" ht="20" customHeight="1">
       <c r="A34" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
@@ -9049,10 +9067,10 @@
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
       <c r="M34" s="20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="N34" s="20" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O34" s="21"/>
       <c r="P34" s="19">
@@ -9195,37 +9213,37 @@
         <v>143</v>
       </c>
       <c r="CY34" s="20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="CZ34" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="DA34" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="DB34" s="20" t="s">
         <v>146</v>
       </c>
       <c r="DC34" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD34" s="20" t="s">
         <v>146</v>
       </c>
       <c r="DE34" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF34" s="20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG34" s="20" t="s">
         <v>143</v>
       </c>
       <c r="DH34" s="20" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="DI34" s="20" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:113" ht="20" customHeight="1">
@@ -9239,7 +9257,7 @@
         <v>107</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>
@@ -9248,10 +9266,10 @@
       <c r="K35" s="31"/>
       <c r="L35" s="31"/>
       <c r="M35" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="N35" s="30" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O35" s="31"/>
       <c r="P35" s="29">
@@ -9315,7 +9333,7 @@
         <v>112</v>
       </c>
       <c r="BD35" s="30" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BE35" s="30" t="s">
         <v>114</v>
@@ -9395,7 +9413,7 @@
     </row>
     <row r="36" spans="1:113" ht="20" customHeight="1">
       <c r="A36" s="50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B36" s="27"/>
       <c r="C36" s="28"/>
@@ -9406,7 +9424,7 @@
         <v>107</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G36" s="31"/>
       <c r="H36" s="31"/>
@@ -9415,10 +9433,10 @@
       <c r="K36" s="31"/>
       <c r="L36" s="31"/>
       <c r="M36" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="N36" s="30" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O36" s="31"/>
       <c r="P36" s="29">
@@ -9550,7 +9568,7 @@
       </c>
       <c r="CU36" s="30"/>
       <c r="CV36" s="30" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="CW36" s="30" t="s">
         <v>143</v>
@@ -9559,37 +9577,37 @@
         <v>143</v>
       </c>
       <c r="CY36" s="30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="CZ36" s="30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="DA36" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="DB36" s="30" t="s">
         <v>146</v>
       </c>
       <c r="DC36" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DD36" s="30" t="s">
         <v>146</v>
       </c>
       <c r="DE36" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DF36" s="30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DG36" s="30" t="s">
         <v>143</v>
       </c>
       <c r="DH36" s="30" t="s">
-        <v>191</v>
+        <v>226</v>
       </c>
       <c r="DI36" s="30" t="s">
-        <v>199</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:113" ht="20" customHeight="1">
@@ -9603,7 +9621,7 @@
         <v>107</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G37" s="31"/>
       <c r="H37" s="31"/>
@@ -9612,10 +9630,10 @@
       <c r="K37" s="31"/>
       <c r="L37" s="31"/>
       <c r="M37" s="30" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="N37" s="30" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O37" s="31"/>
       <c r="P37" s="29">
@@ -9679,7 +9697,7 @@
         <v>112</v>
       </c>
       <c r="BD37" s="30" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="BE37" s="30" t="s">
         <v>114</v>

</xml_diff>

<commit_message>
Include number of non Prop64 convictions in results files
</commit_message>
<xml_diff>
--- a/test_fixtures/los_angeles.xlsx
+++ b/test_fixtures/los_angeles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33840" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28520" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="251">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -769,6 +769,9 @@
   </si>
   <si>
     <t>No applicable eligibility criteria</t>
+  </si>
+  <si>
+    <t># of NON Prop 64 convictions</t>
   </si>
 </sst>
 </file>
@@ -2588,10 +2591,10 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:JB37"/>
+  <dimension ref="A1:JC37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="DA11" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="DH24" sqref="DH24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CS19" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="DC37" sqref="DC37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2687,18 +2690,20 @@
     <col min="96" max="96" width="12.5" style="1" customWidth="1"/>
     <col min="97" max="97" width="29.6640625" style="1" customWidth="1"/>
     <col min="98" max="98" width="24" style="1" customWidth="1"/>
-    <col min="99" max="99" width="56.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="100" max="102" width="23.6640625" style="1" customWidth="1"/>
+    <col min="99" max="99" width="14.5" style="1" customWidth="1"/>
+    <col min="100" max="100" width="11.33203125" style="1" customWidth="1"/>
+    <col min="101" max="101" width="16" style="1" customWidth="1"/>
+    <col min="102" max="102" width="10.83203125" style="1" customWidth="1"/>
     <col min="103" max="104" width="12.5" style="1" customWidth="1"/>
     <col min="105" max="105" width="10" style="1" customWidth="1"/>
-    <col min="106" max="110" width="20.5" style="1" customWidth="1"/>
-    <col min="111" max="111" width="25.83203125" style="1" customWidth="1"/>
-    <col min="112" max="112" width="37" style="1" customWidth="1"/>
-    <col min="113" max="113" width="41.5" style="1" customWidth="1"/>
-    <col min="114" max="262" width="8.33203125" style="1" customWidth="1"/>
+    <col min="106" max="111" width="20.5" style="1" customWidth="1"/>
+    <col min="112" max="112" width="25.83203125" style="1" customWidth="1"/>
+    <col min="113" max="113" width="37" style="1" customWidth="1"/>
+    <col min="114" max="114" width="41.5" style="1" customWidth="1"/>
+    <col min="115" max="263" width="8.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" s="47" customFormat="1" ht="27.75" customHeight="1">
+    <row r="1" spans="1:114" s="47" customFormat="1" ht="27.75" customHeight="1">
       <c r="A1" s="48"/>
       <c r="B1" s="44"/>
       <c r="C1" s="45"/>
@@ -2886,8 +2891,11 @@
       <c r="DI1" s="46" t="s">
         <v>224</v>
       </c>
+      <c r="DJ1" s="46" t="s">
+        <v>224</v>
+      </c>
     </row>
-    <row r="2" spans="1:113" ht="20.25" customHeight="1">
+    <row r="2" spans="1:114" ht="20.25" customHeight="1">
       <c r="A2" s="50" t="s">
         <v>224</v>
       </c>
@@ -3207,28 +3215,31 @@
         <v>103</v>
       </c>
       <c r="DC2" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="DD2" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="DD2" s="2" t="s">
+      <c r="DE2" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="DE2" s="2" t="s">
+      <c r="DF2" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="DF2" s="2" t="s">
+      <c r="DG2" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="DG2" s="2" t="s">
+      <c r="DH2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="DH2" s="2" t="s">
+      <c r="DI2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="DI2" s="2" t="s">
+      <c r="DJ2" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:113" ht="20.25" customHeight="1">
+    <row r="3" spans="1:114" ht="20.25" customHeight="1">
       <c r="A3" s="50"/>
       <c r="B3" s="3"/>
       <c r="C3" s="51"/>
@@ -3389,11 +3400,12 @@
       <c r="DD3" s="5"/>
       <c r="DE3" s="5"/>
       <c r="DF3" s="5"/>
-      <c r="DG3" s="6"/>
+      <c r="DG3" s="5"/>
       <c r="DH3" s="6"/>
       <c r="DI3" s="6"/>
+      <c r="DJ3" s="6"/>
     </row>
-    <row r="4" spans="1:113" ht="20" customHeight="1">
+    <row r="4" spans="1:114" ht="20" customHeight="1">
       <c r="A4" s="50"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -3564,11 +3576,12 @@
       <c r="DD4" s="10"/>
       <c r="DE4" s="10"/>
       <c r="DF4" s="10"/>
-      <c r="DG4" s="11"/>
+      <c r="DG4" s="10"/>
       <c r="DH4" s="11"/>
       <c r="DI4" s="11"/>
+      <c r="DJ4" s="11"/>
     </row>
-    <row r="5" spans="1:113" ht="20" customHeight="1">
+    <row r="5" spans="1:114" ht="20" customHeight="1">
       <c r="A5" s="50"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -3729,11 +3742,12 @@
       <c r="DD5" s="10"/>
       <c r="DE5" s="10"/>
       <c r="DF5" s="10"/>
-      <c r="DG5" s="11"/>
+      <c r="DG5" s="10"/>
       <c r="DH5" s="11"/>
       <c r="DI5" s="11"/>
+      <c r="DJ5" s="11"/>
     </row>
-    <row r="6" spans="1:113" ht="20" customHeight="1">
+    <row r="6" spans="1:114" ht="20" customHeight="1">
       <c r="A6" s="50"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
@@ -3894,11 +3908,12 @@
       <c r="DD6" s="10"/>
       <c r="DE6" s="10"/>
       <c r="DF6" s="10"/>
-      <c r="DG6" s="11"/>
+      <c r="DG6" s="10"/>
       <c r="DH6" s="11"/>
       <c r="DI6" s="11"/>
+      <c r="DJ6" s="11"/>
     </row>
-    <row r="7" spans="1:113" ht="20" customHeight="1">
+    <row r="7" spans="1:114" ht="20" customHeight="1">
       <c r="A7" s="50"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8"/>
@@ -4059,11 +4074,12 @@
       <c r="DD7" s="10"/>
       <c r="DE7" s="10"/>
       <c r="DF7" s="10"/>
-      <c r="DG7" s="11"/>
+      <c r="DG7" s="10"/>
       <c r="DH7" s="11"/>
       <c r="DI7" s="11"/>
+      <c r="DJ7" s="11"/>
     </row>
-    <row r="8" spans="1:113" ht="20" customHeight="1">
+    <row r="8" spans="1:114" ht="20" customHeight="1">
       <c r="A8" s="50" t="s">
         <v>224</v>
       </c>
@@ -4255,28 +4271,31 @@
         <v>146</v>
       </c>
       <c r="DC8" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="DD8" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="DD8" s="10" t="s">
+      <c r="DE8" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="DE8" s="10" t="s">
-        <v>235</v>
       </c>
       <c r="DF8" s="10" t="s">
         <v>235</v>
       </c>
       <c r="DG8" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="DH8" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="DH8" s="10" t="s">
+      <c r="DI8" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="DI8" s="10" t="s">
+      <c r="DJ8" s="10" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:113" ht="20" customHeight="1">
+    <row r="9" spans="1:114" ht="20" customHeight="1">
       <c r="A9" s="50"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13"/>
@@ -4437,11 +4456,12 @@
       <c r="DD9" s="15"/>
       <c r="DE9" s="15"/>
       <c r="DF9" s="15"/>
-      <c r="DG9" s="16"/>
+      <c r="DG9" s="15"/>
       <c r="DH9" s="16"/>
       <c r="DI9" s="16"/>
+      <c r="DJ9" s="16"/>
     </row>
-    <row r="10" spans="1:113" ht="20" customHeight="1">
+    <row r="10" spans="1:114" ht="20" customHeight="1">
       <c r="A10" s="50" t="s">
         <v>224</v>
       </c>
@@ -4629,10 +4649,10 @@
         <v>142</v>
       </c>
       <c r="DC10" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="DD10" s="15" t="s">
         <v>142</v>
-      </c>
-      <c r="DD10" s="15" t="s">
-        <v>235</v>
       </c>
       <c r="DE10" s="15" t="s">
         <v>235</v>
@@ -4641,16 +4661,19 @@
         <v>235</v>
       </c>
       <c r="DG10" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="DH10" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="DH10" s="15" t="s">
+      <c r="DI10" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="DI10" s="15" t="s">
+      <c r="DJ10" s="15" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:113" ht="20" customHeight="1">
+    <row r="11" spans="1:114" ht="20" customHeight="1">
       <c r="A11" s="50"/>
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
@@ -4807,11 +4830,12 @@
       <c r="DD11" s="15"/>
       <c r="DE11" s="15"/>
       <c r="DF11" s="15"/>
-      <c r="DG11" s="16"/>
+      <c r="DG11" s="15"/>
       <c r="DH11" s="16"/>
       <c r="DI11" s="16"/>
+      <c r="DJ11" s="16"/>
     </row>
-    <row r="12" spans="1:113" ht="20" customHeight="1">
+    <row r="12" spans="1:114" ht="20" customHeight="1">
       <c r="A12" s="50" t="s">
         <v>224</v>
       </c>
@@ -5003,10 +5027,10 @@
         <v>142</v>
       </c>
       <c r="DC12" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="DD12" s="15" t="s">
         <v>142</v>
-      </c>
-      <c r="DD12" s="15" t="s">
-        <v>235</v>
       </c>
       <c r="DE12" s="15" t="s">
         <v>235</v>
@@ -5015,16 +5039,19 @@
         <v>235</v>
       </c>
       <c r="DG12" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="DH12" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="DH12" s="15" t="s">
+      <c r="DI12" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="DI12" s="15" t="s">
+      <c r="DJ12" s="15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:113" ht="20" customHeight="1">
+    <row r="13" spans="1:114" ht="20" customHeight="1">
       <c r="A13" s="50"/>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
@@ -5189,11 +5216,12 @@
       <c r="DD13" s="15"/>
       <c r="DE13" s="15"/>
       <c r="DF13" s="15"/>
-      <c r="DG13" s="16"/>
+      <c r="DG13" s="15"/>
       <c r="DH13" s="16"/>
       <c r="DI13" s="16"/>
+      <c r="DJ13" s="16"/>
     </row>
-    <row r="14" spans="1:113" ht="20" customHeight="1">
+    <row r="14" spans="1:114" ht="20" customHeight="1">
       <c r="A14" s="50" t="s">
         <v>224</v>
       </c>
@@ -5386,25 +5414,28 @@
         <v>235</v>
       </c>
       <c r="DD14" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="DE14" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="DE14" s="20" t="s">
+      <c r="DF14" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="DF14" s="20" t="s">
+      <c r="DG14" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="DG14" s="20" t="s">
+      <c r="DH14" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="DH14" s="20" t="s">
+      <c r="DI14" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="DI14" s="20" t="s">
+      <c r="DJ14" s="20" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:113" ht="20" customHeight="1">
+    <row r="15" spans="1:114" ht="20" customHeight="1">
       <c r="A15" s="50"/>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -5575,11 +5606,12 @@
       <c r="DD15" s="20"/>
       <c r="DE15" s="20"/>
       <c r="DF15" s="20"/>
-      <c r="DG15" s="21"/>
+      <c r="DG15" s="20"/>
       <c r="DH15" s="21"/>
       <c r="DI15" s="21"/>
+      <c r="DJ15" s="21"/>
     </row>
-    <row r="16" spans="1:113" ht="20" customHeight="1">
+    <row r="16" spans="1:114" ht="20" customHeight="1">
       <c r="A16" s="50"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -5750,11 +5782,12 @@
       <c r="DD16" s="20"/>
       <c r="DE16" s="20"/>
       <c r="DF16" s="20"/>
-      <c r="DG16" s="21"/>
+      <c r="DG16" s="20"/>
       <c r="DH16" s="21"/>
       <c r="DI16" s="21"/>
+      <c r="DJ16" s="21"/>
     </row>
-    <row r="17" spans="1:113" ht="20" customHeight="1">
+    <row r="17" spans="1:114" ht="20" customHeight="1">
       <c r="A17" s="50" t="s">
         <v>224</v>
       </c>
@@ -5945,25 +5978,28 @@
         <v>235</v>
       </c>
       <c r="DD17" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="DE17" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="DE17" s="20" t="s">
+      <c r="DF17" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="DF17" s="20" t="s">
+      <c r="DG17" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="DG17" s="20" t="s">
+      <c r="DH17" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="DH17" s="20" t="s">
+      <c r="DI17" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="DI17" s="20" t="s">
+      <c r="DJ17" s="20" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="18" spans="1:113" ht="20" customHeight="1">
+    <row r="18" spans="1:114" ht="20" customHeight="1">
       <c r="A18" s="50"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
@@ -6132,11 +6168,12 @@
       <c r="DD18" s="20"/>
       <c r="DE18" s="20"/>
       <c r="DF18" s="20"/>
-      <c r="DG18" s="21"/>
+      <c r="DG18" s="20"/>
       <c r="DH18" s="21"/>
       <c r="DI18" s="21"/>
+      <c r="DJ18" s="21"/>
     </row>
-    <row r="19" spans="1:113" ht="20" customHeight="1">
+    <row r="19" spans="1:114" ht="20" customHeight="1">
       <c r="A19" s="50"/>
       <c r="B19" s="22"/>
       <c r="C19" s="23"/>
@@ -6307,11 +6344,12 @@
       <c r="DD19" s="25"/>
       <c r="DE19" s="25"/>
       <c r="DF19" s="25"/>
-      <c r="DG19" s="26"/>
+      <c r="DG19" s="25"/>
       <c r="DH19" s="26"/>
       <c r="DI19" s="26"/>
+      <c r="DJ19" s="26"/>
     </row>
-    <row r="20" spans="1:113" ht="20" customHeight="1">
+    <row r="20" spans="1:114" ht="20" customHeight="1">
       <c r="A20" s="50" t="s">
         <v>224</v>
       </c>
@@ -6493,28 +6531,31 @@
         <v>142</v>
       </c>
       <c r="DC20" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="DD20" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="DD20" s="25" t="s">
+      <c r="DE20" s="25" t="s">
         <v>142</v>
-      </c>
-      <c r="DE20" s="25" t="s">
-        <v>235</v>
       </c>
       <c r="DF20" s="25" t="s">
         <v>235</v>
       </c>
       <c r="DG20" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="DH20" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="DH20" s="25" t="s">
+      <c r="DI20" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="DI20" s="25" t="s">
+      <c r="DJ20" s="25" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="21" spans="1:113" ht="20" customHeight="1">
+    <row r="21" spans="1:114" ht="20" customHeight="1">
       <c r="A21" s="50"/>
       <c r="B21" s="22"/>
       <c r="C21" s="23"/>
@@ -6685,11 +6726,12 @@
       <c r="DD21" s="25"/>
       <c r="DE21" s="25"/>
       <c r="DF21" s="25"/>
-      <c r="DG21" s="26"/>
+      <c r="DG21" s="25"/>
       <c r="DH21" s="26"/>
       <c r="DI21" s="26"/>
+      <c r="DJ21" s="26"/>
     </row>
-    <row r="22" spans="1:113" ht="20" customHeight="1">
+    <row r="22" spans="1:114" ht="20" customHeight="1">
       <c r="A22" s="50" t="s">
         <v>224</v>
       </c>
@@ -6879,28 +6921,31 @@
         <v>142</v>
       </c>
       <c r="DC22" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="DD22" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="DD22" s="25" t="s">
+      <c r="DE22" s="25" t="s">
         <v>142</v>
-      </c>
-      <c r="DE22" s="25" t="s">
-        <v>235</v>
       </c>
       <c r="DF22" s="25" t="s">
         <v>235</v>
       </c>
       <c r="DG22" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="DH22" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="DH22" s="25" t="s">
+      <c r="DI22" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="DI22" s="25" t="s">
+      <c r="DJ22" s="25" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="23" spans="1:113" ht="20" customHeight="1">
+    <row r="23" spans="1:114" ht="20" customHeight="1">
       <c r="A23" s="50" t="s">
         <v>224</v>
       </c>
@@ -7084,7 +7129,7 @@
         <v>153</v>
       </c>
       <c r="DC23" s="30" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="DD23" s="30" t="s">
         <v>146</v>
@@ -7093,19 +7138,22 @@
         <v>146</v>
       </c>
       <c r="DF23" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="DG23" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="DG23" s="30" t="s">
+      <c r="DH23" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="DH23" s="30" t="s">
+      <c r="DI23" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="DI23" s="30" t="s">
+      <c r="DJ23" s="30" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="24" spans="1:113" ht="20" customHeight="1">
+    <row r="24" spans="1:114" ht="20" customHeight="1">
       <c r="A24" s="50"/>
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
@@ -7272,11 +7320,12 @@
       <c r="DD24" s="30"/>
       <c r="DE24" s="30"/>
       <c r="DF24" s="30"/>
-      <c r="DG24" s="31"/>
+      <c r="DG24" s="30"/>
       <c r="DH24" s="31"/>
       <c r="DI24" s="31"/>
+      <c r="DJ24" s="31"/>
     </row>
-    <row r="25" spans="1:113" ht="20" customHeight="1">
+    <row r="25" spans="1:114" ht="20" customHeight="1">
       <c r="A25" s="50"/>
       <c r="B25" s="27"/>
       <c r="C25" s="28"/>
@@ -7437,11 +7486,12 @@
       <c r="DD25" s="30"/>
       <c r="DE25" s="30"/>
       <c r="DF25" s="30"/>
-      <c r="DG25" s="31"/>
+      <c r="DG25" s="30"/>
       <c r="DH25" s="31"/>
       <c r="DI25" s="31"/>
+      <c r="DJ25" s="31"/>
     </row>
-    <row r="26" spans="1:113" ht="20" customHeight="1">
+    <row r="26" spans="1:114" ht="20" customHeight="1">
       <c r="A26" s="50" t="s">
         <v>224</v>
       </c>
@@ -7623,7 +7673,7 @@
         <v>153</v>
       </c>
       <c r="DC26" s="30" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="DD26" s="30" t="s">
         <v>146</v>
@@ -7632,19 +7682,22 @@
         <v>146</v>
       </c>
       <c r="DF26" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="DG26" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="DG26" s="30" t="s">
+      <c r="DH26" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="DH26" s="30" t="s">
+      <c r="DI26" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="DI26" s="30" t="s">
+      <c r="DJ26" s="30" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="27" spans="1:113" ht="20" customHeight="1">
+    <row r="27" spans="1:114" ht="20" customHeight="1">
       <c r="A27" s="50" t="s">
         <v>224</v>
       </c>
@@ -7824,7 +7877,7 @@
         <v>153</v>
       </c>
       <c r="DC27" s="30" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="DD27" s="30" t="s">
         <v>146</v>
@@ -7833,19 +7886,22 @@
         <v>146</v>
       </c>
       <c r="DF27" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="DG27" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="DG27" s="30" t="s">
+      <c r="DH27" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="DH27" s="30" t="s">
+      <c r="DI27" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="DI27" s="30" t="s">
+      <c r="DJ27" s="30" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:113" ht="20" customHeight="1">
+    <row r="28" spans="1:114" ht="20" customHeight="1">
       <c r="A28" s="50" t="s">
         <v>224</v>
       </c>
@@ -8039,22 +8095,25 @@
         <v>235</v>
       </c>
       <c r="DE28" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="DF28" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="DF28" s="35" t="s">
+      <c r="DG28" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="DG28" s="35" t="s">
+      <c r="DH28" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="DH28" s="35" t="s">
+      <c r="DI28" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="DI28" s="35" t="s">
+      <c r="DJ28" s="35" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="29" spans="1:113" ht="20" customHeight="1">
+    <row r="29" spans="1:114" ht="20" customHeight="1">
       <c r="A29" s="50"/>
       <c r="B29" s="32"/>
       <c r="C29" s="33"/>
@@ -8225,11 +8284,12 @@
       <c r="DD29" s="35"/>
       <c r="DE29" s="35"/>
       <c r="DF29" s="35"/>
-      <c r="DG29" s="36"/>
+      <c r="DG29" s="35"/>
       <c r="DH29" s="36"/>
       <c r="DI29" s="36"/>
+      <c r="DJ29" s="36"/>
     </row>
-    <row r="30" spans="1:113" ht="20" customHeight="1">
+    <row r="30" spans="1:114" ht="20" customHeight="1">
       <c r="A30" s="50" t="s">
         <v>224</v>
       </c>
@@ -8423,22 +8483,25 @@
         <v>235</v>
       </c>
       <c r="DE30" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="DF30" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="DF30" s="35" t="s">
+      <c r="DG30" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="DG30" s="35" t="s">
+      <c r="DH30" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="DH30" s="35" t="s">
+      <c r="DI30" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="DI30" s="35" t="s">
+      <c r="DJ30" s="35" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="31" spans="1:113" ht="20" customHeight="1">
+    <row r="31" spans="1:114" ht="20" customHeight="1">
       <c r="A31" s="50" t="s">
         <v>224</v>
       </c>
@@ -8626,28 +8689,31 @@
         <v>146</v>
       </c>
       <c r="DC31" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="DD31" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="DD31" s="10" t="s">
+      <c r="DE31" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="DE31" s="10" t="s">
-        <v>235</v>
       </c>
       <c r="DF31" s="10" t="s">
         <v>235</v>
       </c>
       <c r="DG31" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="DH31" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="DH31" s="55" t="s">
+      <c r="DI31" s="55" t="s">
         <v>147</v>
       </c>
-      <c r="DI31" s="10" t="s">
+      <c r="DJ31" s="10" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:113" ht="20" customHeight="1">
+    <row r="32" spans="1:114" ht="20" customHeight="1">
       <c r="A32" s="50"/>
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
@@ -8822,11 +8888,12 @@
       <c r="DD32" s="10"/>
       <c r="DE32" s="10"/>
       <c r="DF32" s="10"/>
-      <c r="DG32" s="11"/>
+      <c r="DG32" s="10"/>
       <c r="DH32" s="11"/>
       <c r="DI32" s="11"/>
+      <c r="DJ32" s="11"/>
     </row>
-    <row r="33" spans="1:113" ht="20" customHeight="1">
+    <row r="33" spans="1:114" ht="20" customHeight="1">
       <c r="A33" s="50" t="s">
         <v>224</v>
       </c>
@@ -9009,25 +9076,28 @@
         <v>235</v>
       </c>
       <c r="DD33" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="DE33" s="15" t="s">
         <v>146</v>
-      </c>
-      <c r="DE33" s="15" t="s">
-        <v>235</v>
       </c>
       <c r="DF33" s="15" t="s">
         <v>235</v>
       </c>
       <c r="DG33" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="DH33" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="DH33" s="15" t="s">
+      <c r="DI33" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="DI33" s="15" t="s">
+      <c r="DJ33" s="15" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:113" ht="20" customHeight="1">
+    <row r="34" spans="1:114" ht="20" customHeight="1">
       <c r="A34" s="50" t="s">
         <v>224</v>
       </c>
@@ -9210,25 +9280,28 @@
         <v>235</v>
       </c>
       <c r="DD34" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="DE34" s="20" t="s">
         <v>146</v>
-      </c>
-      <c r="DE34" s="20" t="s">
-        <v>235</v>
       </c>
       <c r="DF34" s="20" t="s">
         <v>235</v>
       </c>
       <c r="DG34" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="DH34" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="DH34" s="20" t="s">
+      <c r="DI34" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="DI34" s="20" t="s">
+      <c r="DJ34" s="20" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="35" spans="1:113" ht="20" customHeight="1">
+    <row r="35" spans="1:114" ht="20" customHeight="1">
       <c r="A35" s="50"/>
       <c r="B35" s="27"/>
       <c r="C35" s="28"/>
@@ -9389,11 +9462,12 @@
       <c r="DD35" s="30"/>
       <c r="DE35" s="30"/>
       <c r="DF35" s="30"/>
-      <c r="DG35" s="31"/>
+      <c r="DG35" s="30"/>
       <c r="DH35" s="31"/>
       <c r="DI35" s="31"/>
+      <c r="DJ35" s="31"/>
     </row>
-    <row r="36" spans="1:113" ht="20" customHeight="1">
+    <row r="36" spans="1:114" ht="20" customHeight="1">
       <c r="A36" s="50" t="s">
         <v>224</v>
       </c>
@@ -9571,28 +9645,31 @@
         <v>146</v>
       </c>
       <c r="DC36" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="DD36" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="DD36" s="30" t="s">
+      <c r="DE36" s="30" t="s">
         <v>146</v>
-      </c>
-      <c r="DE36" s="30" t="s">
-        <v>235</v>
       </c>
       <c r="DF36" s="30" t="s">
         <v>235</v>
       </c>
       <c r="DG36" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="DH36" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="DH36" s="30" t="s">
+      <c r="DI36" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="DI36" s="30" t="s">
+      <c r="DJ36" s="30" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="1:113" ht="20" customHeight="1">
+    <row r="37" spans="1:114" ht="20" customHeight="1">
       <c r="A37" s="50"/>
       <c r="B37" s="27"/>
       <c r="C37" s="28"/>
@@ -9758,6 +9835,7 @@
       <c r="DG37" s="30"/>
       <c r="DH37" s="30"/>
       <c r="DI37" s="30"/>
+      <c r="DJ37" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>